<commit_message>
Update: boiling plan reader + functional tests
</commit_message>
<xml_diff>
--- a/app/data/static/templates/constructor_mascarpone.xlsx
+++ b/app/data/static/templates/constructor_mascarpone.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t xml:space="preserve">Тип варки</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve">Номер группы варок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выход с одной варки, кг</t>
   </si>
   <si>
     <t xml:space="preserve">SKU</t>
@@ -145,13 +148,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0"/>
-    <numFmt numFmtId="168" formatCode="General"/>
-    <numFmt numFmtId="169" formatCode="@"/>
+    <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -371,7 +373,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -383,19 +385,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -688,7 +690,6 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="11" width="5.76"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="11" width="5.14"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="20" min="20" style="0" width="9.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -699,23 +700,23 @@
         <v>0</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J1" s="15"/>
       <c r="L1" s="15"/>
@@ -736,13 +737,13 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" s="15" t="n">
         <v>0</v>
@@ -761,7 +762,7 @@
         <v/>
       </c>
       <c r="E3" s="19" t="str">
-        <f aca="false">IF(D3="-", "-", IF(D3="", "", F3*VLOOKUP(D3, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D3="-", "-", IF(D3="", "", INT(F3*VLOOKUP(D3, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F3" s="20"/>
@@ -769,17 +770,14 @@
         <f aca="true">IF(J3="","",(INDIRECT("N" &amp; ROW() - 1) - N3))</f>
         <v/>
       </c>
-      <c r="H3" s="18" t="str">
-        <f aca="true">IF(J3 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H3" s="18"/>
       <c r="I3" s="18" t="str">
         <f aca="true">IF(J3 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K3" s="20" t="n">
-        <f aca="true">IF(J3 = "-", -INDIRECT("C" &amp; ROW() - 1),F3)</f>
-        <v>0</v>
+      <c r="K3" s="20" t="str">
+        <f aca="true">IF(J3 = "-", -INDIRECT("C" &amp; ROW() - 1),E3)</f>
+        <v/>
       </c>
       <c r="L3" s="17" t="n">
         <f aca="true">IF(J3 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K3)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K3)))), 0)</f>
@@ -813,7 +811,7 @@
         <v/>
       </c>
       <c r="E4" s="19" t="str">
-        <f aca="false">IF(D4="-", "-", IF(D4="", "", F4*VLOOKUP(D4, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D4="-", "-", IF(D4="", "", INT(F4*VLOOKUP(D4, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F4" s="20"/>
@@ -821,17 +819,14 @@
         <f aca="true">IF(J4="","",(INDIRECT("N" &amp; ROW() - 1) - N4))</f>
         <v/>
       </c>
-      <c r="H4" s="18" t="str">
-        <f aca="true">IF(J4 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H4" s="18"/>
       <c r="I4" s="18" t="str">
         <f aca="true">IF(J4 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K4" s="20" t="n">
-        <f aca="true">IF(J4 = "-", -INDIRECT("C" &amp; ROW() - 1),F4)</f>
-        <v>0</v>
+      <c r="K4" s="20" t="str">
+        <f aca="true">IF(J4 = "-", -INDIRECT("C" &amp; ROW() - 1),E4)</f>
+        <v/>
       </c>
       <c r="L4" s="17" t="n">
         <f aca="true">IF(J4 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K4)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K4)))), 0)</f>
@@ -865,7 +860,7 @@
         <v/>
       </c>
       <c r="E5" s="19" t="str">
-        <f aca="false">IF(D5="-", "-", IF(D5="", "", F5*VLOOKUP(D5, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D5="-", "-", IF(D5="", "", INT(F5*VLOOKUP(D5, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F5" s="20"/>
@@ -873,17 +868,14 @@
         <f aca="true">IF(J5="","",(INDIRECT("N" &amp; ROW() - 1) - N5))</f>
         <v/>
       </c>
-      <c r="H5" s="18" t="str">
-        <f aca="true">IF(J5 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H5" s="18"/>
       <c r="I5" s="18" t="str">
         <f aca="true">IF(J5 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K5" s="20" t="n">
-        <f aca="true">IF(J5 = "-", -INDIRECT("C" &amp; ROW() - 1),F5)</f>
-        <v>0</v>
+      <c r="K5" s="20" t="str">
+        <f aca="true">IF(J5 = "-", -INDIRECT("C" &amp; ROW() - 1),E5)</f>
+        <v/>
       </c>
       <c r="L5" s="17" t="n">
         <f aca="true">IF(J5 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K5)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K5)))), 0)</f>
@@ -917,7 +909,7 @@
         <v/>
       </c>
       <c r="E6" s="19" t="str">
-        <f aca="false">IF(D6="-", "-", IF(D6="", "", F6*VLOOKUP(D6, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D6="-", "-", IF(D6="", "", INT(F6*VLOOKUP(D6, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F6" s="20"/>
@@ -925,17 +917,14 @@
         <f aca="true">IF(J6="","",(INDIRECT("N" &amp; ROW() - 1) - N6))</f>
         <v/>
       </c>
-      <c r="H6" s="18" t="str">
-        <f aca="true">IF(J6 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H6" s="18"/>
       <c r="I6" s="18" t="str">
         <f aca="true">IF(J6 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K6" s="20" t="n">
-        <f aca="true">IF(J6 = "-", -INDIRECT("C" &amp; ROW() - 1),F6)</f>
-        <v>0</v>
+      <c r="K6" s="20" t="str">
+        <f aca="true">IF(J6 = "-", -INDIRECT("C" &amp; ROW() - 1),E6)</f>
+        <v/>
       </c>
       <c r="L6" s="17" t="n">
         <f aca="true">IF(J6 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K6)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K6)))), 0)</f>
@@ -969,7 +958,7 @@
         <v/>
       </c>
       <c r="E7" s="19" t="str">
-        <f aca="false">IF(D7="-", "-", IF(D7="", "", F7*VLOOKUP(D7, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D7="-", "-", IF(D7="", "", INT(F7*VLOOKUP(D7, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F7" s="20"/>
@@ -977,17 +966,14 @@
         <f aca="true">IF(J7="","",(INDIRECT("N" &amp; ROW() - 1) - N7))</f>
         <v/>
       </c>
-      <c r="H7" s="18" t="str">
-        <f aca="true">IF(J7 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H7" s="18"/>
       <c r="I7" s="18" t="str">
         <f aca="true">IF(J7 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K7" s="20" t="n">
-        <f aca="true">IF(J7 = "-", -INDIRECT("C" &amp; ROW() - 1),F7)</f>
-        <v>0</v>
+      <c r="K7" s="20" t="str">
+        <f aca="true">IF(J7 = "-", -INDIRECT("C" &amp; ROW() - 1),E7)</f>
+        <v/>
       </c>
       <c r="L7" s="17" t="n">
         <f aca="true">IF(J7 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K7)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K7)))), 0)</f>
@@ -1021,7 +1007,7 @@
         <v/>
       </c>
       <c r="E8" s="19" t="str">
-        <f aca="false">IF(D8="-", "-", IF(D8="", "", F8*VLOOKUP(D8, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D8="-", "-", IF(D8="", "", INT(F8*VLOOKUP(D8, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F8" s="20"/>
@@ -1029,17 +1015,14 @@
         <f aca="true">IF(J8="","",(INDIRECT("N" &amp; ROW() - 1) - N8))</f>
         <v/>
       </c>
-      <c r="H8" s="18" t="str">
-        <f aca="true">IF(J8 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H8" s="18"/>
       <c r="I8" s="18" t="str">
         <f aca="true">IF(J8 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K8" s="20" t="n">
-        <f aca="true">IF(J8 = "-", -INDIRECT("C" &amp; ROW() - 1),F8)</f>
-        <v>0</v>
+      <c r="K8" s="20" t="str">
+        <f aca="true">IF(J8 = "-", -INDIRECT("C" &amp; ROW() - 1),E8)</f>
+        <v/>
       </c>
       <c r="L8" s="17" t="n">
         <f aca="true">IF(J8 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K8)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K8)))), 0)</f>
@@ -1073,7 +1056,7 @@
         <v/>
       </c>
       <c r="E9" s="19" t="str">
-        <f aca="false">IF(D9="-", "-", IF(D9="", "", F9*VLOOKUP(D9, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D9="-", "-", IF(D9="", "", INT(F9*VLOOKUP(D9, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F9" s="20"/>
@@ -1081,17 +1064,14 @@
         <f aca="true">IF(J9="","",(INDIRECT("N" &amp; ROW() - 1) - N9))</f>
         <v/>
       </c>
-      <c r="H9" s="18" t="str">
-        <f aca="true">IF(J9 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H9" s="18"/>
       <c r="I9" s="18" t="str">
         <f aca="true">IF(J9 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K9" s="20" t="n">
-        <f aca="true">IF(J9 = "-", -INDIRECT("C" &amp; ROW() - 1),F9)</f>
-        <v>0</v>
+      <c r="K9" s="20" t="str">
+        <f aca="true">IF(J9 = "-", -INDIRECT("C" &amp; ROW() - 1),E9)</f>
+        <v/>
       </c>
       <c r="L9" s="17" t="n">
         <f aca="true">IF(J9 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K9)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K9)))), 0)</f>
@@ -1125,7 +1105,7 @@
         <v/>
       </c>
       <c r="E10" s="19" t="str">
-        <f aca="false">IF(D10="-", "-", IF(D10="", "", F10*VLOOKUP(D10, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D10="-", "-", IF(D10="", "", INT(F10*VLOOKUP(D10, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F10" s="20"/>
@@ -1133,17 +1113,14 @@
         <f aca="true">IF(J10="","",(INDIRECT("N" &amp; ROW() - 1) - N10))</f>
         <v/>
       </c>
-      <c r="H10" s="18" t="str">
-        <f aca="true">IF(J10 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H10" s="18"/>
       <c r="I10" s="18" t="str">
         <f aca="true">IF(J10 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K10" s="20" t="n">
-        <f aca="true">IF(J10 = "-", -INDIRECT("C" &amp; ROW() - 1),F10)</f>
-        <v>0</v>
+      <c r="K10" s="20" t="str">
+        <f aca="true">IF(J10 = "-", -INDIRECT("C" &amp; ROW() - 1),E10)</f>
+        <v/>
       </c>
       <c r="L10" s="17" t="n">
         <f aca="true">IF(J10 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K10)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K10)))), 0)</f>
@@ -1177,7 +1154,7 @@
         <v/>
       </c>
       <c r="E11" s="19" t="str">
-        <f aca="false">IF(D11="-", "-", IF(D11="", "", F11*VLOOKUP(D11, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D11="-", "-", IF(D11="", "", INT(F11*VLOOKUP(D11, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F11" s="20"/>
@@ -1185,17 +1162,14 @@
         <f aca="true">IF(J11="","",(INDIRECT("N" &amp; ROW() - 1) - N11))</f>
         <v/>
       </c>
-      <c r="H11" s="18" t="str">
-        <f aca="true">IF(J11 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H11" s="18"/>
       <c r="I11" s="18" t="str">
         <f aca="true">IF(J11 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K11" s="20" t="n">
-        <f aca="true">IF(J11 = "-", -INDIRECT("C" &amp; ROW() - 1),F11)</f>
-        <v>0</v>
+      <c r="K11" s="20" t="str">
+        <f aca="true">IF(J11 = "-", -INDIRECT("C" &amp; ROW() - 1),E11)</f>
+        <v/>
       </c>
       <c r="L11" s="17" t="n">
         <f aca="true">IF(J11 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K11)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K11)))), 0)</f>
@@ -1229,7 +1203,7 @@
         <v/>
       </c>
       <c r="E12" s="19" t="str">
-        <f aca="false">IF(D12="-", "-", IF(D12="", "", F12*VLOOKUP(D12, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D12="-", "-", IF(D12="", "", INT(F12*VLOOKUP(D12, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F12" s="20"/>
@@ -1237,17 +1211,14 @@
         <f aca="true">IF(J12="","",(INDIRECT("N" &amp; ROW() - 1) - N12))</f>
         <v/>
       </c>
-      <c r="H12" s="18" t="str">
-        <f aca="true">IF(J12 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H12" s="18"/>
       <c r="I12" s="18" t="str">
         <f aca="true">IF(J12 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K12" s="20" t="n">
-        <f aca="true">IF(J12 = "-", -INDIRECT("C" &amp; ROW() - 1),F12)</f>
-        <v>0</v>
+      <c r="K12" s="20" t="str">
+        <f aca="true">IF(J12 = "-", -INDIRECT("C" &amp; ROW() - 1),E12)</f>
+        <v/>
       </c>
       <c r="L12" s="17" t="n">
         <f aca="true">IF(J12 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K12)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K12)))), 0)</f>
@@ -1281,7 +1252,7 @@
         <v/>
       </c>
       <c r="E13" s="19" t="str">
-        <f aca="false">IF(D13="-", "-", IF(D13="", "", F13*VLOOKUP(D13, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D13="-", "-", IF(D13="", "", INT(F13*VLOOKUP(D13, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F13" s="20"/>
@@ -1289,17 +1260,14 @@
         <f aca="true">IF(J13="","",(INDIRECT("N" &amp; ROW() - 1) - N13))</f>
         <v/>
       </c>
-      <c r="H13" s="18" t="str">
-        <f aca="true">IF(J13 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H13" s="18"/>
       <c r="I13" s="18" t="str">
         <f aca="true">IF(J13 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K13" s="20" t="n">
-        <f aca="true">IF(J13 = "-", -INDIRECT("C" &amp; ROW() - 1),F13)</f>
-        <v>0</v>
+      <c r="K13" s="20" t="str">
+        <f aca="true">IF(J13 = "-", -INDIRECT("C" &amp; ROW() - 1),E13)</f>
+        <v/>
       </c>
       <c r="L13" s="17" t="n">
         <f aca="true">IF(J13 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K13)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K13)))), 0)</f>
@@ -1333,7 +1301,7 @@
         <v/>
       </c>
       <c r="E14" s="19" t="str">
-        <f aca="false">IF(D14="-", "-", IF(D14="", "", F14*VLOOKUP(D14, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D14="-", "-", IF(D14="", "", INT(F14*VLOOKUP(D14, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F14" s="20"/>
@@ -1341,17 +1309,14 @@
         <f aca="true">IF(J14="","",(INDIRECT("N" &amp; ROW() - 1) - N14))</f>
         <v/>
       </c>
-      <c r="H14" s="18" t="str">
-        <f aca="true">IF(J14 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H14" s="18"/>
       <c r="I14" s="18" t="str">
         <f aca="true">IF(J14 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K14" s="20" t="n">
-        <f aca="true">IF(J14 = "-", -INDIRECT("C" &amp; ROW() - 1),F14)</f>
-        <v>0</v>
+      <c r="K14" s="20" t="str">
+        <f aca="true">IF(J14 = "-", -INDIRECT("C" &amp; ROW() - 1),E14)</f>
+        <v/>
       </c>
       <c r="L14" s="17" t="n">
         <f aca="true">IF(J14 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K14)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K14)))), 0)</f>
@@ -1385,7 +1350,7 @@
         <v/>
       </c>
       <c r="E15" s="19" t="str">
-        <f aca="false">IF(D15="-", "-", IF(D15="", "", F15*VLOOKUP(D15, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D15="-", "-", IF(D15="", "", INT(F15*VLOOKUP(D15, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F15" s="20"/>
@@ -1393,17 +1358,14 @@
         <f aca="true">IF(J15="","",(INDIRECT("N" &amp; ROW() - 1) - N15))</f>
         <v/>
       </c>
-      <c r="H15" s="18" t="str">
-        <f aca="true">IF(J15 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H15" s="18"/>
       <c r="I15" s="18" t="str">
         <f aca="true">IF(J15 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K15" s="20" t="n">
-        <f aca="true">IF(J15 = "-", -INDIRECT("C" &amp; ROW() - 1),F15)</f>
-        <v>0</v>
+      <c r="K15" s="20" t="str">
+        <f aca="true">IF(J15 = "-", -INDIRECT("C" &amp; ROW() - 1),E15)</f>
+        <v/>
       </c>
       <c r="L15" s="17" t="n">
         <f aca="true">IF(J15 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K15)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K15)))), 0)</f>
@@ -1437,7 +1399,7 @@
         <v/>
       </c>
       <c r="E16" s="19" t="str">
-        <f aca="false">IF(D16="-", "-", IF(D16="", "", F16*VLOOKUP(D16, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D16="-", "-", IF(D16="", "", INT(F16*VLOOKUP(D16, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F16" s="20"/>
@@ -1445,17 +1407,14 @@
         <f aca="true">IF(J16="","",(INDIRECT("N" &amp; ROW() - 1) - N16))</f>
         <v/>
       </c>
-      <c r="H16" s="18" t="str">
-        <f aca="true">IF(J16 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H16" s="18"/>
       <c r="I16" s="18" t="str">
         <f aca="true">IF(J16 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K16" s="20" t="n">
-        <f aca="true">IF(J16 = "-", -INDIRECT("C" &amp; ROW() - 1),F16)</f>
-        <v>0</v>
+      <c r="K16" s="20" t="str">
+        <f aca="true">IF(J16 = "-", -INDIRECT("C" &amp; ROW() - 1),E16)</f>
+        <v/>
       </c>
       <c r="L16" s="17" t="n">
         <f aca="true">IF(J16 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K16)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K16)))), 0)</f>
@@ -1489,7 +1448,7 @@
         <v/>
       </c>
       <c r="E17" s="19" t="str">
-        <f aca="false">IF(D17="-", "-", IF(D17="", "", F17*VLOOKUP(D17, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D17="-", "-", IF(D17="", "", INT(F17*VLOOKUP(D17, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F17" s="20"/>
@@ -1497,17 +1456,14 @@
         <f aca="true">IF(J17="","",(INDIRECT("N" &amp; ROW() - 1) - N17))</f>
         <v/>
       </c>
-      <c r="H17" s="18" t="str">
-        <f aca="true">IF(J17 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H17" s="18"/>
       <c r="I17" s="18" t="str">
         <f aca="true">IF(J17 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K17" s="20" t="n">
-        <f aca="true">IF(J17 = "-", -INDIRECT("C" &amp; ROW() - 1),F17)</f>
-        <v>0</v>
+      <c r="K17" s="20" t="str">
+        <f aca="true">IF(J17 = "-", -INDIRECT("C" &amp; ROW() - 1),E17)</f>
+        <v/>
       </c>
       <c r="L17" s="17" t="n">
         <f aca="true">IF(J17 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K17)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K17)))), 0)</f>
@@ -1541,7 +1497,7 @@
         <v/>
       </c>
       <c r="E18" s="19" t="str">
-        <f aca="false">IF(D18="-", "-", IF(D18="", "", F18*VLOOKUP(D18, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D18="-", "-", IF(D18="", "", INT(F18*VLOOKUP(D18, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F18" s="20"/>
@@ -1549,17 +1505,14 @@
         <f aca="true">IF(J18="","",(INDIRECT("N" &amp; ROW() - 1) - N18))</f>
         <v/>
       </c>
-      <c r="H18" s="18" t="str">
-        <f aca="true">IF(J18 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H18" s="18"/>
       <c r="I18" s="18" t="str">
         <f aca="true">IF(J18 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K18" s="20" t="n">
-        <f aca="true">IF(J18 = "-", -INDIRECT("C" &amp; ROW() - 1),F18)</f>
-        <v>0</v>
+      <c r="K18" s="20" t="str">
+        <f aca="true">IF(J18 = "-", -INDIRECT("C" &amp; ROW() - 1),E18)</f>
+        <v/>
       </c>
       <c r="L18" s="17" t="n">
         <f aca="true">IF(J18 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K18)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K18)))), 0)</f>
@@ -1593,7 +1546,7 @@
         <v/>
       </c>
       <c r="E19" s="19" t="str">
-        <f aca="false">IF(D19="-", "-", IF(D19="", "", F19*VLOOKUP(D19, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D19="-", "-", IF(D19="", "", INT(F19*VLOOKUP(D19, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F19" s="20"/>
@@ -1601,17 +1554,14 @@
         <f aca="true">IF(J19="","",(INDIRECT("N" &amp; ROW() - 1) - N19))</f>
         <v/>
       </c>
-      <c r="H19" s="18" t="str">
-        <f aca="true">IF(J19 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H19" s="18"/>
       <c r="I19" s="18" t="str">
         <f aca="true">IF(J19 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K19" s="20" t="n">
-        <f aca="true">IF(J19 = "-", -INDIRECT("C" &amp; ROW() - 1),F19)</f>
-        <v>0</v>
+      <c r="K19" s="20" t="str">
+        <f aca="true">IF(J19 = "-", -INDIRECT("C" &amp; ROW() - 1),E19)</f>
+        <v/>
       </c>
       <c r="L19" s="17" t="n">
         <f aca="true">IF(J19 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K19)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K19)))), 0)</f>
@@ -1645,7 +1595,7 @@
         <v/>
       </c>
       <c r="E20" s="19" t="str">
-        <f aca="false">IF(D20="-", "-", IF(D20="", "", F20*VLOOKUP(D20, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D20="-", "-", IF(D20="", "", INT(F20*VLOOKUP(D20, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F20" s="20"/>
@@ -1653,17 +1603,14 @@
         <f aca="true">IF(J20="","",(INDIRECT("N" &amp; ROW() - 1) - N20))</f>
         <v/>
       </c>
-      <c r="H20" s="18" t="str">
-        <f aca="true">IF(J20 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H20" s="18"/>
       <c r="I20" s="18" t="str">
         <f aca="true">IF(J20 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K20" s="20" t="n">
-        <f aca="true">IF(J20 = "-", -INDIRECT("C" &amp; ROW() - 1),F20)</f>
-        <v>0</v>
+      <c r="K20" s="20" t="str">
+        <f aca="true">IF(J20 = "-", -INDIRECT("C" &amp; ROW() - 1),E20)</f>
+        <v/>
       </c>
       <c r="L20" s="17" t="n">
         <f aca="true">IF(J20 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K20)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K20)))), 0)</f>
@@ -1697,7 +1644,7 @@
         <v/>
       </c>
       <c r="E21" s="19" t="str">
-        <f aca="false">IF(D21="-", "-", IF(D21="", "", F21*VLOOKUP(D21, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D21="-", "-", IF(D21="", "", INT(F21*VLOOKUP(D21, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F21" s="20"/>
@@ -1705,17 +1652,14 @@
         <f aca="true">IF(J21="","",(INDIRECT("N" &amp; ROW() - 1) - N21))</f>
         <v/>
       </c>
-      <c r="H21" s="18" t="str">
-        <f aca="true">IF(J21 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H21" s="18"/>
       <c r="I21" s="18" t="str">
         <f aca="true">IF(J21 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K21" s="20" t="n">
-        <f aca="true">IF(J21 = "-", -INDIRECT("C" &amp; ROW() - 1),F21)</f>
-        <v>0</v>
+      <c r="K21" s="20" t="str">
+        <f aca="true">IF(J21 = "-", -INDIRECT("C" &amp; ROW() - 1),E21)</f>
+        <v/>
       </c>
       <c r="L21" s="17" t="n">
         <f aca="true">IF(J21 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K21)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K21)))), 0)</f>
@@ -1749,7 +1693,7 @@
         <v/>
       </c>
       <c r="E22" s="19" t="str">
-        <f aca="false">IF(D22="-", "-", IF(D22="", "", F22*VLOOKUP(D22, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D22="-", "-", IF(D22="", "", INT(F22*VLOOKUP(D22, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F22" s="20"/>
@@ -1757,17 +1701,14 @@
         <f aca="true">IF(J22="","",(INDIRECT("N" &amp; ROW() - 1) - N22))</f>
         <v/>
       </c>
-      <c r="H22" s="18" t="str">
-        <f aca="true">IF(J22 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H22" s="18"/>
       <c r="I22" s="18" t="str">
         <f aca="true">IF(J22 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K22" s="20" t="n">
-        <f aca="true">IF(J22 = "-", -INDIRECT("C" &amp; ROW() - 1),F22)</f>
-        <v>0</v>
+      <c r="K22" s="20" t="str">
+        <f aca="true">IF(J22 = "-", -INDIRECT("C" &amp; ROW() - 1),E22)</f>
+        <v/>
       </c>
       <c r="L22" s="17" t="n">
         <f aca="true">IF(J22 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K22)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K22)))), 0)</f>
@@ -1801,7 +1742,7 @@
         <v/>
       </c>
       <c r="E23" s="19" t="str">
-        <f aca="false">IF(D23="-", "-", IF(D23="", "", F23*VLOOKUP(D23, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D23="-", "-", IF(D23="", "", INT(F23*VLOOKUP(D23, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F23" s="20"/>
@@ -1809,17 +1750,14 @@
         <f aca="true">IF(J23="","",(INDIRECT("N" &amp; ROW() - 1) - N23))</f>
         <v/>
       </c>
-      <c r="H23" s="18" t="str">
-        <f aca="true">IF(J23 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H23" s="18"/>
       <c r="I23" s="18" t="str">
         <f aca="true">IF(J23 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K23" s="20" t="n">
-        <f aca="true">IF(J23 = "-", -INDIRECT("C" &amp; ROW() - 1),F23)</f>
-        <v>0</v>
+      <c r="K23" s="20" t="str">
+        <f aca="true">IF(J23 = "-", -INDIRECT("C" &amp; ROW() - 1),E23)</f>
+        <v/>
       </c>
       <c r="L23" s="17" t="n">
         <f aca="true">IF(J23 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K23)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K23)))), 0)</f>
@@ -1853,7 +1791,7 @@
         <v/>
       </c>
       <c r="E24" s="19" t="str">
-        <f aca="false">IF(D24="-", "-", IF(D24="", "", F24*VLOOKUP(D24, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D24="-", "-", IF(D24="", "", INT(F24*VLOOKUP(D24, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F24" s="20"/>
@@ -1861,17 +1799,14 @@
         <f aca="true">IF(J24="","",(INDIRECT("N" &amp; ROW() - 1) - N24))</f>
         <v/>
       </c>
-      <c r="H24" s="18" t="str">
-        <f aca="true">IF(J24 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H24" s="18"/>
       <c r="I24" s="18" t="str">
         <f aca="true">IF(J24 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K24" s="20" t="n">
-        <f aca="true">IF(J24 = "-", -INDIRECT("C" &amp; ROW() - 1),F24)</f>
-        <v>0</v>
+      <c r="K24" s="20" t="str">
+        <f aca="true">IF(J24 = "-", -INDIRECT("C" &amp; ROW() - 1),E24)</f>
+        <v/>
       </c>
       <c r="L24" s="17" t="n">
         <f aca="true">IF(J24 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K24)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K24)))), 0)</f>
@@ -1905,7 +1840,7 @@
         <v/>
       </c>
       <c r="E25" s="19" t="str">
-        <f aca="false">IF(D25="-", "-", IF(D25="", "", F25*VLOOKUP(D25, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D25="-", "-", IF(D25="", "", INT(F25*VLOOKUP(D25, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F25" s="20"/>
@@ -1913,17 +1848,14 @@
         <f aca="true">IF(J25="","",(INDIRECT("N" &amp; ROW() - 1) - N25))</f>
         <v/>
       </c>
-      <c r="H25" s="18" t="str">
-        <f aca="true">IF(J25 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H25" s="18"/>
       <c r="I25" s="18" t="str">
         <f aca="true">IF(J25 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K25" s="20" t="n">
-        <f aca="true">IF(J25 = "-", -INDIRECT("C" &amp; ROW() - 1),F25)</f>
-        <v>0</v>
+      <c r="K25" s="20" t="str">
+        <f aca="true">IF(J25 = "-", -INDIRECT("C" &amp; ROW() - 1),E25)</f>
+        <v/>
       </c>
       <c r="L25" s="17" t="n">
         <f aca="true">IF(J25 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K25)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K25)))), 0)</f>
@@ -1957,7 +1889,7 @@
         <v/>
       </c>
       <c r="E26" s="19" t="str">
-        <f aca="false">IF(D26="-", "-", IF(D26="", "", F26*VLOOKUP(D26, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D26="-", "-", IF(D26="", "", INT(F26*VLOOKUP(D26, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F26" s="20"/>
@@ -1965,17 +1897,14 @@
         <f aca="true">IF(J26="","",(INDIRECT("N" &amp; ROW() - 1) - N26))</f>
         <v/>
       </c>
-      <c r="H26" s="18" t="str">
-        <f aca="true">IF(J26 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H26" s="18"/>
       <c r="I26" s="18" t="str">
         <f aca="true">IF(J26 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K26" s="20" t="n">
-        <f aca="true">IF(J26 = "-", -INDIRECT("C" &amp; ROW() - 1),F26)</f>
-        <v>0</v>
+      <c r="K26" s="20" t="str">
+        <f aca="true">IF(J26 = "-", -INDIRECT("C" &amp; ROW() - 1),E26)</f>
+        <v/>
       </c>
       <c r="L26" s="17" t="n">
         <f aca="true">IF(J26 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K26)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K26)))), 0)</f>
@@ -2009,7 +1938,7 @@
         <v/>
       </c>
       <c r="E27" s="19" t="str">
-        <f aca="false">IF(D27="-", "-", IF(D27="", "", F27*VLOOKUP(D27, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D27="-", "-", IF(D27="", "", INT(F27*VLOOKUP(D27, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F27" s="20"/>
@@ -2017,17 +1946,14 @@
         <f aca="true">IF(J27="","",(INDIRECT("N" &amp; ROW() - 1) - N27))</f>
         <v/>
       </c>
-      <c r="H27" s="18" t="str">
-        <f aca="true">IF(J27 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H27" s="18"/>
       <c r="I27" s="18" t="str">
         <f aca="true">IF(J27 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K27" s="20" t="n">
-        <f aca="true">IF(J27 = "-", -INDIRECT("C" &amp; ROW() - 1),F27)</f>
-        <v>0</v>
+      <c r="K27" s="20" t="str">
+        <f aca="true">IF(J27 = "-", -INDIRECT("C" &amp; ROW() - 1),E27)</f>
+        <v/>
       </c>
       <c r="L27" s="17" t="n">
         <f aca="true">IF(J27 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K27)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K27)))), 0)</f>
@@ -2061,7 +1987,7 @@
         <v/>
       </c>
       <c r="E28" s="19" t="str">
-        <f aca="false">IF(D28="-", "-", IF(D28="", "", F28*VLOOKUP(D28, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D28="-", "-", IF(D28="", "", INT(F28*VLOOKUP(D28, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F28" s="20"/>
@@ -2069,17 +1995,14 @@
         <f aca="true">IF(J28="","",(INDIRECT("N" &amp; ROW() - 1) - N28))</f>
         <v/>
       </c>
-      <c r="H28" s="18" t="str">
-        <f aca="true">IF(J28 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H28" s="18"/>
       <c r="I28" s="18" t="str">
         <f aca="true">IF(J28 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K28" s="20" t="n">
-        <f aca="true">IF(J28 = "-", -INDIRECT("C" &amp; ROW() - 1),F28)</f>
-        <v>0</v>
+      <c r="K28" s="20" t="str">
+        <f aca="true">IF(J28 = "-", -INDIRECT("C" &amp; ROW() - 1),E28)</f>
+        <v/>
       </c>
       <c r="L28" s="17" t="n">
         <f aca="true">IF(J28 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K28)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K28)))), 0)</f>
@@ -2113,7 +2036,7 @@
         <v/>
       </c>
       <c r="E29" s="19" t="str">
-        <f aca="false">IF(D29="-", "-", IF(D29="", "", F29*VLOOKUP(D29, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D29="-", "-", IF(D29="", "", INT(F29*VLOOKUP(D29, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F29" s="20"/>
@@ -2121,17 +2044,14 @@
         <f aca="true">IF(J29="","",(INDIRECT("N" &amp; ROW() - 1) - N29))</f>
         <v/>
       </c>
-      <c r="H29" s="18" t="str">
-        <f aca="true">IF(J29 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H29" s="18"/>
       <c r="I29" s="18" t="str">
         <f aca="true">IF(J29 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K29" s="20" t="n">
-        <f aca="true">IF(J29 = "-", -INDIRECT("C" &amp; ROW() - 1),F29)</f>
-        <v>0</v>
+      <c r="K29" s="20" t="str">
+        <f aca="true">IF(J29 = "-", -INDIRECT("C" &amp; ROW() - 1),E29)</f>
+        <v/>
       </c>
       <c r="L29" s="17" t="n">
         <f aca="true">IF(J29 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K29)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K29)))), 0)</f>
@@ -2165,7 +2085,7 @@
         <v/>
       </c>
       <c r="E30" s="19" t="str">
-        <f aca="false">IF(D30="-", "-", IF(D30="", "", F30*VLOOKUP(D30, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D30="-", "-", IF(D30="", "", INT(F30*VLOOKUP(D30, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F30" s="20"/>
@@ -2173,17 +2093,14 @@
         <f aca="true">IF(J30="","",(INDIRECT("N" &amp; ROW() - 1) - N30))</f>
         <v/>
       </c>
-      <c r="H30" s="18" t="str">
-        <f aca="true">IF(J30 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H30" s="18"/>
       <c r="I30" s="18" t="str">
         <f aca="true">IF(J30 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K30" s="20" t="n">
-        <f aca="true">IF(J30 = "-", -INDIRECT("C" &amp; ROW() - 1),F30)</f>
-        <v>0</v>
+      <c r="K30" s="20" t="str">
+        <f aca="true">IF(J30 = "-", -INDIRECT("C" &amp; ROW() - 1),E30)</f>
+        <v/>
       </c>
       <c r="L30" s="17" t="n">
         <f aca="true">IF(J30 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K30)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K30)))), 0)</f>
@@ -2217,7 +2134,7 @@
         <v/>
       </c>
       <c r="E31" s="19" t="str">
-        <f aca="false">IF(D31="-", "-", IF(D31="", "", F31*VLOOKUP(D31, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D31="-", "-", IF(D31="", "", INT(F31*VLOOKUP(D31, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F31" s="20"/>
@@ -2225,17 +2142,14 @@
         <f aca="true">IF(J31="","",(INDIRECT("N" &amp; ROW() - 1) - N31))</f>
         <v/>
       </c>
-      <c r="H31" s="18" t="str">
-        <f aca="true">IF(J31 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H31" s="18"/>
       <c r="I31" s="18" t="str">
         <f aca="true">IF(J31 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K31" s="20" t="n">
-        <f aca="true">IF(J31 = "-", -INDIRECT("C" &amp; ROW() - 1),F31)</f>
-        <v>0</v>
+      <c r="K31" s="20" t="str">
+        <f aca="true">IF(J31 = "-", -INDIRECT("C" &amp; ROW() - 1),E31)</f>
+        <v/>
       </c>
       <c r="L31" s="17" t="n">
         <f aca="true">IF(J31 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K31)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K31)))), 0)</f>
@@ -2269,7 +2183,7 @@
         <v/>
       </c>
       <c r="E32" s="19" t="str">
-        <f aca="false">IF(D32="-", "-", IF(D32="", "", F32*VLOOKUP(D32, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D32="-", "-", IF(D32="", "", INT(F32*VLOOKUP(D32, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F32" s="20"/>
@@ -2277,17 +2191,14 @@
         <f aca="true">IF(J32="","",(INDIRECT("N" &amp; ROW() - 1) - N32))</f>
         <v/>
       </c>
-      <c r="H32" s="18" t="str">
-        <f aca="true">IF(J32 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H32" s="18"/>
       <c r="I32" s="18" t="str">
         <f aca="true">IF(J32 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K32" s="20" t="n">
-        <f aca="true">IF(J32 = "-", -INDIRECT("C" &amp; ROW() - 1),F32)</f>
-        <v>0</v>
+      <c r="K32" s="20" t="str">
+        <f aca="true">IF(J32 = "-", -INDIRECT("C" &amp; ROW() - 1),E32)</f>
+        <v/>
       </c>
       <c r="L32" s="17" t="n">
         <f aca="true">IF(J32 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K32)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K32)))), 0)</f>
@@ -2321,7 +2232,7 @@
         <v/>
       </c>
       <c r="E33" s="19" t="str">
-        <f aca="false">IF(D33="-", "-", IF(D33="", "", F33*VLOOKUP(D33, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D33="-", "-", IF(D33="", "", INT(F33*VLOOKUP(D33, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F33" s="20"/>
@@ -2329,17 +2240,14 @@
         <f aca="true">IF(J33="","",(INDIRECT("N" &amp; ROW() - 1) - N33))</f>
         <v/>
       </c>
-      <c r="H33" s="18" t="str">
-        <f aca="true">IF(J33 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H33" s="18"/>
       <c r="I33" s="18" t="str">
         <f aca="true">IF(J33 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K33" s="20" t="n">
-        <f aca="true">IF(J33 = "-", -INDIRECT("C" &amp; ROW() - 1),F33)</f>
-        <v>0</v>
+      <c r="K33" s="20" t="str">
+        <f aca="true">IF(J33 = "-", -INDIRECT("C" &amp; ROW() - 1),E33)</f>
+        <v/>
       </c>
       <c r="L33" s="17" t="n">
         <f aca="true">IF(J33 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K33)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K33)))), 0)</f>
@@ -2373,7 +2281,7 @@
         <v/>
       </c>
       <c r="E34" s="19" t="str">
-        <f aca="false">IF(D34="-", "-", IF(D34="", "", F34*VLOOKUP(D34, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D34="-", "-", IF(D34="", "", INT(F34*VLOOKUP(D34, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F34" s="20"/>
@@ -2381,17 +2289,14 @@
         <f aca="true">IF(J34="","",(INDIRECT("N" &amp; ROW() - 1) - N34))</f>
         <v/>
       </c>
-      <c r="H34" s="18" t="str">
-        <f aca="true">IF(J34 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H34" s="18"/>
       <c r="I34" s="18" t="str">
         <f aca="true">IF(J34 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K34" s="20" t="n">
-        <f aca="true">IF(J34 = "-", -INDIRECT("C" &amp; ROW() - 1),F34)</f>
-        <v>0</v>
+      <c r="K34" s="20" t="str">
+        <f aca="true">IF(J34 = "-", -INDIRECT("C" &amp; ROW() - 1),E34)</f>
+        <v/>
       </c>
       <c r="L34" s="17" t="n">
         <f aca="true">IF(J34 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K34)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K34)))), 0)</f>
@@ -2425,7 +2330,7 @@
         <v/>
       </c>
       <c r="E35" s="19" t="str">
-        <f aca="false">IF(D35="-", "-", IF(D35="", "", F35*VLOOKUP(D35, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D35="-", "-", IF(D35="", "", INT(F35*VLOOKUP(D35, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F35" s="20"/>
@@ -2433,17 +2338,14 @@
         <f aca="true">IF(J35="","",(INDIRECT("N" &amp; ROW() - 1) - N35))</f>
         <v/>
       </c>
-      <c r="H35" s="18" t="str">
-        <f aca="true">IF(J35 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H35" s="18"/>
       <c r="I35" s="18" t="str">
         <f aca="true">IF(J35 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K35" s="20" t="n">
-        <f aca="true">IF(J35 = "-", -INDIRECT("C" &amp; ROW() - 1),F35)</f>
-        <v>0</v>
+      <c r="K35" s="20" t="str">
+        <f aca="true">IF(J35 = "-", -INDIRECT("C" &amp; ROW() - 1),E35)</f>
+        <v/>
       </c>
       <c r="L35" s="17" t="n">
         <f aca="true">IF(J35 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K35)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K35)))), 0)</f>
@@ -2477,7 +2379,7 @@
         <v/>
       </c>
       <c r="E36" s="19" t="str">
-        <f aca="false">IF(D36="-", "-", IF(D36="", "", F36*VLOOKUP(D36, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D36="-", "-", IF(D36="", "", INT(F36*VLOOKUP(D36, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F36" s="20"/>
@@ -2485,17 +2387,14 @@
         <f aca="true">IF(J36="","",(INDIRECT("N" &amp; ROW() - 1) - N36))</f>
         <v/>
       </c>
-      <c r="H36" s="18" t="str">
-        <f aca="true">IF(J36 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H36" s="18"/>
       <c r="I36" s="18" t="str">
         <f aca="true">IF(J36 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K36" s="20" t="n">
-        <f aca="true">IF(J36 = "-", -INDIRECT("C" &amp; ROW() - 1),F36)</f>
-        <v>0</v>
+      <c r="K36" s="20" t="str">
+        <f aca="true">IF(J36 = "-", -INDIRECT("C" &amp; ROW() - 1),E36)</f>
+        <v/>
       </c>
       <c r="L36" s="17" t="n">
         <f aca="true">IF(J36 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K36)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K36)))), 0)</f>
@@ -2529,7 +2428,7 @@
         <v/>
       </c>
       <c r="E37" s="19" t="str">
-        <f aca="false">IF(D37="-", "-", IF(D37="", "", F37*VLOOKUP(D37, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D37="-", "-", IF(D37="", "", INT(F37*VLOOKUP(D37, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F37" s="20"/>
@@ -2537,17 +2436,14 @@
         <f aca="true">IF(J37="","",(INDIRECT("N" &amp; ROW() - 1) - N37))</f>
         <v/>
       </c>
-      <c r="H37" s="18" t="str">
-        <f aca="true">IF(J37 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H37" s="18"/>
       <c r="I37" s="18" t="str">
         <f aca="true">IF(J37 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K37" s="20" t="n">
-        <f aca="true">IF(J37 = "-", -INDIRECT("C" &amp; ROW() - 1),F37)</f>
-        <v>0</v>
+      <c r="K37" s="20" t="str">
+        <f aca="true">IF(J37 = "-", -INDIRECT("C" &amp; ROW() - 1),E37)</f>
+        <v/>
       </c>
       <c r="L37" s="17" t="n">
         <f aca="true">IF(J37 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K37)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K37)))), 0)</f>
@@ -2581,7 +2477,7 @@
         <v/>
       </c>
       <c r="E38" s="19" t="str">
-        <f aca="false">IF(D38="-", "-", IF(D38="", "", F38*VLOOKUP(D38, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D38="-", "-", IF(D38="", "", INT(F38*VLOOKUP(D38, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F38" s="20"/>
@@ -2589,17 +2485,14 @@
         <f aca="true">IF(J38="","",(INDIRECT("N" &amp; ROW() - 1) - N38))</f>
         <v/>
       </c>
-      <c r="H38" s="18" t="str">
-        <f aca="true">IF(J38 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H38" s="18"/>
       <c r="I38" s="18" t="str">
         <f aca="true">IF(J38 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K38" s="20" t="n">
-        <f aca="true">IF(J38 = "-", -INDIRECT("C" &amp; ROW() - 1),F38)</f>
-        <v>0</v>
+      <c r="K38" s="20" t="str">
+        <f aca="true">IF(J38 = "-", -INDIRECT("C" &amp; ROW() - 1),E38)</f>
+        <v/>
       </c>
       <c r="L38" s="17" t="n">
         <f aca="true">IF(J38 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K38)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K38)))), 0)</f>
@@ -2633,7 +2526,7 @@
         <v/>
       </c>
       <c r="E39" s="19" t="str">
-        <f aca="false">IF(D39="-", "-", IF(D39="", "", F39*VLOOKUP(D39, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D39="-", "-", IF(D39="", "", INT(F39*VLOOKUP(D39, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F39" s="20"/>
@@ -2641,17 +2534,14 @@
         <f aca="true">IF(J39="","",(INDIRECT("N" &amp; ROW() - 1) - N39))</f>
         <v/>
       </c>
-      <c r="H39" s="18" t="str">
-        <f aca="true">IF(J39 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H39" s="18"/>
       <c r="I39" s="18" t="str">
         <f aca="true">IF(J39 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K39" s="20" t="n">
-        <f aca="true">IF(J39 = "-", -INDIRECT("C" &amp; ROW() - 1),F39)</f>
-        <v>0</v>
+      <c r="K39" s="20" t="str">
+        <f aca="true">IF(J39 = "-", -INDIRECT("C" &amp; ROW() - 1),E39)</f>
+        <v/>
       </c>
       <c r="L39" s="17" t="n">
         <f aca="true">IF(J39 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K39)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K39)))), 0)</f>
@@ -2685,7 +2575,7 @@
         <v/>
       </c>
       <c r="E40" s="19" t="str">
-        <f aca="false">IF(D40="-", "-", IF(D40="", "", F40*VLOOKUP(D40, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D40="-", "-", IF(D40="", "", INT(F40*VLOOKUP(D40, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F40" s="20"/>
@@ -2693,17 +2583,14 @@
         <f aca="true">IF(J40="","",(INDIRECT("N" &amp; ROW() - 1) - N40))</f>
         <v/>
       </c>
-      <c r="H40" s="18" t="str">
-        <f aca="true">IF(J40 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H40" s="18"/>
       <c r="I40" s="18" t="str">
         <f aca="true">IF(J40 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K40" s="20" t="n">
-        <f aca="true">IF(J40 = "-", -INDIRECT("C" &amp; ROW() - 1),F40)</f>
-        <v>0</v>
+      <c r="K40" s="20" t="str">
+        <f aca="true">IF(J40 = "-", -INDIRECT("C" &amp; ROW() - 1),E40)</f>
+        <v/>
       </c>
       <c r="L40" s="17" t="n">
         <f aca="true">IF(J40 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K40)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K40)))), 0)</f>
@@ -2737,7 +2624,7 @@
         <v/>
       </c>
       <c r="E41" s="19" t="str">
-        <f aca="false">IF(D41="-", "-", IF(D41="", "", F41*VLOOKUP(D41, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D41="-", "-", IF(D41="", "", INT(F41*VLOOKUP(D41, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F41" s="20"/>
@@ -2745,17 +2632,14 @@
         <f aca="true">IF(J41="","",(INDIRECT("N" &amp; ROW() - 1) - N41))</f>
         <v/>
       </c>
-      <c r="H41" s="18" t="str">
-        <f aca="true">IF(J41 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H41" s="18"/>
       <c r="I41" s="18" t="str">
         <f aca="true">IF(J41 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K41" s="20" t="n">
-        <f aca="true">IF(J41 = "-", -INDIRECT("C" &amp; ROW() - 1),F41)</f>
-        <v>0</v>
+      <c r="K41" s="20" t="str">
+        <f aca="true">IF(J41 = "-", -INDIRECT("C" &amp; ROW() - 1),E41)</f>
+        <v/>
       </c>
       <c r="L41" s="17" t="n">
         <f aca="true">IF(J41 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K41)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K41)))), 0)</f>
@@ -2789,7 +2673,7 @@
         <v/>
       </c>
       <c r="E42" s="19" t="str">
-        <f aca="false">IF(D42="-", "-", IF(D42="", "", F42*VLOOKUP(D42, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D42="-", "-", IF(D42="", "", INT(F42*VLOOKUP(D42, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F42" s="20"/>
@@ -2797,17 +2681,14 @@
         <f aca="true">IF(J42="","",(INDIRECT("N" &amp; ROW() - 1) - N42))</f>
         <v/>
       </c>
-      <c r="H42" s="18" t="str">
-        <f aca="true">IF(J42 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H42" s="18"/>
       <c r="I42" s="18" t="str">
         <f aca="true">IF(J42 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K42" s="20" t="n">
-        <f aca="true">IF(J42 = "-", -INDIRECT("C" &amp; ROW() - 1),F42)</f>
-        <v>0</v>
+      <c r="K42" s="20" t="str">
+        <f aca="true">IF(J42 = "-", -INDIRECT("C" &amp; ROW() - 1),E42)</f>
+        <v/>
       </c>
       <c r="L42" s="17" t="n">
         <f aca="true">IF(J42 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K42)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K42)))), 0)</f>
@@ -2841,7 +2722,7 @@
         <v/>
       </c>
       <c r="E43" s="19" t="str">
-        <f aca="false">IF(D43="-", "-", IF(D43="", "", F43*VLOOKUP(D43, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D43="-", "-", IF(D43="", "", INT(F43*VLOOKUP(D43, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F43" s="20"/>
@@ -2849,17 +2730,14 @@
         <f aca="true">IF(J43="","",(INDIRECT("N" &amp; ROW() - 1) - N43))</f>
         <v/>
       </c>
-      <c r="H43" s="18" t="str">
-        <f aca="true">IF(J43 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H43" s="18"/>
       <c r="I43" s="18" t="str">
         <f aca="true">IF(J43 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K43" s="20" t="n">
-        <f aca="true">IF(J43 = "-", -INDIRECT("C" &amp; ROW() - 1),F43)</f>
-        <v>0</v>
+      <c r="K43" s="20" t="str">
+        <f aca="true">IF(J43 = "-", -INDIRECT("C" &amp; ROW() - 1),E43)</f>
+        <v/>
       </c>
       <c r="L43" s="17" t="n">
         <f aca="true">IF(J43 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K43)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K43)))), 0)</f>
@@ -2893,7 +2771,7 @@
         <v/>
       </c>
       <c r="E44" s="19" t="str">
-        <f aca="false">IF(D44="-", "-", IF(D44="", "", F44*VLOOKUP(D44, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D44="-", "-", IF(D44="", "", INT(F44*VLOOKUP(D44, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F44" s="20"/>
@@ -2901,17 +2779,14 @@
         <f aca="true">IF(J44="","",(INDIRECT("N" &amp; ROW() - 1) - N44))</f>
         <v/>
       </c>
-      <c r="H44" s="18" t="str">
-        <f aca="true">IF(J44 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H44" s="18"/>
       <c r="I44" s="18" t="str">
         <f aca="true">IF(J44 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K44" s="20" t="n">
-        <f aca="true">IF(J44 = "-", -INDIRECT("C" &amp; ROW() - 1),F44)</f>
-        <v>0</v>
+      <c r="K44" s="20" t="str">
+        <f aca="true">IF(J44 = "-", -INDIRECT("C" &amp; ROW() - 1),E44)</f>
+        <v/>
       </c>
       <c r="L44" s="17" t="n">
         <f aca="true">IF(J44 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K44)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K44)))), 0)</f>
@@ -2945,7 +2820,7 @@
         <v/>
       </c>
       <c r="E45" s="19" t="str">
-        <f aca="false">IF(D45="-", "-", IF(D45="", "", F45*VLOOKUP(D45, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D45="-", "-", IF(D45="", "", INT(F45*VLOOKUP(D45, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F45" s="20"/>
@@ -2953,17 +2828,14 @@
         <f aca="true">IF(J45="","",(INDIRECT("N" &amp; ROW() - 1) - N45))</f>
         <v/>
       </c>
-      <c r="H45" s="18" t="str">
-        <f aca="true">IF(J45 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H45" s="18"/>
       <c r="I45" s="18" t="str">
         <f aca="true">IF(J45 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K45" s="20" t="n">
-        <f aca="true">IF(J45 = "-", -INDIRECT("C" &amp; ROW() - 1),F45)</f>
-        <v>0</v>
+      <c r="K45" s="20" t="str">
+        <f aca="true">IF(J45 = "-", -INDIRECT("C" &amp; ROW() - 1),E45)</f>
+        <v/>
       </c>
       <c r="L45" s="17" t="n">
         <f aca="true">IF(J45 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K45)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K45)))), 0)</f>
@@ -2997,7 +2869,7 @@
         <v/>
       </c>
       <c r="E46" s="19" t="str">
-        <f aca="false">IF(D46="-", "-", IF(D46="", "", F46*VLOOKUP(D46, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D46="-", "-", IF(D46="", "", INT(F46*VLOOKUP(D46, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F46" s="20"/>
@@ -3005,17 +2877,14 @@
         <f aca="true">IF(J46="","",(INDIRECT("N" &amp; ROW() - 1) - N46))</f>
         <v/>
       </c>
-      <c r="H46" s="18" t="str">
-        <f aca="true">IF(J46 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H46" s="18"/>
       <c r="I46" s="18" t="str">
         <f aca="true">IF(J46 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K46" s="20" t="n">
-        <f aca="true">IF(J46 = "-", -INDIRECT("C" &amp; ROW() - 1),F46)</f>
-        <v>0</v>
+      <c r="K46" s="20" t="str">
+        <f aca="true">IF(J46 = "-", -INDIRECT("C" &amp; ROW() - 1),E46)</f>
+        <v/>
       </c>
       <c r="L46" s="17" t="n">
         <f aca="true">IF(J46 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K46)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K46)))), 0)</f>
@@ -3049,7 +2918,7 @@
         <v/>
       </c>
       <c r="E47" s="19" t="str">
-        <f aca="false">IF(D47="-", "-", IF(D47="", "", F47*VLOOKUP(D47, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D47="-", "-", IF(D47="", "", INT(F47*VLOOKUP(D47, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F47" s="20"/>
@@ -3057,17 +2926,14 @@
         <f aca="true">IF(J47="","",(INDIRECT("N" &amp; ROW() - 1) - N47))</f>
         <v/>
       </c>
-      <c r="H47" s="18" t="str">
-        <f aca="true">IF(J47 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H47" s="18"/>
       <c r="I47" s="18" t="str">
         <f aca="true">IF(J47 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K47" s="20" t="n">
-        <f aca="true">IF(J47 = "-", -INDIRECT("C" &amp; ROW() - 1),F47)</f>
-        <v>0</v>
+      <c r="K47" s="20" t="str">
+        <f aca="true">IF(J47 = "-", -INDIRECT("C" &amp; ROW() - 1),E47)</f>
+        <v/>
       </c>
       <c r="L47" s="17" t="n">
         <f aca="true">IF(J47 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K47)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K47)))), 0)</f>
@@ -3101,7 +2967,7 @@
         <v/>
       </c>
       <c r="E48" s="19" t="str">
-        <f aca="false">IF(D48="-", "-", IF(D48="", "", F48*VLOOKUP(D48, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D48="-", "-", IF(D48="", "", INT(F48*VLOOKUP(D48, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F48" s="20"/>
@@ -3109,17 +2975,14 @@
         <f aca="true">IF(J48="","",(INDIRECT("N" &amp; ROW() - 1) - N48))</f>
         <v/>
       </c>
-      <c r="H48" s="18" t="str">
-        <f aca="true">IF(J48 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H48" s="18"/>
       <c r="I48" s="18" t="str">
         <f aca="true">IF(J48 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K48" s="20" t="n">
-        <f aca="true">IF(J48 = "-", -INDIRECT("C" &amp; ROW() - 1),F48)</f>
-        <v>0</v>
+      <c r="K48" s="20" t="str">
+        <f aca="true">IF(J48 = "-", -INDIRECT("C" &amp; ROW() - 1),E48)</f>
+        <v/>
       </c>
       <c r="L48" s="17" t="n">
         <f aca="true">IF(J48 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K48)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K48)))), 0)</f>
@@ -3153,7 +3016,7 @@
         <v/>
       </c>
       <c r="E49" s="19" t="str">
-        <f aca="false">IF(D49="-", "-", IF(D49="", "", F49*VLOOKUP(D49, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D49="-", "-", IF(D49="", "", INT(F49*VLOOKUP(D49, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F49" s="20"/>
@@ -3161,17 +3024,14 @@
         <f aca="true">IF(J49="","",(INDIRECT("N" &amp; ROW() - 1) - N49))</f>
         <v/>
       </c>
-      <c r="H49" s="18" t="str">
-        <f aca="true">IF(J49 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H49" s="18"/>
       <c r="I49" s="18" t="str">
         <f aca="true">IF(J49 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K49" s="20" t="n">
-        <f aca="true">IF(J49 = "-", -INDIRECT("C" &amp; ROW() - 1),F49)</f>
-        <v>0</v>
+      <c r="K49" s="20" t="str">
+        <f aca="true">IF(J49 = "-", -INDIRECT("C" &amp; ROW() - 1),E49)</f>
+        <v/>
       </c>
       <c r="L49" s="17" t="n">
         <f aca="true">IF(J49 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K49)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K49)))), 0)</f>
@@ -3205,7 +3065,7 @@
         <v/>
       </c>
       <c r="E50" s="19" t="str">
-        <f aca="false">IF(D50="-", "-", IF(D50="", "", F50*VLOOKUP(D50, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D50="-", "-", IF(D50="", "", INT(F50*VLOOKUP(D50, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F50" s="20"/>
@@ -3213,17 +3073,14 @@
         <f aca="true">IF(J50="","",(INDIRECT("N" &amp; ROW() - 1) - N50))</f>
         <v/>
       </c>
-      <c r="H50" s="18" t="str">
-        <f aca="true">IF(J50 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H50" s="18"/>
       <c r="I50" s="18" t="str">
         <f aca="true">IF(J50 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K50" s="20" t="n">
-        <f aca="true">IF(J50 = "-", -INDIRECT("C" &amp; ROW() - 1),F50)</f>
-        <v>0</v>
+      <c r="K50" s="20" t="str">
+        <f aca="true">IF(J50 = "-", -INDIRECT("C" &amp; ROW() - 1),E50)</f>
+        <v/>
       </c>
       <c r="L50" s="17" t="n">
         <f aca="true">IF(J50 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K50)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K50)))), 0)</f>
@@ -3257,7 +3114,7 @@
         <v/>
       </c>
       <c r="E51" s="19" t="str">
-        <f aca="false">IF(D51="-", "-", IF(D51="", "", F51*VLOOKUP(D51, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D51="-", "-", IF(D51="", "", INT(F51*VLOOKUP(D51, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F51" s="20"/>
@@ -3265,17 +3122,14 @@
         <f aca="true">IF(J51="","",(INDIRECT("N" &amp; ROW() - 1) - N51))</f>
         <v/>
       </c>
-      <c r="H51" s="18" t="str">
-        <f aca="true">IF(J51 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H51" s="18"/>
       <c r="I51" s="18" t="str">
         <f aca="true">IF(J51 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K51" s="20" t="n">
-        <f aca="true">IF(J51 = "-", -INDIRECT("C" &amp; ROW() - 1),F51)</f>
-        <v>0</v>
+      <c r="K51" s="20" t="str">
+        <f aca="true">IF(J51 = "-", -INDIRECT("C" &amp; ROW() - 1),E51)</f>
+        <v/>
       </c>
       <c r="L51" s="17" t="n">
         <f aca="true">IF(J51 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K51)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K51)))), 0)</f>
@@ -3309,7 +3163,7 @@
         <v/>
       </c>
       <c r="E52" s="19" t="str">
-        <f aca="false">IF(D52="-", "-", IF(D52="", "", F52*VLOOKUP(D52, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D52="-", "-", IF(D52="", "", INT(F52*VLOOKUP(D52, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F52" s="20"/>
@@ -3317,17 +3171,14 @@
         <f aca="true">IF(J52="","",(INDIRECT("N" &amp; ROW() - 1) - N52))</f>
         <v/>
       </c>
-      <c r="H52" s="18" t="str">
-        <f aca="true">IF(J52 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H52" s="18"/>
       <c r="I52" s="18" t="str">
         <f aca="true">IF(J52 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K52" s="20" t="n">
-        <f aca="true">IF(J52 = "-", -INDIRECT("C" &amp; ROW() - 1),F52)</f>
-        <v>0</v>
+      <c r="K52" s="20" t="str">
+        <f aca="true">IF(J52 = "-", -INDIRECT("C" &amp; ROW() - 1),E52)</f>
+        <v/>
       </c>
       <c r="L52" s="17" t="n">
         <f aca="true">IF(J52 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K52)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K52)))), 0)</f>
@@ -3361,7 +3212,7 @@
         <v/>
       </c>
       <c r="E53" s="19" t="str">
-        <f aca="false">IF(D53="-", "-", IF(D53="", "", F53*VLOOKUP(D53, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D53="-", "-", IF(D53="", "", INT(F53*VLOOKUP(D53, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F53" s="20"/>
@@ -3369,17 +3220,14 @@
         <f aca="true">IF(J53="","",(INDIRECT("N" &amp; ROW() - 1) - N53))</f>
         <v/>
       </c>
-      <c r="H53" s="18" t="str">
-        <f aca="true">IF(J53 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H53" s="18"/>
       <c r="I53" s="18" t="str">
         <f aca="true">IF(J53 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K53" s="20" t="n">
-        <f aca="true">IF(J53 = "-", -INDIRECT("C" &amp; ROW() - 1),F53)</f>
-        <v>0</v>
+      <c r="K53" s="20" t="str">
+        <f aca="true">IF(J53 = "-", -INDIRECT("C" &amp; ROW() - 1),E53)</f>
+        <v/>
       </c>
       <c r="L53" s="17" t="n">
         <f aca="true">IF(J53 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K53)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K53)))), 0)</f>
@@ -3413,7 +3261,7 @@
         <v/>
       </c>
       <c r="E54" s="19" t="str">
-        <f aca="false">IF(D54="-", "-", IF(D54="", "", F54*VLOOKUP(D54, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D54="-", "-", IF(D54="", "", INT(F54*VLOOKUP(D54, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F54" s="20"/>
@@ -3421,17 +3269,14 @@
         <f aca="true">IF(J54="","",(INDIRECT("N" &amp; ROW() - 1) - N54))</f>
         <v/>
       </c>
-      <c r="H54" s="18" t="str">
-        <f aca="true">IF(J54 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H54" s="18"/>
       <c r="I54" s="18" t="str">
         <f aca="true">IF(J54 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K54" s="20" t="n">
-        <f aca="true">IF(J54 = "-", -INDIRECT("C" &amp; ROW() - 1),F54)</f>
-        <v>0</v>
+      <c r="K54" s="20" t="str">
+        <f aca="true">IF(J54 = "-", -INDIRECT("C" &amp; ROW() - 1),E54)</f>
+        <v/>
       </c>
       <c r="L54" s="17" t="n">
         <f aca="true">IF(J54 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K54)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K54)))), 0)</f>
@@ -3465,7 +3310,7 @@
         <v/>
       </c>
       <c r="E55" s="19" t="str">
-        <f aca="false">IF(D55="-", "-", IF(D55="", "", F55*VLOOKUP(D55, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D55="-", "-", IF(D55="", "", INT(F55*VLOOKUP(D55, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F55" s="20"/>
@@ -3473,17 +3318,14 @@
         <f aca="true">IF(J55="","",(INDIRECT("N" &amp; ROW() - 1) - N55))</f>
         <v/>
       </c>
-      <c r="H55" s="18" t="str">
-        <f aca="true">IF(J55 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H55" s="18"/>
       <c r="I55" s="18" t="str">
         <f aca="true">IF(J55 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K55" s="20" t="n">
-        <f aca="true">IF(J55 = "-", -INDIRECT("C" &amp; ROW() - 1),F55)</f>
-        <v>0</v>
+      <c r="K55" s="20" t="str">
+        <f aca="true">IF(J55 = "-", -INDIRECT("C" &amp; ROW() - 1),E55)</f>
+        <v/>
       </c>
       <c r="L55" s="17" t="n">
         <f aca="true">IF(J55 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K55)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K55)))), 0)</f>
@@ -3517,7 +3359,7 @@
         <v/>
       </c>
       <c r="E56" s="19" t="str">
-        <f aca="false">IF(D56="-", "-", IF(D56="", "", F56*VLOOKUP(D56, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D56="-", "-", IF(D56="", "", INT(F56*VLOOKUP(D56, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F56" s="20"/>
@@ -3525,17 +3367,14 @@
         <f aca="true">IF(J56="","",(INDIRECT("N" &amp; ROW() - 1) - N56))</f>
         <v/>
       </c>
-      <c r="H56" s="18" t="str">
-        <f aca="true">IF(J56 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H56" s="18"/>
       <c r="I56" s="18" t="str">
         <f aca="true">IF(J56 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K56" s="20" t="n">
-        <f aca="true">IF(J56 = "-", -INDIRECT("C" &amp; ROW() - 1),F56)</f>
-        <v>0</v>
+      <c r="K56" s="20" t="str">
+        <f aca="true">IF(J56 = "-", -INDIRECT("C" &amp; ROW() - 1),E56)</f>
+        <v/>
       </c>
       <c r="L56" s="17" t="n">
         <f aca="true">IF(J56 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K56)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K56)))), 0)</f>
@@ -3569,7 +3408,7 @@
         <v/>
       </c>
       <c r="E57" s="19" t="str">
-        <f aca="false">IF(D57="-", "-", IF(D57="", "", F57*VLOOKUP(D57, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D57="-", "-", IF(D57="", "", INT(F57*VLOOKUP(D57, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F57" s="20"/>
@@ -3577,17 +3416,14 @@
         <f aca="true">IF(J57="","",(INDIRECT("N" &amp; ROW() - 1) - N57))</f>
         <v/>
       </c>
-      <c r="H57" s="18" t="str">
-        <f aca="true">IF(J57 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H57" s="18"/>
       <c r="I57" s="18" t="str">
         <f aca="true">IF(J57 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K57" s="20" t="n">
-        <f aca="true">IF(J57 = "-", -INDIRECT("C" &amp; ROW() - 1),F57)</f>
-        <v>0</v>
+      <c r="K57" s="20" t="str">
+        <f aca="true">IF(J57 = "-", -INDIRECT("C" &amp; ROW() - 1),E57)</f>
+        <v/>
       </c>
       <c r="L57" s="17" t="n">
         <f aca="true">IF(J57 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K57)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K57)))), 0)</f>
@@ -3621,7 +3457,7 @@
         <v/>
       </c>
       <c r="E58" s="19" t="str">
-        <f aca="false">IF(D58="-", "-", IF(D58="", "", F58*VLOOKUP(D58, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D58="-", "-", IF(D58="", "", INT(F58*VLOOKUP(D58, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F58" s="20"/>
@@ -3629,17 +3465,14 @@
         <f aca="true">IF(J58="","",(INDIRECT("N" &amp; ROW() - 1) - N58))</f>
         <v/>
       </c>
-      <c r="H58" s="18" t="str">
-        <f aca="true">IF(J58 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H58" s="18"/>
       <c r="I58" s="18" t="str">
         <f aca="true">IF(J58 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K58" s="20" t="n">
-        <f aca="true">IF(J58 = "-", -INDIRECT("C" &amp; ROW() - 1),F58)</f>
-        <v>0</v>
+      <c r="K58" s="20" t="str">
+        <f aca="true">IF(J58 = "-", -INDIRECT("C" &amp; ROW() - 1),E58)</f>
+        <v/>
       </c>
       <c r="L58" s="17" t="n">
         <f aca="true">IF(J58 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K58)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K58)))), 0)</f>
@@ -3673,7 +3506,7 @@
         <v/>
       </c>
       <c r="E59" s="19" t="str">
-        <f aca="false">IF(D59="-", "-", IF(D59="", "", F59*VLOOKUP(D59, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D59="-", "-", IF(D59="", "", INT(F59*VLOOKUP(D59, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F59" s="20"/>
@@ -3681,17 +3514,14 @@
         <f aca="true">IF(J59="","",(INDIRECT("N" &amp; ROW() - 1) - N59))</f>
         <v/>
       </c>
-      <c r="H59" s="18" t="str">
-        <f aca="true">IF(J59 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H59" s="18"/>
       <c r="I59" s="18" t="str">
         <f aca="true">IF(J59 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K59" s="20" t="n">
-        <f aca="true">IF(J59 = "-", -INDIRECT("C" &amp; ROW() - 1),F59)</f>
-        <v>0</v>
+      <c r="K59" s="20" t="str">
+        <f aca="true">IF(J59 = "-", -INDIRECT("C" &amp; ROW() - 1),E59)</f>
+        <v/>
       </c>
       <c r="L59" s="17" t="n">
         <f aca="true">IF(J59 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K59)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K59)))), 0)</f>
@@ -3725,7 +3555,7 @@
         <v/>
       </c>
       <c r="E60" s="19" t="str">
-        <f aca="false">IF(D60="-", "-", IF(D60="", "", F60*VLOOKUP(D60, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D60="-", "-", IF(D60="", "", INT(F60*VLOOKUP(D60, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F60" s="20"/>
@@ -3733,17 +3563,14 @@
         <f aca="true">IF(J60="","",(INDIRECT("N" &amp; ROW() - 1) - N60))</f>
         <v/>
       </c>
-      <c r="H60" s="18" t="str">
-        <f aca="true">IF(J60 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H60" s="18"/>
       <c r="I60" s="18" t="str">
         <f aca="true">IF(J60 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K60" s="20" t="n">
-        <f aca="true">IF(J60 = "-", -INDIRECT("C" &amp; ROW() - 1),F60)</f>
-        <v>0</v>
+      <c r="K60" s="20" t="str">
+        <f aca="true">IF(J60 = "-", -INDIRECT("C" &amp; ROW() - 1),E60)</f>
+        <v/>
       </c>
       <c r="L60" s="17" t="n">
         <f aca="true">IF(J60 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K60)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K60)))), 0)</f>
@@ -3777,7 +3604,7 @@
         <v/>
       </c>
       <c r="E61" s="19" t="str">
-        <f aca="false">IF(D61="-", "-", IF(D61="", "", F61*VLOOKUP(D61, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D61="-", "-", IF(D61="", "", INT(F61*VLOOKUP(D61, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F61" s="20"/>
@@ -3785,17 +3612,14 @@
         <f aca="true">IF(J61="","",(INDIRECT("N" &amp; ROW() - 1) - N61))</f>
         <v/>
       </c>
-      <c r="H61" s="18" t="str">
-        <f aca="true">IF(J61 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H61" s="18"/>
       <c r="I61" s="18" t="str">
         <f aca="true">IF(J61 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K61" s="20" t="n">
-        <f aca="true">IF(J61 = "-", -INDIRECT("C" &amp; ROW() - 1),F61)</f>
-        <v>0</v>
+      <c r="K61" s="20" t="str">
+        <f aca="true">IF(J61 = "-", -INDIRECT("C" &amp; ROW() - 1),E61)</f>
+        <v/>
       </c>
       <c r="L61" s="17" t="n">
         <f aca="true">IF(J61 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K61)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K61)))), 0)</f>
@@ -3829,7 +3653,7 @@
         <v/>
       </c>
       <c r="E62" s="19" t="str">
-        <f aca="false">IF(D62="-", "-", IF(D62="", "", F62*VLOOKUP(D62, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D62="-", "-", IF(D62="", "", INT(F62*VLOOKUP(D62, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F62" s="20"/>
@@ -3837,17 +3661,14 @@
         <f aca="true">IF(J62="","",(INDIRECT("N" &amp; ROW() - 1) - N62))</f>
         <v/>
       </c>
-      <c r="H62" s="18" t="str">
-        <f aca="true">IF(J62 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H62" s="18"/>
       <c r="I62" s="18" t="str">
         <f aca="true">IF(J62 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K62" s="20" t="n">
-        <f aca="true">IF(J62 = "-", -INDIRECT("C" &amp; ROW() - 1),F62)</f>
-        <v>0</v>
+      <c r="K62" s="20" t="str">
+        <f aca="true">IF(J62 = "-", -INDIRECT("C" &amp; ROW() - 1),E62)</f>
+        <v/>
       </c>
       <c r="L62" s="17" t="n">
         <f aca="true">IF(J62 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K62)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K62)))), 0)</f>
@@ -3881,7 +3702,7 @@
         <v/>
       </c>
       <c r="E63" s="19" t="str">
-        <f aca="false">IF(D63="-", "-", IF(D63="", "", F63*VLOOKUP(D63, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D63="-", "-", IF(D63="", "", INT(F63*VLOOKUP(D63, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F63" s="20"/>
@@ -3889,17 +3710,14 @@
         <f aca="true">IF(J63="","",(INDIRECT("N" &amp; ROW() - 1) - N63))</f>
         <v/>
       </c>
-      <c r="H63" s="18" t="str">
-        <f aca="true">IF(J63 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H63" s="18"/>
       <c r="I63" s="18" t="str">
         <f aca="true">IF(J63 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K63" s="20" t="n">
-        <f aca="true">IF(J63 = "-", -INDIRECT("C" &amp; ROW() - 1),F63)</f>
-        <v>0</v>
+      <c r="K63" s="20" t="str">
+        <f aca="true">IF(J63 = "-", -INDIRECT("C" &amp; ROW() - 1),E63)</f>
+        <v/>
       </c>
       <c r="L63" s="17" t="n">
         <f aca="true">IF(J63 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K63)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K63)))), 0)</f>
@@ -3933,7 +3751,7 @@
         <v/>
       </c>
       <c r="E64" s="19" t="str">
-        <f aca="false">IF(D64="-", "-", IF(D64="", "", F64*VLOOKUP(D64, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D64="-", "-", IF(D64="", "", INT(F64*VLOOKUP(D64, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F64" s="20"/>
@@ -3941,17 +3759,14 @@
         <f aca="true">IF(J64="","",(INDIRECT("N" &amp; ROW() - 1) - N64))</f>
         <v/>
       </c>
-      <c r="H64" s="18" t="str">
-        <f aca="true">IF(J64 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H64" s="18"/>
       <c r="I64" s="18" t="str">
         <f aca="true">IF(J64 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K64" s="20" t="n">
-        <f aca="true">IF(J64 = "-", -INDIRECT("C" &amp; ROW() - 1),F64)</f>
-        <v>0</v>
+      <c r="K64" s="20" t="str">
+        <f aca="true">IF(J64 = "-", -INDIRECT("C" &amp; ROW() - 1),E64)</f>
+        <v/>
       </c>
       <c r="L64" s="17" t="n">
         <f aca="true">IF(J64 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K64)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K64)))), 0)</f>
@@ -3985,7 +3800,7 @@
         <v/>
       </c>
       <c r="E65" s="19" t="str">
-        <f aca="false">IF(D65="-", "-", IF(D65="", "", F65*VLOOKUP(D65, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D65="-", "-", IF(D65="", "", INT(F65*VLOOKUP(D65, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F65" s="20"/>
@@ -3993,17 +3808,14 @@
         <f aca="true">IF(J65="","",(INDIRECT("N" &amp; ROW() - 1) - N65))</f>
         <v/>
       </c>
-      <c r="H65" s="18" t="str">
-        <f aca="true">IF(J65 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H65" s="18"/>
       <c r="I65" s="18" t="str">
         <f aca="true">IF(J65 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K65" s="20" t="n">
-        <f aca="true">IF(J65 = "-", -INDIRECT("C" &amp; ROW() - 1),F65)</f>
-        <v>0</v>
+      <c r="K65" s="20" t="str">
+        <f aca="true">IF(J65 = "-", -INDIRECT("C" &amp; ROW() - 1),E65)</f>
+        <v/>
       </c>
       <c r="L65" s="17" t="n">
         <f aca="true">IF(J65 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K65)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K65)))), 0)</f>
@@ -4037,7 +3849,7 @@
         <v/>
       </c>
       <c r="E66" s="19" t="str">
-        <f aca="false">IF(D66="-", "-", IF(D66="", "", F66*VLOOKUP(D66, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D66="-", "-", IF(D66="", "", INT(F66*VLOOKUP(D66, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F66" s="20"/>
@@ -4045,17 +3857,14 @@
         <f aca="true">IF(J66="","",(INDIRECT("N" &amp; ROW() - 1) - N66))</f>
         <v/>
       </c>
-      <c r="H66" s="18" t="str">
-        <f aca="true">IF(J66 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H66" s="18"/>
       <c r="I66" s="18" t="str">
         <f aca="true">IF(J66 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K66" s="20" t="n">
-        <f aca="true">IF(J66 = "-", -INDIRECT("C" &amp; ROW() - 1),F66)</f>
-        <v>0</v>
+      <c r="K66" s="20" t="str">
+        <f aca="true">IF(J66 = "-", -INDIRECT("C" &amp; ROW() - 1),E66)</f>
+        <v/>
       </c>
       <c r="L66" s="17" t="n">
         <f aca="true">IF(J66 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K66)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K66)))), 0)</f>
@@ -4089,7 +3898,7 @@
         <v/>
       </c>
       <c r="E67" s="19" t="str">
-        <f aca="false">IF(D67="-", "-", IF(D67="", "", F67*VLOOKUP(D67, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D67="-", "-", IF(D67="", "", INT(F67*VLOOKUP(D67, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F67" s="20"/>
@@ -4097,17 +3906,14 @@
         <f aca="true">IF(J67="","",(INDIRECT("N" &amp; ROW() - 1) - N67))</f>
         <v/>
       </c>
-      <c r="H67" s="18" t="str">
-        <f aca="true">IF(J67 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H67" s="18"/>
       <c r="I67" s="18" t="str">
         <f aca="true">IF(J67 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K67" s="20" t="n">
-        <f aca="true">IF(J67 = "-", -INDIRECT("C" &amp; ROW() - 1),F67)</f>
-        <v>0</v>
+      <c r="K67" s="20" t="str">
+        <f aca="true">IF(J67 = "-", -INDIRECT("C" &amp; ROW() - 1),E67)</f>
+        <v/>
       </c>
       <c r="L67" s="17" t="n">
         <f aca="true">IF(J67 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K67)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K67)))), 0)</f>
@@ -4141,7 +3947,7 @@
         <v/>
       </c>
       <c r="E68" s="19" t="str">
-        <f aca="false">IF(D68="-", "-", IF(D68="", "", F68*VLOOKUP(D68, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D68="-", "-", IF(D68="", "", INT(F68*VLOOKUP(D68, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F68" s="20"/>
@@ -4149,17 +3955,14 @@
         <f aca="true">IF(J68="","",(INDIRECT("N" &amp; ROW() - 1) - N68))</f>
         <v/>
       </c>
-      <c r="H68" s="18" t="str">
-        <f aca="true">IF(J68 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H68" s="18"/>
       <c r="I68" s="18" t="str">
         <f aca="true">IF(J68 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K68" s="20" t="n">
-        <f aca="true">IF(J68 = "-", -INDIRECT("C" &amp; ROW() - 1),F68)</f>
-        <v>0</v>
+      <c r="K68" s="20" t="str">
+        <f aca="true">IF(J68 = "-", -INDIRECT("C" &amp; ROW() - 1),E68)</f>
+        <v/>
       </c>
       <c r="L68" s="17" t="n">
         <f aca="true">IF(J68 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K68)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K68)))), 0)</f>
@@ -4193,7 +3996,7 @@
         <v/>
       </c>
       <c r="E69" s="19" t="str">
-        <f aca="false">IF(D69="-", "-", IF(D69="", "", F69*VLOOKUP(D69, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D69="-", "-", IF(D69="", "", INT(F69*VLOOKUP(D69, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F69" s="20"/>
@@ -4201,17 +4004,14 @@
         <f aca="true">IF(J69="","",(INDIRECT("N" &amp; ROW() - 1) - N69))</f>
         <v/>
       </c>
-      <c r="H69" s="18" t="str">
-        <f aca="true">IF(J69 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H69" s="18"/>
       <c r="I69" s="18" t="str">
         <f aca="true">IF(J69 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K69" s="20" t="n">
-        <f aca="true">IF(J69 = "-", -INDIRECT("C" &amp; ROW() - 1),F69)</f>
-        <v>0</v>
+      <c r="K69" s="20" t="str">
+        <f aca="true">IF(J69 = "-", -INDIRECT("C" &amp; ROW() - 1),E69)</f>
+        <v/>
       </c>
       <c r="L69" s="17" t="n">
         <f aca="true">IF(J69 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K69)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K69)))), 0)</f>
@@ -4245,7 +4045,7 @@
         <v/>
       </c>
       <c r="E70" s="19" t="str">
-        <f aca="false">IF(D70="-", "-", IF(D70="", "", F70*VLOOKUP(D70, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D70="-", "-", IF(D70="", "", INT(F70*VLOOKUP(D70, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F70" s="20"/>
@@ -4253,17 +4053,14 @@
         <f aca="true">IF(J70="","",(INDIRECT("N" &amp; ROW() - 1) - N70))</f>
         <v/>
       </c>
-      <c r="H70" s="18" t="str">
-        <f aca="true">IF(J70 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H70" s="18"/>
       <c r="I70" s="18" t="str">
         <f aca="true">IF(J70 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K70" s="20" t="n">
-        <f aca="true">IF(J70 = "-", -INDIRECT("C" &amp; ROW() - 1),F70)</f>
-        <v>0</v>
+      <c r="K70" s="20" t="str">
+        <f aca="true">IF(J70 = "-", -INDIRECT("C" &amp; ROW() - 1),E70)</f>
+        <v/>
       </c>
       <c r="L70" s="17" t="n">
         <f aca="true">IF(J70 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K70)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K70)))), 0)</f>
@@ -4297,7 +4094,7 @@
         <v/>
       </c>
       <c r="E71" s="19" t="str">
-        <f aca="false">IF(D71="-", "-", IF(D71="", "", F71*VLOOKUP(D71, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D71="-", "-", IF(D71="", "", INT(F71*VLOOKUP(D71, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F71" s="20"/>
@@ -4305,17 +4102,14 @@
         <f aca="true">IF(J71="","",(INDIRECT("N" &amp; ROW() - 1) - N71))</f>
         <v/>
       </c>
-      <c r="H71" s="18" t="str">
-        <f aca="true">IF(J71 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H71" s="18"/>
       <c r="I71" s="18" t="str">
         <f aca="true">IF(J71 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K71" s="20" t="n">
-        <f aca="true">IF(J71 = "-", -INDIRECT("C" &amp; ROW() - 1),F71)</f>
-        <v>0</v>
+      <c r="K71" s="20" t="str">
+        <f aca="true">IF(J71 = "-", -INDIRECT("C" &amp; ROW() - 1),E71)</f>
+        <v/>
       </c>
       <c r="L71" s="17" t="n">
         <f aca="true">IF(J71 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K71)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K71)))), 0)</f>
@@ -4349,7 +4143,7 @@
         <v/>
       </c>
       <c r="E72" s="19" t="str">
-        <f aca="false">IF(D72="-", "-", IF(D72="", "", F72*VLOOKUP(D72, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D72="-", "-", IF(D72="", "", INT(F72*VLOOKUP(D72, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F72" s="20"/>
@@ -4357,17 +4151,14 @@
         <f aca="true">IF(J72="","",(INDIRECT("N" &amp; ROW() - 1) - N72))</f>
         <v/>
       </c>
-      <c r="H72" s="18" t="str">
-        <f aca="true">IF(J72 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H72" s="18"/>
       <c r="I72" s="18" t="str">
         <f aca="true">IF(J72 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K72" s="20" t="n">
-        <f aca="true">IF(J72 = "-", -INDIRECT("C" &amp; ROW() - 1),F72)</f>
-        <v>0</v>
+      <c r="K72" s="20" t="str">
+        <f aca="true">IF(J72 = "-", -INDIRECT("C" &amp; ROW() - 1),E72)</f>
+        <v/>
       </c>
       <c r="L72" s="17" t="n">
         <f aca="true">IF(J72 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K72)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K72)))), 0)</f>
@@ -4401,7 +4192,7 @@
         <v/>
       </c>
       <c r="E73" s="19" t="str">
-        <f aca="false">IF(D73="-", "-", IF(D73="", "", F73*VLOOKUP(D73, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D73="-", "-", IF(D73="", "", INT(F73*VLOOKUP(D73, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F73" s="20"/>
@@ -4409,17 +4200,14 @@
         <f aca="true">IF(J73="","",(INDIRECT("N" &amp; ROW() - 1) - N73))</f>
         <v/>
       </c>
-      <c r="H73" s="18" t="str">
-        <f aca="true">IF(J73 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H73" s="18"/>
       <c r="I73" s="18" t="str">
         <f aca="true">IF(J73 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K73" s="20" t="n">
-        <f aca="true">IF(J73 = "-", -INDIRECT("C" &amp; ROW() - 1),F73)</f>
-        <v>0</v>
+      <c r="K73" s="20" t="str">
+        <f aca="true">IF(J73 = "-", -INDIRECT("C" &amp; ROW() - 1),E73)</f>
+        <v/>
       </c>
       <c r="L73" s="17" t="n">
         <f aca="true">IF(J73 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K73)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K73)))), 0)</f>
@@ -4453,7 +4241,7 @@
         <v/>
       </c>
       <c r="E74" s="19" t="str">
-        <f aca="false">IF(D74="-", "-", IF(D74="", "", F74*VLOOKUP(D74, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D74="-", "-", IF(D74="", "", INT(F74*VLOOKUP(D74, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F74" s="20"/>
@@ -4461,17 +4249,14 @@
         <f aca="true">IF(J74="","",(INDIRECT("N" &amp; ROW() - 1) - N74))</f>
         <v/>
       </c>
-      <c r="H74" s="18" t="str">
-        <f aca="true">IF(J74 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H74" s="18"/>
       <c r="I74" s="18" t="str">
         <f aca="true">IF(J74 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K74" s="20" t="n">
-        <f aca="true">IF(J74 = "-", -INDIRECT("C" &amp; ROW() - 1),F74)</f>
-        <v>0</v>
+      <c r="K74" s="20" t="str">
+        <f aca="true">IF(J74 = "-", -INDIRECT("C" &amp; ROW() - 1),E74)</f>
+        <v/>
       </c>
       <c r="L74" s="17" t="n">
         <f aca="true">IF(J74 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K74)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K74)))), 0)</f>
@@ -4505,7 +4290,7 @@
         <v/>
       </c>
       <c r="E75" s="19" t="str">
-        <f aca="false">IF(D75="-", "-", IF(D75="", "", F75*VLOOKUP(D75, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D75="-", "-", IF(D75="", "", INT(F75*VLOOKUP(D75, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F75" s="20"/>
@@ -4513,17 +4298,14 @@
         <f aca="true">IF(J75="","",(INDIRECT("N" &amp; ROW() - 1) - N75))</f>
         <v/>
       </c>
-      <c r="H75" s="18" t="str">
-        <f aca="true">IF(J75 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H75" s="18"/>
       <c r="I75" s="18" t="str">
         <f aca="true">IF(J75 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K75" s="20" t="n">
-        <f aca="true">IF(J75 = "-", -INDIRECT("C" &amp; ROW() - 1),F75)</f>
-        <v>0</v>
+      <c r="K75" s="20" t="str">
+        <f aca="true">IF(J75 = "-", -INDIRECT("C" &amp; ROW() - 1),E75)</f>
+        <v/>
       </c>
       <c r="L75" s="17" t="n">
         <f aca="true">IF(J75="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K75))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K75)))),0)</f>
@@ -4557,7 +4339,7 @@
         <v/>
       </c>
       <c r="E76" s="19" t="str">
-        <f aca="false">IF(D76="-", "-", IF(D76="", "", F76*VLOOKUP(D76, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D76="-", "-", IF(D76="", "", INT(F76*VLOOKUP(D76, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F76" s="20"/>
@@ -4565,17 +4347,14 @@
         <f aca="true">IF(J76="","",(INDIRECT("N" &amp; ROW() - 1) - N76))</f>
         <v/>
       </c>
-      <c r="H76" s="18" t="str">
-        <f aca="true">IF(J76 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H76" s="18"/>
       <c r="I76" s="18" t="str">
         <f aca="true">IF(J76 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K76" s="20" t="n">
-        <f aca="true">IF(J76 = "-", -INDIRECT("C" &amp; ROW() - 1),F76)</f>
-        <v>0</v>
+      <c r="K76" s="20" t="str">
+        <f aca="true">IF(J76 = "-", -INDIRECT("C" &amp; ROW() - 1),E76)</f>
+        <v/>
       </c>
       <c r="L76" s="17" t="n">
         <f aca="true">IF(J76="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K76))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K76)))),0)</f>
@@ -4609,7 +4388,7 @@
         <v/>
       </c>
       <c r="E77" s="19" t="str">
-        <f aca="false">IF(D77="-", "-", IF(D77="", "", F77*VLOOKUP(D77, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D77="-", "-", IF(D77="", "", INT(F77*VLOOKUP(D77, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F77" s="20"/>
@@ -4617,17 +4396,14 @@
         <f aca="true">IF(J77="","",(INDIRECT("N" &amp; ROW() - 1) - N77))</f>
         <v/>
       </c>
-      <c r="H77" s="18" t="str">
-        <f aca="true">IF(J77 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H77" s="18"/>
       <c r="I77" s="18" t="str">
         <f aca="true">IF(J77 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K77" s="20" t="n">
-        <f aca="true">IF(J77 = "-", -INDIRECT("C" &amp; ROW() - 1),F77)</f>
-        <v>0</v>
+      <c r="K77" s="20" t="str">
+        <f aca="true">IF(J77 = "-", -INDIRECT("C" &amp; ROW() - 1),E77)</f>
+        <v/>
       </c>
       <c r="L77" s="17" t="n">
         <f aca="true">IF(J77="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K77))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K77)))),0)</f>
@@ -4661,7 +4437,7 @@
         <v/>
       </c>
       <c r="E78" s="19" t="str">
-        <f aca="false">IF(D78="-", "-", IF(D78="", "", F78*VLOOKUP(D78, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D78="-", "-", IF(D78="", "", INT(F78*VLOOKUP(D78, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F78" s="20"/>
@@ -4669,17 +4445,14 @@
         <f aca="true">IF(J78="","",(INDIRECT("N" &amp; ROW() - 1) - N78))</f>
         <v/>
       </c>
-      <c r="H78" s="18" t="str">
-        <f aca="true">IF(J78 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H78" s="18"/>
       <c r="I78" s="18" t="str">
         <f aca="true">IF(J78 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K78" s="20" t="n">
-        <f aca="true">IF(J78 = "-", -INDIRECT("C" &amp; ROW() - 1),F78)</f>
-        <v>0</v>
+      <c r="K78" s="20" t="str">
+        <f aca="true">IF(J78 = "-", -INDIRECT("C" &amp; ROW() - 1),E78)</f>
+        <v/>
       </c>
       <c r="L78" s="17" t="n">
         <f aca="true">IF(J78="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K78))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K78)))),0)</f>
@@ -4713,7 +4486,7 @@
         <v/>
       </c>
       <c r="E79" s="19" t="str">
-        <f aca="false">IF(D79="-", "-", IF(D79="", "", F79*VLOOKUP(D79, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D79="-", "-", IF(D79="", "", INT(F79*VLOOKUP(D79, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F79" s="20"/>
@@ -4721,17 +4494,14 @@
         <f aca="true">IF(J79="","",(INDIRECT("N" &amp; ROW() - 1) - N79))</f>
         <v/>
       </c>
-      <c r="H79" s="18" t="str">
-        <f aca="true">IF(J79 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H79" s="18"/>
       <c r="I79" s="18" t="str">
         <f aca="true">IF(J79 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K79" s="20" t="n">
-        <f aca="true">IF(J79 = "-", -INDIRECT("C" &amp; ROW() - 1),F79)</f>
-        <v>0</v>
+      <c r="K79" s="20" t="str">
+        <f aca="true">IF(J79 = "-", -INDIRECT("C" &amp; ROW() - 1),E79)</f>
+        <v/>
       </c>
       <c r="L79" s="17" t="n">
         <f aca="true">IF(J79="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K79))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K79)))),0)</f>
@@ -4765,7 +4535,7 @@
         <v/>
       </c>
       <c r="E80" s="19" t="str">
-        <f aca="false">IF(D80="-", "-", IF(D80="", "", F80*VLOOKUP(D80, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D80="-", "-", IF(D80="", "", INT(F80*VLOOKUP(D80, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F80" s="20"/>
@@ -4773,17 +4543,14 @@
         <f aca="true">IF(J80="","",(INDIRECT("N" &amp; ROW() - 1) - N80))</f>
         <v/>
       </c>
-      <c r="H80" s="18" t="str">
-        <f aca="true">IF(J80 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H80" s="18"/>
       <c r="I80" s="18" t="str">
         <f aca="true">IF(J80 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K80" s="20" t="n">
-        <f aca="true">IF(J80 = "-", -INDIRECT("C" &amp; ROW() - 1),F80)</f>
-        <v>0</v>
+      <c r="K80" s="20" t="str">
+        <f aca="true">IF(J80 = "-", -INDIRECT("C" &amp; ROW() - 1),E80)</f>
+        <v/>
       </c>
       <c r="L80" s="17" t="n">
         <f aca="true">IF(J80="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K80))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K80)))),0)</f>
@@ -4817,7 +4584,7 @@
         <v/>
       </c>
       <c r="E81" s="19" t="str">
-        <f aca="false">IF(D81="-", "-", IF(D81="", "", F81*VLOOKUP(D81, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D81="-", "-", IF(D81="", "", INT(F81*VLOOKUP(D81, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F81" s="20"/>
@@ -4825,17 +4592,14 @@
         <f aca="true">IF(J81="","",(INDIRECT("N" &amp; ROW() - 1) - N81))</f>
         <v/>
       </c>
-      <c r="H81" s="18" t="str">
-        <f aca="true">IF(J81 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H81" s="18"/>
       <c r="I81" s="18" t="str">
         <f aca="true">IF(J81 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K81" s="20" t="n">
-        <f aca="true">IF(J81 = "-", -INDIRECT("C" &amp; ROW() - 1),F81)</f>
-        <v>0</v>
+      <c r="K81" s="20" t="str">
+        <f aca="true">IF(J81 = "-", -INDIRECT("C" &amp; ROW() - 1),E81)</f>
+        <v/>
       </c>
       <c r="L81" s="17" t="n">
         <f aca="true">IF(J81="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K81))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K81)))),0)</f>
@@ -4869,7 +4633,7 @@
         <v/>
       </c>
       <c r="E82" s="19" t="str">
-        <f aca="false">IF(D82="-", "-", IF(D82="", "", F82*VLOOKUP(D82, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D82="-", "-", IF(D82="", "", INT(F82*VLOOKUP(D82, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F82" s="20"/>
@@ -4877,17 +4641,14 @@
         <f aca="true">IF(J82="","",(INDIRECT("N" &amp; ROW() - 1) - N82))</f>
         <v/>
       </c>
-      <c r="H82" s="18" t="str">
-        <f aca="true">IF(J82 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H82" s="18"/>
       <c r="I82" s="18" t="str">
         <f aca="true">IF(J82 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K82" s="20" t="n">
-        <f aca="true">IF(J82 = "-", -INDIRECT("C" &amp; ROW() - 1),F82)</f>
-        <v>0</v>
+      <c r="K82" s="20" t="str">
+        <f aca="true">IF(J82 = "-", -INDIRECT("C" &amp; ROW() - 1),E82)</f>
+        <v/>
       </c>
       <c r="L82" s="17" t="n">
         <f aca="true">IF(J82="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K82))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K82)))),0)</f>
@@ -4921,7 +4682,7 @@
         <v/>
       </c>
       <c r="E83" s="19" t="str">
-        <f aca="false">IF(D83="-", "-", IF(D83="", "", F83*VLOOKUP(D83, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D83="-", "-", IF(D83="", "", INT(F83*VLOOKUP(D83, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F83" s="20"/>
@@ -4929,17 +4690,14 @@
         <f aca="true">IF(J83="","",(INDIRECT("N" &amp; ROW() - 1) - N83))</f>
         <v/>
       </c>
-      <c r="H83" s="18" t="str">
-        <f aca="true">IF(J83 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H83" s="18"/>
       <c r="I83" s="18" t="str">
         <f aca="true">IF(J83 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K83" s="20" t="n">
-        <f aca="true">IF(J83 = "-", -INDIRECT("C" &amp; ROW() - 1),F83)</f>
-        <v>0</v>
+      <c r="K83" s="20" t="str">
+        <f aca="true">IF(J83 = "-", -INDIRECT("C" &amp; ROW() - 1),E83)</f>
+        <v/>
       </c>
       <c r="L83" s="17" t="n">
         <f aca="true">IF(J83="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K83))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K83)))),0)</f>
@@ -4973,7 +4731,7 @@
         <v/>
       </c>
       <c r="E84" s="19" t="str">
-        <f aca="false">IF(D84="-", "-", IF(D84="", "", F84*VLOOKUP(D84, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D84="-", "-", IF(D84="", "", INT(F84*VLOOKUP(D84, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F84" s="20"/>
@@ -4981,17 +4739,14 @@
         <f aca="true">IF(J84="","",(INDIRECT("N" &amp; ROW() - 1) - N84))</f>
         <v/>
       </c>
-      <c r="H84" s="18" t="str">
-        <f aca="true">IF(J84 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H84" s="18"/>
       <c r="I84" s="18" t="str">
         <f aca="true">IF(J84 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K84" s="20" t="n">
-        <f aca="true">IF(J84 = "-", -INDIRECT("C" &amp; ROW() - 1),F84)</f>
-        <v>0</v>
+      <c r="K84" s="20" t="str">
+        <f aca="true">IF(J84 = "-", -INDIRECT("C" &amp; ROW() - 1),E84)</f>
+        <v/>
       </c>
       <c r="L84" s="17" t="n">
         <f aca="true">IF(J84="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K84))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K84)))),0)</f>
@@ -5025,7 +4780,7 @@
         <v/>
       </c>
       <c r="E85" s="19" t="str">
-        <f aca="false">IF(D85="-", "-", IF(D85="", "", F85*VLOOKUP(D85, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D85="-", "-", IF(D85="", "", INT(F85*VLOOKUP(D85, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F85" s="20"/>
@@ -5033,17 +4788,14 @@
         <f aca="true">IF(J85="","",(INDIRECT("N" &amp; ROW() - 1) - N85))</f>
         <v/>
       </c>
-      <c r="H85" s="18" t="str">
-        <f aca="true">IF(J85 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H85" s="18"/>
       <c r="I85" s="18" t="str">
         <f aca="true">IF(J85 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K85" s="20" t="n">
-        <f aca="true">IF(J85 = "-", -INDIRECT("C" &amp; ROW() - 1),F85)</f>
-        <v>0</v>
+      <c r="K85" s="20" t="str">
+        <f aca="true">IF(J85 = "-", -INDIRECT("C" &amp; ROW() - 1),E85)</f>
+        <v/>
       </c>
       <c r="L85" s="17" t="n">
         <f aca="true">IF(J85="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K85))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K85)))),0)</f>
@@ -5077,7 +4829,7 @@
         <v/>
       </c>
       <c r="E86" s="19" t="str">
-        <f aca="false">IF(D86="-", "-", IF(D86="", "", F86*VLOOKUP(D86, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D86="-", "-", IF(D86="", "", INT(F86*VLOOKUP(D86, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F86" s="20"/>
@@ -5085,17 +4837,14 @@
         <f aca="true">IF(J86="","",(INDIRECT("N" &amp; ROW() - 1) - N86))</f>
         <v/>
       </c>
-      <c r="H86" s="18" t="str">
-        <f aca="true">IF(J86 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H86" s="18"/>
       <c r="I86" s="18" t="str">
         <f aca="true">IF(J86 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K86" s="20" t="n">
-        <f aca="true">IF(J86 = "-", -INDIRECT("C" &amp; ROW() - 1),F86)</f>
-        <v>0</v>
+      <c r="K86" s="20" t="str">
+        <f aca="true">IF(J86 = "-", -INDIRECT("C" &amp; ROW() - 1),E86)</f>
+        <v/>
       </c>
       <c r="L86" s="17" t="n">
         <f aca="true">IF(J86="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K86))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K86)))),0)</f>
@@ -5129,7 +4878,7 @@
         <v/>
       </c>
       <c r="E87" s="19" t="str">
-        <f aca="false">IF(D87="-", "-", IF(D87="", "", F87*VLOOKUP(D87, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D87="-", "-", IF(D87="", "", INT(F87*VLOOKUP(D87, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F87" s="20"/>
@@ -5137,17 +4886,14 @@
         <f aca="true">IF(J87="","",(INDIRECT("N" &amp; ROW() - 1) - N87))</f>
         <v/>
       </c>
-      <c r="H87" s="18" t="str">
-        <f aca="true">IF(J87 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H87" s="18"/>
       <c r="I87" s="18" t="str">
         <f aca="true">IF(J87 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K87" s="20" t="n">
-        <f aca="true">IF(J87 = "-", -INDIRECT("C" &amp; ROW() - 1),F87)</f>
-        <v>0</v>
+      <c r="K87" s="20" t="str">
+        <f aca="true">IF(J87 = "-", -INDIRECT("C" &amp; ROW() - 1),E87)</f>
+        <v/>
       </c>
       <c r="L87" s="17" t="n">
         <f aca="true">IF(J87="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K87))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K87)))),0)</f>
@@ -5181,7 +4927,7 @@
         <v/>
       </c>
       <c r="E88" s="19" t="str">
-        <f aca="false">IF(D88="-", "-", IF(D88="", "", F88*VLOOKUP(D88, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D88="-", "-", IF(D88="", "", INT(F88*VLOOKUP(D88, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F88" s="20"/>
@@ -5189,17 +4935,14 @@
         <f aca="true">IF(J88="","",(INDIRECT("N" &amp; ROW() - 1) - N88))</f>
         <v/>
       </c>
-      <c r="H88" s="18" t="str">
-        <f aca="true">IF(J88 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H88" s="18"/>
       <c r="I88" s="18" t="str">
         <f aca="true">IF(J88 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K88" s="20" t="n">
-        <f aca="true">IF(J88 = "-", -INDIRECT("C" &amp; ROW() - 1),F88)</f>
-        <v>0</v>
+      <c r="K88" s="20" t="str">
+        <f aca="true">IF(J88 = "-", -INDIRECT("C" &amp; ROW() - 1),E88)</f>
+        <v/>
       </c>
       <c r="L88" s="17" t="n">
         <f aca="true">IF(J88="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K88))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K88)))),0)</f>
@@ -5233,7 +4976,7 @@
         <v/>
       </c>
       <c r="E89" s="19" t="str">
-        <f aca="false">IF(D89="-", "-", IF(D89="", "", F89*VLOOKUP(D89, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D89="-", "-", IF(D89="", "", INT(F89*VLOOKUP(D89, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F89" s="20"/>
@@ -5241,17 +4984,14 @@
         <f aca="true">IF(J89="","",(INDIRECT("N" &amp; ROW() - 1) - N89))</f>
         <v/>
       </c>
-      <c r="H89" s="18" t="str">
-        <f aca="true">IF(J89 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H89" s="18"/>
       <c r="I89" s="18" t="str">
         <f aca="true">IF(J89 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K89" s="20" t="n">
-        <f aca="true">IF(J89 = "-", -INDIRECT("C" &amp; ROW() - 1),F89)</f>
-        <v>0</v>
+      <c r="K89" s="20" t="str">
+        <f aca="true">IF(J89 = "-", -INDIRECT("C" &amp; ROW() - 1),E89)</f>
+        <v/>
       </c>
       <c r="L89" s="17" t="n">
         <f aca="true">IF(J89="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K89))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K89)))),0)</f>
@@ -5285,7 +5025,7 @@
         <v/>
       </c>
       <c r="E90" s="19" t="str">
-        <f aca="false">IF(D90="-", "-", IF(D90="", "", F90*VLOOKUP(D90, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D90="-", "-", IF(D90="", "", INT(F90*VLOOKUP(D90, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F90" s="20"/>
@@ -5293,17 +5033,14 @@
         <f aca="true">IF(J90="","",(INDIRECT("N" &amp; ROW() - 1) - N90))</f>
         <v/>
       </c>
-      <c r="H90" s="18" t="str">
-        <f aca="true">IF(J90 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H90" s="18"/>
       <c r="I90" s="18" t="str">
         <f aca="true">IF(J90 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K90" s="20" t="n">
-        <f aca="true">IF(J90 = "-", -INDIRECT("C" &amp; ROW() - 1),F90)</f>
-        <v>0</v>
+      <c r="K90" s="20" t="str">
+        <f aca="true">IF(J90 = "-", -INDIRECT("C" &amp; ROW() - 1),E90)</f>
+        <v/>
       </c>
       <c r="L90" s="17" t="n">
         <f aca="true">IF(J90="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K90))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K90)))),0)</f>
@@ -5337,7 +5074,7 @@
         <v/>
       </c>
       <c r="E91" s="19" t="str">
-        <f aca="false">IF(D91="-", "-", IF(D91="", "", F91*VLOOKUP(D91, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D91="-", "-", IF(D91="", "", INT(F91*VLOOKUP(D91, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F91" s="20"/>
@@ -5345,17 +5082,14 @@
         <f aca="true">IF(J91="","",(INDIRECT("N" &amp; ROW() - 1) - N91))</f>
         <v/>
       </c>
-      <c r="H91" s="18" t="str">
-        <f aca="true">IF(J91 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H91" s="18"/>
       <c r="I91" s="18" t="str">
         <f aca="true">IF(J91 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K91" s="20" t="n">
-        <f aca="true">IF(J91 = "-", -INDIRECT("C" &amp; ROW() - 1),F91)</f>
-        <v>0</v>
+      <c r="K91" s="20" t="str">
+        <f aca="true">IF(J91 = "-", -INDIRECT("C" &amp; ROW() - 1),E91)</f>
+        <v/>
       </c>
       <c r="L91" s="17" t="n">
         <f aca="true">IF(J91="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K91))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K91)))),0)</f>
@@ -5389,7 +5123,7 @@
         <v/>
       </c>
       <c r="E92" s="19" t="str">
-        <f aca="false">IF(D92="-", "-", IF(D92="", "", F92*VLOOKUP(D92, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D92="-", "-", IF(D92="", "", INT(F92*VLOOKUP(D92, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F92" s="20"/>
@@ -5397,17 +5131,14 @@
         <f aca="true">IF(J92="","",(INDIRECT("N" &amp; ROW() - 1) - N92))</f>
         <v/>
       </c>
-      <c r="H92" s="18" t="str">
-        <f aca="true">IF(J92 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H92" s="18"/>
       <c r="I92" s="18" t="str">
         <f aca="true">IF(J92 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K92" s="20" t="n">
-        <f aca="true">IF(J92 = "-", -INDIRECT("C" &amp; ROW() - 1),F92)</f>
-        <v>0</v>
+      <c r="K92" s="20" t="str">
+        <f aca="true">IF(J92 = "-", -INDIRECT("C" &amp; ROW() - 1),E92)</f>
+        <v/>
       </c>
       <c r="L92" s="17" t="n">
         <f aca="true">IF(J92="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K92))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K92)))),0)</f>
@@ -5441,7 +5172,7 @@
         <v/>
       </c>
       <c r="E93" s="19" t="str">
-        <f aca="false">IF(D93="-", "-", IF(D93="", "", F93*VLOOKUP(D93, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D93="-", "-", IF(D93="", "", INT(F93*VLOOKUP(D93, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F93" s="20"/>
@@ -5449,17 +5180,14 @@
         <f aca="true">IF(J93="","",(INDIRECT("N" &amp; ROW() - 1) - N93))</f>
         <v/>
       </c>
-      <c r="H93" s="18" t="str">
-        <f aca="true">IF(J93 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H93" s="18"/>
       <c r="I93" s="18" t="str">
         <f aca="true">IF(J93 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K93" s="20" t="n">
-        <f aca="true">IF(J93 = "-", -INDIRECT("C" &amp; ROW() - 1),F93)</f>
-        <v>0</v>
+      <c r="K93" s="20" t="str">
+        <f aca="true">IF(J93 = "-", -INDIRECT("C" &amp; ROW() - 1),E93)</f>
+        <v/>
       </c>
       <c r="L93" s="17" t="n">
         <f aca="true">IF(J93="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K93))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K93)))),0)</f>
@@ -5493,7 +5221,7 @@
         <v/>
       </c>
       <c r="E94" s="19" t="str">
-        <f aca="false">IF(D94="-", "-", IF(D94="", "", F94*VLOOKUP(D94, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D94="-", "-", IF(D94="", "", INT(F94*VLOOKUP(D94, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F94" s="20"/>
@@ -5501,17 +5229,14 @@
         <f aca="true">IF(J94="","",(INDIRECT("N" &amp; ROW() - 1) - N94))</f>
         <v/>
       </c>
-      <c r="H94" s="18" t="str">
-        <f aca="true">IF(J94 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H94" s="18"/>
       <c r="I94" s="18" t="str">
         <f aca="true">IF(J94 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K94" s="20" t="n">
-        <f aca="true">IF(J94 = "-", -INDIRECT("C" &amp; ROW() - 1),F94)</f>
-        <v>0</v>
+      <c r="K94" s="20" t="str">
+        <f aca="true">IF(J94 = "-", -INDIRECT("C" &amp; ROW() - 1),E94)</f>
+        <v/>
       </c>
       <c r="L94" s="17" t="n">
         <f aca="true">IF(J94="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K94))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K94)))),0)</f>
@@ -5545,7 +5270,7 @@
         <v/>
       </c>
       <c r="E95" s="19" t="str">
-        <f aca="false">IF(D95="-", "-", IF(D95="", "", F95*VLOOKUP(D95, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D95="-", "-", IF(D95="", "", INT(F95*VLOOKUP(D95, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F95" s="20"/>
@@ -5553,17 +5278,14 @@
         <f aca="true">IF(J95="","",(INDIRECT("N" &amp; ROW() - 1) - N95))</f>
         <v/>
       </c>
-      <c r="H95" s="18" t="str">
-        <f aca="true">IF(J95 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H95" s="18"/>
       <c r="I95" s="18" t="str">
         <f aca="true">IF(J95 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K95" s="20" t="n">
-        <f aca="true">IF(J95 = "-", -INDIRECT("C" &amp; ROW() - 1),F95)</f>
-        <v>0</v>
+      <c r="K95" s="20" t="str">
+        <f aca="true">IF(J95 = "-", -INDIRECT("C" &amp; ROW() - 1),E95)</f>
+        <v/>
       </c>
       <c r="L95" s="17" t="n">
         <f aca="true">IF(J95="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K95))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K95)))),0)</f>
@@ -5597,7 +5319,7 @@
         <v/>
       </c>
       <c r="E96" s="19" t="str">
-        <f aca="false">IF(D96="-", "-", IF(D96="", "", F96*VLOOKUP(D96, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D96="-", "-", IF(D96="", "", INT(F96*VLOOKUP(D96, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F96" s="20"/>
@@ -5605,17 +5327,14 @@
         <f aca="true">IF(J96="","",(INDIRECT("N" &amp; ROW() - 1) - N96))</f>
         <v/>
       </c>
-      <c r="H96" s="18" t="str">
-        <f aca="true">IF(J96 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H96" s="18"/>
       <c r="I96" s="18" t="str">
         <f aca="true">IF(J96 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K96" s="20" t="n">
-        <f aca="true">IF(J96 = "-", -INDIRECT("C" &amp; ROW() - 1),F96)</f>
-        <v>0</v>
+      <c r="K96" s="20" t="str">
+        <f aca="true">IF(J96 = "-", -INDIRECT("C" &amp; ROW() - 1),E96)</f>
+        <v/>
       </c>
       <c r="L96" s="17" t="n">
         <f aca="true">IF(J96="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K96))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K96)))),0)</f>
@@ -5649,7 +5368,7 @@
         <v/>
       </c>
       <c r="E97" s="19" t="str">
-        <f aca="false">IF(D97="-", "-", IF(D97="", "", F97*VLOOKUP(D97, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D97="-", "-", IF(D97="", "", INT(F97*VLOOKUP(D97, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F97" s="20"/>
@@ -5657,17 +5376,14 @@
         <f aca="true">IF(J97="","",(INDIRECT("N" &amp; ROW() - 1) - N97))</f>
         <v/>
       </c>
-      <c r="H97" s="18" t="str">
-        <f aca="true">IF(J97 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H97" s="18"/>
       <c r="I97" s="18" t="str">
         <f aca="true">IF(J97 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K97" s="20" t="n">
-        <f aca="true">IF(J97 = "-", -INDIRECT("C" &amp; ROW() - 1),F97)</f>
-        <v>0</v>
+      <c r="K97" s="20" t="str">
+        <f aca="true">IF(J97 = "-", -INDIRECT("C" &amp; ROW() - 1),E97)</f>
+        <v/>
       </c>
       <c r="L97" s="17" t="n">
         <f aca="true">IF(J97="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K97))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K97)))),0)</f>
@@ -5701,7 +5417,7 @@
         <v/>
       </c>
       <c r="E98" s="19" t="str">
-        <f aca="false">IF(D98="-", "-", IF(D98="", "", F98*VLOOKUP(D98, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D98="-", "-", IF(D98="", "", INT(F98*VLOOKUP(D98, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F98" s="20"/>
@@ -5709,17 +5425,14 @@
         <f aca="true">IF(J98="","",(INDIRECT("N" &amp; ROW() - 1) - N98))</f>
         <v/>
       </c>
-      <c r="H98" s="18" t="str">
-        <f aca="true">IF(J98 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H98" s="18"/>
       <c r="I98" s="18" t="str">
         <f aca="true">IF(J98 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K98" s="20" t="n">
-        <f aca="true">IF(J98 = "-", -INDIRECT("C" &amp; ROW() - 1),F98)</f>
-        <v>0</v>
+      <c r="K98" s="20" t="str">
+        <f aca="true">IF(J98 = "-", -INDIRECT("C" &amp; ROW() - 1),E98)</f>
+        <v/>
       </c>
       <c r="L98" s="17" t="n">
         <f aca="true">IF(J98="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K98))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K98)))),0)</f>
@@ -5753,7 +5466,7 @@
         <v/>
       </c>
       <c r="E99" s="19" t="str">
-        <f aca="false">IF(D99="-", "-", IF(D99="", "", F99*VLOOKUP(D99, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D99="-", "-", IF(D99="", "", INT(F99*VLOOKUP(D99, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F99" s="20"/>
@@ -5761,17 +5474,14 @@
         <f aca="true">IF(J99="","",(INDIRECT("N" &amp; ROW() - 1) - N99))</f>
         <v/>
       </c>
-      <c r="H99" s="18" t="str">
-        <f aca="true">IF(J99 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H99" s="18"/>
       <c r="I99" s="18" t="str">
         <f aca="true">IF(J99 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K99" s="20" t="n">
-        <f aca="true">IF(J99 = "-", -INDIRECT("C" &amp; ROW() - 1),F99)</f>
-        <v>0</v>
+      <c r="K99" s="20" t="str">
+        <f aca="true">IF(J99 = "-", -INDIRECT("C" &amp; ROW() - 1),E99)</f>
+        <v/>
       </c>
       <c r="L99" s="17" t="n">
         <f aca="true">IF(J99="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K99))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K99)))),0)</f>
@@ -5805,7 +5515,7 @@
         <v/>
       </c>
       <c r="E100" s="19" t="str">
-        <f aca="false">IF(D100="-", "-", IF(D100="", "", F100*VLOOKUP(D100, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D100="-", "-", IF(D100="", "", INT(F100*VLOOKUP(D100, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F100" s="20"/>
@@ -5813,17 +5523,14 @@
         <f aca="true">IF(J100="","",(INDIRECT("N" &amp; ROW() - 1) - N100))</f>
         <v/>
       </c>
-      <c r="H100" s="18" t="str">
-        <f aca="true">IF(J100 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H100" s="18"/>
       <c r="I100" s="18" t="str">
         <f aca="true">IF(J100 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K100" s="20" t="n">
-        <f aca="true">IF(J100 = "-", -INDIRECT("C" &amp; ROW() - 1),F100)</f>
-        <v>0</v>
+      <c r="K100" s="20" t="str">
+        <f aca="true">IF(J100 = "-", -INDIRECT("C" &amp; ROW() - 1),E100)</f>
+        <v/>
       </c>
       <c r="L100" s="17" t="n">
         <f aca="true">IF(J100="-",SUM(INDIRECT(ADDRESS(2,COLUMN(K100))&amp;":"&amp;ADDRESS(ROW(),COLUMN(K100)))),0)</f>
@@ -5857,7 +5564,7 @@
         <v/>
       </c>
       <c r="E101" s="19" t="str">
-        <f aca="false">IF(D101="-", "-", IF(D101="", "", F101*VLOOKUP(D101, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D101="-", "-", IF(D101="", "", INT(F101*VLOOKUP(D101, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F101" s="20"/>
@@ -5865,17 +5572,14 @@
         <f aca="true">IF(J101="","",(INDIRECT("N" &amp; ROW() - 1) - N101))</f>
         <v/>
       </c>
-      <c r="H101" s="18" t="str">
-        <f aca="true">IF(J101 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H101" s="18"/>
       <c r="I101" s="18" t="str">
         <f aca="true">IF(J101 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K101" s="20" t="n">
-        <f aca="true">IF(J101 = "-", -INDIRECT("C" &amp; ROW() - 1),F101)</f>
-        <v>0</v>
+      <c r="K101" s="20" t="str">
+        <f aca="true">IF(J101 = "-", -INDIRECT("C" &amp; ROW() - 1),E101)</f>
+        <v/>
       </c>
       <c r="L101" s="17" t="n">
         <f aca="true">IF(J101 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K101)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K101)))), 0)</f>
@@ -5909,7 +5613,7 @@
         <v/>
       </c>
       <c r="E102" s="19" t="str">
-        <f aca="false">IF(D102="-", "-", IF(D102="", "", F102*VLOOKUP(D102, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D102="-", "-", IF(D102="", "", INT(F102*VLOOKUP(D102, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F102" s="20"/>
@@ -5917,17 +5621,14 @@
         <f aca="true">IF(J102="","",(INDIRECT("N" &amp; ROW() - 1) - N102))</f>
         <v/>
       </c>
-      <c r="H102" s="18" t="str">
-        <f aca="true">IF(J102 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H102" s="18"/>
       <c r="I102" s="18" t="str">
         <f aca="true">IF(J102 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K102" s="20" t="n">
-        <f aca="true">IF(J102 = "-", -INDIRECT("C" &amp; ROW() - 1),F102)</f>
-        <v>0</v>
+      <c r="K102" s="20" t="str">
+        <f aca="true">IF(J102 = "-", -INDIRECT("C" &amp; ROW() - 1),E102)</f>
+        <v/>
       </c>
       <c r="L102" s="17" t="n">
         <f aca="true">IF(J102 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K102)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K102)))), 0)</f>
@@ -5961,7 +5662,7 @@
         <v/>
       </c>
       <c r="E103" s="19" t="str">
-        <f aca="false">IF(D103="-", "-", IF(D103="", "", F103*VLOOKUP(D103, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D103="-", "-", IF(D103="", "", INT(F103*VLOOKUP(D103, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F103" s="20"/>
@@ -5969,17 +5670,14 @@
         <f aca="true">IF(J103="","",(INDIRECT("N" &amp; ROW() - 1) - N103))</f>
         <v/>
       </c>
-      <c r="H103" s="18" t="str">
-        <f aca="true">IF(J103 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H103" s="18"/>
       <c r="I103" s="18" t="str">
         <f aca="true">IF(J103 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K103" s="20" t="n">
-        <f aca="true">IF(J103 = "-", -INDIRECT("C" &amp; ROW() - 1),F103)</f>
-        <v>0</v>
+      <c r="K103" s="20" t="str">
+        <f aca="true">IF(J103 = "-", -INDIRECT("C" &amp; ROW() - 1),E103)</f>
+        <v/>
       </c>
       <c r="L103" s="17" t="n">
         <f aca="true">IF(J103 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K103)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K103)))), 0)</f>
@@ -6013,7 +5711,7 @@
         <v/>
       </c>
       <c r="E104" s="19" t="str">
-        <f aca="false">IF(D104="-", "-", IF(D104="", "", F104*VLOOKUP(D104, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D104="-", "-", IF(D104="", "", INT(F104*VLOOKUP(D104, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F104" s="20"/>
@@ -6021,17 +5719,14 @@
         <f aca="true">IF(J104="","",(INDIRECT("N" &amp; ROW() - 1) - N104))</f>
         <v/>
       </c>
-      <c r="H104" s="18" t="str">
-        <f aca="true">IF(J104 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H104" s="18"/>
       <c r="I104" s="18" t="str">
         <f aca="true">IF(J104 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K104" s="20" t="n">
-        <f aca="true">IF(J104 = "-", -INDIRECT("C" &amp; ROW() - 1),F104)</f>
-        <v>0</v>
+      <c r="K104" s="20" t="str">
+        <f aca="true">IF(J104 = "-", -INDIRECT("C" &amp; ROW() - 1),E104)</f>
+        <v/>
       </c>
       <c r="L104" s="17" t="n">
         <f aca="true">IF(J104 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K104)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K104)))), 0)</f>
@@ -6065,7 +5760,7 @@
         <v/>
       </c>
       <c r="E105" s="19" t="str">
-        <f aca="false">IF(D105="-", "-", IF(D105="", "", F105*VLOOKUP(D105, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D105="-", "-", IF(D105="", "", INT(F105*VLOOKUP(D105, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F105" s="20"/>
@@ -6073,17 +5768,14 @@
         <f aca="true">IF(J105="","",(INDIRECT("N" &amp; ROW() - 1) - N105))</f>
         <v/>
       </c>
-      <c r="H105" s="18" t="str">
-        <f aca="true">IF(J105 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H105" s="18"/>
       <c r="I105" s="18" t="str">
         <f aca="true">IF(J105 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K105" s="20" t="n">
-        <f aca="true">IF(J105 = "-", -INDIRECT("C" &amp; ROW() - 1),F105)</f>
-        <v>0</v>
+      <c r="K105" s="20" t="str">
+        <f aca="true">IF(J105 = "-", -INDIRECT("C" &amp; ROW() - 1),E105)</f>
+        <v/>
       </c>
       <c r="L105" s="17" t="n">
         <f aca="true">IF(J105 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K105)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K105)))), 0)</f>
@@ -6117,7 +5809,7 @@
         <v/>
       </c>
       <c r="E106" s="19" t="str">
-        <f aca="false">IF(D106="-", "-", IF(D106="", "", F106*VLOOKUP(D106, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D106="-", "-", IF(D106="", "", INT(F106*VLOOKUP(D106, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F106" s="20"/>
@@ -6125,17 +5817,14 @@
         <f aca="true">IF(J106="","",(INDIRECT("N" &amp; ROW() - 1) - N106))</f>
         <v/>
       </c>
-      <c r="H106" s="18" t="str">
-        <f aca="true">IF(J106 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H106" s="18"/>
       <c r="I106" s="18" t="str">
         <f aca="true">IF(J106 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K106" s="20" t="n">
-        <f aca="true">IF(J106 = "-", -INDIRECT("C" &amp; ROW() - 1),F106)</f>
-        <v>0</v>
+      <c r="K106" s="20" t="str">
+        <f aca="true">IF(J106 = "-", -INDIRECT("C" &amp; ROW() - 1),E106)</f>
+        <v/>
       </c>
       <c r="L106" s="17" t="n">
         <f aca="true">IF(J106 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K106)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K106)))), 0)</f>
@@ -6169,7 +5858,7 @@
         <v/>
       </c>
       <c r="E107" s="19" t="str">
-        <f aca="false">IF(D107="-", "-", IF(D107="", "", F107*VLOOKUP(D107, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D107="-", "-", IF(D107="", "", INT(F107*VLOOKUP(D107, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F107" s="20"/>
@@ -6177,17 +5866,14 @@
         <f aca="true">IF(J107="","",(INDIRECT("N" &amp; ROW() - 1) - N107))</f>
         <v/>
       </c>
-      <c r="H107" s="18" t="str">
-        <f aca="true">IF(J107 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H107" s="18"/>
       <c r="I107" s="18" t="str">
         <f aca="true">IF(J107 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K107" s="20" t="n">
-        <f aca="true">IF(J107 = "-", -INDIRECT("C" &amp; ROW() - 1),F107)</f>
-        <v>0</v>
+      <c r="K107" s="20" t="str">
+        <f aca="true">IF(J107 = "-", -INDIRECT("C" &amp; ROW() - 1),E107)</f>
+        <v/>
       </c>
       <c r="L107" s="17" t="n">
         <f aca="true">IF(J107 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K107)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K107)))), 0)</f>
@@ -6221,7 +5907,7 @@
         <v/>
       </c>
       <c r="E108" s="19" t="str">
-        <f aca="false">IF(D108="-", "-", IF(D108="", "", F108*VLOOKUP(D108, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D108="-", "-", IF(D108="", "", INT(F108*VLOOKUP(D108, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F108" s="20"/>
@@ -6229,17 +5915,14 @@
         <f aca="true">IF(J108="","",(INDIRECT("N" &amp; ROW() - 1) - N108))</f>
         <v/>
       </c>
-      <c r="H108" s="18" t="str">
-        <f aca="true">IF(J108 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H108" s="18"/>
       <c r="I108" s="18" t="str">
         <f aca="true">IF(J108 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K108" s="20" t="n">
-        <f aca="true">IF(J108 = "-", -INDIRECT("C" &amp; ROW() - 1),F108)</f>
-        <v>0</v>
+      <c r="K108" s="20" t="str">
+        <f aca="true">IF(J108 = "-", -INDIRECT("C" &amp; ROW() - 1),E108)</f>
+        <v/>
       </c>
       <c r="L108" s="17" t="n">
         <f aca="true">IF(J108 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K108)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K108)))), 0)</f>
@@ -6273,7 +5956,7 @@
         <v/>
       </c>
       <c r="E109" s="19" t="str">
-        <f aca="false">IF(D109="-", "-", IF(D109="", "", F109*VLOOKUP(D109, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D109="-", "-", IF(D109="", "", INT(F109*VLOOKUP(D109, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F109" s="20"/>
@@ -6281,17 +5964,14 @@
         <f aca="true">IF(J109="","",(INDIRECT("N" &amp; ROW() - 1) - N109))</f>
         <v/>
       </c>
-      <c r="H109" s="18" t="str">
-        <f aca="true">IF(J109 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H109" s="18"/>
       <c r="I109" s="18" t="str">
         <f aca="true">IF(J109 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K109" s="20" t="n">
-        <f aca="true">IF(J109 = "-", -INDIRECT("C" &amp; ROW() - 1),F109)</f>
-        <v>0</v>
+      <c r="K109" s="20" t="str">
+        <f aca="true">IF(J109 = "-", -INDIRECT("C" &amp; ROW() - 1),E109)</f>
+        <v/>
       </c>
       <c r="L109" s="17" t="n">
         <f aca="true">IF(J109 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K109)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K109)))), 0)</f>
@@ -6325,7 +6005,7 @@
         <v/>
       </c>
       <c r="E110" s="19" t="str">
-        <f aca="false">IF(D110="-", "-", IF(D110="", "", F110*VLOOKUP(D110, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D110="-", "-", IF(D110="", "", INT(F110*VLOOKUP(D110, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F110" s="20"/>
@@ -6333,17 +6013,14 @@
         <f aca="true">IF(J110="","",(INDIRECT("N" &amp; ROW() - 1) - N110))</f>
         <v/>
       </c>
-      <c r="H110" s="18" t="str">
-        <f aca="true">IF(J110 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H110" s="18"/>
       <c r="I110" s="18" t="str">
         <f aca="true">IF(J110 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K110" s="20" t="n">
-        <f aca="true">IF(J110 = "-", -INDIRECT("C" &amp; ROW() - 1),F110)</f>
-        <v>0</v>
+      <c r="K110" s="20" t="str">
+        <f aca="true">IF(J110 = "-", -INDIRECT("C" &amp; ROW() - 1),E110)</f>
+        <v/>
       </c>
       <c r="L110" s="17" t="n">
         <f aca="true">IF(J110 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K110)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K110)))), 0)</f>
@@ -6377,7 +6054,7 @@
         <v/>
       </c>
       <c r="E111" s="19" t="str">
-        <f aca="false">IF(D111="-", "-", IF(D111="", "", F111*VLOOKUP(D111, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D111="-", "-", IF(D111="", "", INT(F111*VLOOKUP(D111, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F111" s="20"/>
@@ -6385,17 +6062,14 @@
         <f aca="true">IF(J111="","",(INDIRECT("N" &amp; ROW() - 1) - N111))</f>
         <v/>
       </c>
-      <c r="H111" s="18" t="str">
-        <f aca="true">IF(J111 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H111" s="18"/>
       <c r="I111" s="18" t="str">
         <f aca="true">IF(J111 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K111" s="20" t="n">
-        <f aca="true">IF(J111 = "-", -INDIRECT("C" &amp; ROW() - 1),F111)</f>
-        <v>0</v>
+      <c r="K111" s="20" t="str">
+        <f aca="true">IF(J111 = "-", -INDIRECT("C" &amp; ROW() - 1),E111)</f>
+        <v/>
       </c>
       <c r="L111" s="17" t="n">
         <f aca="true">IF(J111 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K111)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K111)))), 0)</f>
@@ -6429,7 +6103,7 @@
         <v/>
       </c>
       <c r="E112" s="19" t="str">
-        <f aca="false">IF(D112="-", "-", IF(D112="", "", F112*VLOOKUP(D112, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D112="-", "-", IF(D112="", "", INT(F112*VLOOKUP(D112, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F112" s="20"/>
@@ -6437,17 +6111,14 @@
         <f aca="true">IF(J112="","",(INDIRECT("N" &amp; ROW() - 1) - N112))</f>
         <v/>
       </c>
-      <c r="H112" s="18" t="str">
-        <f aca="true">IF(J112 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H112" s="18"/>
       <c r="I112" s="18" t="str">
         <f aca="true">IF(J112 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K112" s="20" t="n">
-        <f aca="true">IF(J112 = "-", -INDIRECT("C" &amp; ROW() - 1),F112)</f>
-        <v>0</v>
+      <c r="K112" s="20" t="str">
+        <f aca="true">IF(J112 = "-", -INDIRECT("C" &amp; ROW() - 1),E112)</f>
+        <v/>
       </c>
       <c r="L112" s="17" t="n">
         <f aca="true">IF(J112 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K112)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K112)))), 0)</f>
@@ -6481,7 +6152,7 @@
         <v/>
       </c>
       <c r="E113" s="19" t="str">
-        <f aca="false">IF(D113="-", "-", IF(D113="", "", F113*VLOOKUP(D113, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D113="-", "-", IF(D113="", "", INT(F113*VLOOKUP(D113, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F113" s="20"/>
@@ -6489,17 +6160,14 @@
         <f aca="true">IF(J113="","",(INDIRECT("N" &amp; ROW() - 1) - N113))</f>
         <v/>
       </c>
-      <c r="H113" s="18" t="str">
-        <f aca="true">IF(J113 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H113" s="18"/>
       <c r="I113" s="18" t="str">
         <f aca="true">IF(J113 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K113" s="20" t="n">
-        <f aca="true">IF(J113 = "-", -INDIRECT("C" &amp; ROW() - 1),F113)</f>
-        <v>0</v>
+      <c r="K113" s="20" t="str">
+        <f aca="true">IF(J113 = "-", -INDIRECT("C" &amp; ROW() - 1),E113)</f>
+        <v/>
       </c>
       <c r="L113" s="17" t="n">
         <f aca="true">IF(J113 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K113)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K113)))), 0)</f>
@@ -6533,7 +6201,7 @@
         <v/>
       </c>
       <c r="E114" s="19" t="str">
-        <f aca="false">IF(D114="-", "-", IF(D114="", "", F114*VLOOKUP(D114, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D114="-", "-", IF(D114="", "", INT(F114*VLOOKUP(D114, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F114" s="20"/>
@@ -6541,17 +6209,14 @@
         <f aca="true">IF(J114="","",(INDIRECT("N" &amp; ROW() - 1) - N114))</f>
         <v/>
       </c>
-      <c r="H114" s="18" t="str">
-        <f aca="true">IF(J114 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H114" s="18"/>
       <c r="I114" s="18" t="str">
         <f aca="true">IF(J114 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K114" s="20" t="n">
-        <f aca="true">IF(J114 = "-", -INDIRECT("C" &amp; ROW() - 1),F114)</f>
-        <v>0</v>
+      <c r="K114" s="20" t="str">
+        <f aca="true">IF(J114 = "-", -INDIRECT("C" &amp; ROW() - 1),E114)</f>
+        <v/>
       </c>
       <c r="L114" s="17" t="n">
         <f aca="true">IF(J114 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K114)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K114)))), 0)</f>
@@ -6585,7 +6250,7 @@
         <v/>
       </c>
       <c r="E115" s="19" t="str">
-        <f aca="false">IF(D115="-", "-", IF(D115="", "", F115*VLOOKUP(D115, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D115="-", "-", IF(D115="", "", INT(F115*VLOOKUP(D115, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F115" s="20"/>
@@ -6593,17 +6258,14 @@
         <f aca="true">IF(J115="","",(INDIRECT("N" &amp; ROW() - 1) - N115))</f>
         <v/>
       </c>
-      <c r="H115" s="18" t="str">
-        <f aca="true">IF(J115 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H115" s="18"/>
       <c r="I115" s="18" t="str">
         <f aca="true">IF(J115 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K115" s="20" t="n">
-        <f aca="true">IF(J115 = "-", -INDIRECT("C" &amp; ROW() - 1),F115)</f>
-        <v>0</v>
+      <c r="K115" s="20" t="str">
+        <f aca="true">IF(J115 = "-", -INDIRECT("C" &amp; ROW() - 1),E115)</f>
+        <v/>
       </c>
       <c r="L115" s="17" t="n">
         <f aca="true">IF(J115 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K115)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K115)))), 0)</f>
@@ -6637,7 +6299,7 @@
         <v/>
       </c>
       <c r="E116" s="19" t="str">
-        <f aca="false">IF(D116="-", "-", IF(D116="", "", F116*VLOOKUP(D116, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D116="-", "-", IF(D116="", "", INT(F116*VLOOKUP(D116, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F116" s="20"/>
@@ -6645,17 +6307,14 @@
         <f aca="true">IF(J116="","",(INDIRECT("N" &amp; ROW() - 1) - N116))</f>
         <v/>
       </c>
-      <c r="H116" s="18" t="str">
-        <f aca="true">IF(J116 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H116" s="18"/>
       <c r="I116" s="18" t="str">
         <f aca="true">IF(J116 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K116" s="20" t="n">
-        <f aca="true">IF(J116 = "-", -INDIRECT("C" &amp; ROW() - 1),F116)</f>
-        <v>0</v>
+      <c r="K116" s="20" t="str">
+        <f aca="true">IF(J116 = "-", -INDIRECT("C" &amp; ROW() - 1),E116)</f>
+        <v/>
       </c>
       <c r="L116" s="17" t="n">
         <f aca="true">IF(J116 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K116)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K116)))), 0)</f>
@@ -6689,7 +6348,7 @@
         <v/>
       </c>
       <c r="E117" s="19" t="str">
-        <f aca="false">IF(D117="-", "-", IF(D117="", "", F117*VLOOKUP(D117, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D117="-", "-", IF(D117="", "", INT(F117*VLOOKUP(D117, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F117" s="20"/>
@@ -6697,17 +6356,14 @@
         <f aca="true">IF(J117="","",(INDIRECT("N" &amp; ROW() - 1) - N117))</f>
         <v/>
       </c>
-      <c r="H117" s="18" t="str">
-        <f aca="true">IF(J117 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H117" s="18"/>
       <c r="I117" s="18" t="str">
         <f aca="true">IF(J117 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K117" s="20" t="n">
-        <f aca="true">IF(J117 = "-", -INDIRECT("C" &amp; ROW() - 1),F117)</f>
-        <v>0</v>
+      <c r="K117" s="20" t="str">
+        <f aca="true">IF(J117 = "-", -INDIRECT("C" &amp; ROW() - 1),E117)</f>
+        <v/>
       </c>
       <c r="L117" s="17" t="n">
         <f aca="true">IF(J117 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K117)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K117)))), 0)</f>
@@ -6741,7 +6397,7 @@
         <v/>
       </c>
       <c r="E118" s="19" t="str">
-        <f aca="false">IF(D118="-", "-", IF(D118="", "", F118*VLOOKUP(D118, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D118="-", "-", IF(D118="", "", INT(F118*VLOOKUP(D118, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F118" s="20"/>
@@ -6749,17 +6405,14 @@
         <f aca="true">IF(J118="","",(INDIRECT("N" &amp; ROW() - 1) - N118))</f>
         <v/>
       </c>
-      <c r="H118" s="18" t="str">
-        <f aca="true">IF(J118 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H118" s="18"/>
       <c r="I118" s="18" t="str">
         <f aca="true">IF(J118 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K118" s="20" t="n">
-        <f aca="true">IF(J118 = "-", -INDIRECT("C" &amp; ROW() - 1),F118)</f>
-        <v>0</v>
+      <c r="K118" s="20" t="str">
+        <f aca="true">IF(J118 = "-", -INDIRECT("C" &amp; ROW() - 1),E118)</f>
+        <v/>
       </c>
       <c r="L118" s="17" t="n">
         <f aca="true">IF(J118 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K118)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K118)))), 0)</f>
@@ -6793,7 +6446,7 @@
         <v/>
       </c>
       <c r="E119" s="19" t="str">
-        <f aca="false">IF(D119="-", "-", IF(D119="", "", F119*VLOOKUP(D119, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D119="-", "-", IF(D119="", "", INT(F119*VLOOKUP(D119, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F119" s="20"/>
@@ -6801,17 +6454,14 @@
         <f aca="true">IF(J119="","",(INDIRECT("N" &amp; ROW() - 1) - N119))</f>
         <v/>
       </c>
-      <c r="H119" s="18" t="str">
-        <f aca="true">IF(J119 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H119" s="18"/>
       <c r="I119" s="18" t="str">
         <f aca="true">IF(J119 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K119" s="20" t="n">
-        <f aca="true">IF(J119 = "-", -INDIRECT("C" &amp; ROW() - 1),F119)</f>
-        <v>0</v>
+      <c r="K119" s="20" t="str">
+        <f aca="true">IF(J119 = "-", -INDIRECT("C" &amp; ROW() - 1),E119)</f>
+        <v/>
       </c>
       <c r="L119" s="17" t="n">
         <f aca="true">IF(J119 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K119)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K119)))), 0)</f>
@@ -6845,7 +6495,7 @@
         <v/>
       </c>
       <c r="E120" s="19" t="str">
-        <f aca="false">IF(D120="-", "-", IF(D120="", "", F120*VLOOKUP(D120, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D120="-", "-", IF(D120="", "", INT(F120*VLOOKUP(D120, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F120" s="20"/>
@@ -6853,17 +6503,14 @@
         <f aca="true">IF(J120="","",(INDIRECT("N" &amp; ROW() - 1) - N120))</f>
         <v/>
       </c>
-      <c r="H120" s="18" t="str">
-        <f aca="true">IF(J120 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H120" s="18"/>
       <c r="I120" s="18" t="str">
         <f aca="true">IF(J120 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K120" s="20" t="n">
-        <f aca="true">IF(J120 = "-", -INDIRECT("C" &amp; ROW() - 1),F120)</f>
-        <v>0</v>
+      <c r="K120" s="20" t="str">
+        <f aca="true">IF(J120 = "-", -INDIRECT("C" &amp; ROW() - 1),E120)</f>
+        <v/>
       </c>
       <c r="L120" s="17" t="n">
         <f aca="true">IF(J120 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K120)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K120)))), 0)</f>
@@ -6897,7 +6544,7 @@
         <v/>
       </c>
       <c r="E121" s="19" t="str">
-        <f aca="false">IF(D121="-", "-", IF(D121="", "", F121*VLOOKUP(D121, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D121="-", "-", IF(D121="", "", INT(F121*VLOOKUP(D121, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F121" s="20"/>
@@ -6905,17 +6552,14 @@
         <f aca="true">IF(J121="","",(INDIRECT("N" &amp; ROW() - 1) - N121))</f>
         <v/>
       </c>
-      <c r="H121" s="18" t="str">
-        <f aca="true">IF(J121 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H121" s="18"/>
       <c r="I121" s="18" t="str">
         <f aca="true">IF(J121 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K121" s="20" t="n">
-        <f aca="true">IF(J121 = "-", -INDIRECT("C" &amp; ROW() - 1),F121)</f>
-        <v>0</v>
+      <c r="K121" s="20" t="str">
+        <f aca="true">IF(J121 = "-", -INDIRECT("C" &amp; ROW() - 1),E121)</f>
+        <v/>
       </c>
       <c r="L121" s="17" t="n">
         <f aca="true">IF(J121 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K121)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K121)))), 0)</f>
@@ -6949,7 +6593,7 @@
         <v/>
       </c>
       <c r="E122" s="19" t="str">
-        <f aca="false">IF(D122="-", "-", IF(D122="", "", F122*VLOOKUP(D122, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D122="-", "-", IF(D122="", "", INT(F122*VLOOKUP(D122, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F122" s="20"/>
@@ -6957,17 +6601,14 @@
         <f aca="true">IF(J122="","",(INDIRECT("N" &amp; ROW() - 1) - N122))</f>
         <v/>
       </c>
-      <c r="H122" s="18" t="str">
-        <f aca="true">IF(J122 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H122" s="18"/>
       <c r="I122" s="18" t="str">
         <f aca="true">IF(J122 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K122" s="20" t="n">
-        <f aca="true">IF(J122 = "-", -INDIRECT("C" &amp; ROW() - 1),F122)</f>
-        <v>0</v>
+      <c r="K122" s="20" t="str">
+        <f aca="true">IF(J122 = "-", -INDIRECT("C" &amp; ROW() - 1),E122)</f>
+        <v/>
       </c>
       <c r="L122" s="17" t="n">
         <f aca="true">IF(J122 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K122)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K122)))), 0)</f>
@@ -7001,7 +6642,7 @@
         <v/>
       </c>
       <c r="E123" s="19" t="str">
-        <f aca="false">IF(D123="-", "-", IF(D123="", "", F123*VLOOKUP(D123, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D123="-", "-", IF(D123="", "", INT(F123*VLOOKUP(D123, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F123" s="20"/>
@@ -7009,17 +6650,14 @@
         <f aca="true">IF(J123="","",(INDIRECT("N" &amp; ROW() - 1) - N123))</f>
         <v/>
       </c>
-      <c r="H123" s="18" t="str">
-        <f aca="true">IF(J123 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
-        <v/>
-      </c>
+      <c r="H123" s="18"/>
       <c r="I123" s="18" t="str">
         <f aca="true">IF(J123 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="K123" s="20" t="n">
-        <f aca="true">IF(J123 = "-", -INDIRECT("C" &amp; ROW() - 1),F123)</f>
-        <v>0</v>
+      <c r="K123" s="20" t="str">
+        <f aca="true">IF(J123 = "-", -INDIRECT("C" &amp; ROW() - 1),E123)</f>
+        <v/>
       </c>
       <c r="L123" s="17" t="n">
         <f aca="true">IF(J123 = "-", SUM(INDIRECT(ADDRESS(2,COLUMN(K123)) &amp; ":" &amp; ADDRESS(ROW(),COLUMN(K123)))), 0)</f>
@@ -7053,7 +6691,7 @@
         <v/>
       </c>
       <c r="E124" s="19" t="str">
-        <f aca="false">IF(D124="-", "-", IF(D124="", "", F124*VLOOKUP(D124, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D124="-", "-", IF(D124="", "", INT(F124*VLOOKUP(D124, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F124" s="20"/>
@@ -7089,7 +6727,7 @@
         <v/>
       </c>
       <c r="E125" s="19" t="str">
-        <f aca="false">IF(D125="-", "-", IF(D125="", "", F125*VLOOKUP(D125, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D125="-", "-", IF(D125="", "", INT(F125*VLOOKUP(D125, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F125" s="20"/>
@@ -7125,7 +6763,7 @@
         <v/>
       </c>
       <c r="E126" s="19" t="str">
-        <f aca="false">IF(D126="-", "-", IF(D126="", "", F126*VLOOKUP(D126, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D126="-", "-", IF(D126="", "", INT(F126*VLOOKUP(D126, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F126" s="20"/>
@@ -7161,7 +6799,7 @@
         <v/>
       </c>
       <c r="E127" s="19" t="str">
-        <f aca="false">IF(D127="-", "-", IF(D127="", "", F127*VLOOKUP(D127, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D127="-", "-", IF(D127="", "", INT(F127*VLOOKUP(D127, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F127" s="20"/>
@@ -7197,7 +6835,7 @@
         <v/>
       </c>
       <c r="E128" s="19" t="str">
-        <f aca="false">IF(D128="-", "-", IF(D128="", "", F128*VLOOKUP(D128, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D128="-", "-", IF(D128="", "", INT(F128*VLOOKUP(D128, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F128" s="20"/>
@@ -7233,7 +6871,7 @@
         <v/>
       </c>
       <c r="E129" s="19" t="str">
-        <f aca="false">IF(D129="-", "-", IF(D129="", "", F129*VLOOKUP(D129, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D129="-", "-", IF(D129="", "", INT(F129*VLOOKUP(D129, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F129" s="20"/>
@@ -7269,7 +6907,7 @@
         <v/>
       </c>
       <c r="E130" s="19" t="str">
-        <f aca="false">IF(D130="-", "-", IF(D130="", "", F130*VLOOKUP(D130, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D130="-", "-", IF(D130="", "", INT(F130*VLOOKUP(D130, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F130" s="20"/>
@@ -7305,7 +6943,7 @@
         <v/>
       </c>
       <c r="E131" s="19" t="str">
-        <f aca="false">IF(D131="-", "-", IF(D131="", "", F131*VLOOKUP(D131, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D131="-", "-", IF(D131="", "", INT(F131*VLOOKUP(D131, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F131" s="20"/>
@@ -7341,7 +6979,7 @@
         <v/>
       </c>
       <c r="E132" s="19" t="str">
-        <f aca="false">IF(D132="-", "-", IF(D132="", "", F132*VLOOKUP(D132, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D132="-", "-", IF(D132="", "", INT(F132*VLOOKUP(D132, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F132" s="20"/>
@@ -7377,7 +7015,7 @@
         <v/>
       </c>
       <c r="E133" s="19" t="str">
-        <f aca="false">IF(D133="-", "-", IF(D133="", "", F133*VLOOKUP(D133, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D133="-", "-", IF(D133="", "", INT(F133*VLOOKUP(D133, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F133" s="20"/>
@@ -7413,7 +7051,7 @@
         <v/>
       </c>
       <c r="E134" s="19" t="str">
-        <f aca="false">IF(D134="-", "-", IF(D134="", "", F134*VLOOKUP(D134, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D134="-", "-", IF(D134="", "", INT(F134*VLOOKUP(D134, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F134" s="20"/>
@@ -7449,7 +7087,7 @@
         <v/>
       </c>
       <c r="E135" s="19" t="str">
-        <f aca="false">IF(D135="-", "-", IF(D135="", "", F135*VLOOKUP(D135, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D135="-", "-", IF(D135="", "", INT(F135*VLOOKUP(D135, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F135" s="20"/>
@@ -7485,7 +7123,7 @@
         <v/>
       </c>
       <c r="E136" s="19" t="str">
-        <f aca="false">IF(D136="-", "-", IF(D136="", "", F136*VLOOKUP(D136, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D136="-", "-", IF(D136="", "", INT(F136*VLOOKUP(D136, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F136" s="20"/>
@@ -7521,7 +7159,7 @@
         <v/>
       </c>
       <c r="E137" s="19" t="str">
-        <f aca="false">IF(D137="-", "-", IF(D137="", "", F137*VLOOKUP(D137, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D137="-", "-", IF(D137="", "", INT(F137*VLOOKUP(D137, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F137" s="20"/>
@@ -7557,7 +7195,7 @@
         <v/>
       </c>
       <c r="E138" s="19" t="str">
-        <f aca="false">IF(D138="-", "-", IF(D138="", "", F138*VLOOKUP(D138, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D138="-", "-", IF(D138="", "", INT(F138*VLOOKUP(D138, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F138" s="20"/>
@@ -7593,7 +7231,7 @@
         <v/>
       </c>
       <c r="E139" s="19" t="str">
-        <f aca="false">IF(D139="-", "-", IF(D139="", "", F139*VLOOKUP(D139, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D139="-", "-", IF(D139="", "", INT(F139*VLOOKUP(D139, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F139" s="20"/>
@@ -7629,7 +7267,7 @@
         <v/>
       </c>
       <c r="E140" s="19" t="str">
-        <f aca="false">IF(D140="-", "-", IF(D140="", "", F140*VLOOKUP(D140, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D140="-", "-", IF(D140="", "", INT(F140*VLOOKUP(D140, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F140" s="20"/>
@@ -7665,7 +7303,7 @@
         <v/>
       </c>
       <c r="E141" s="19" t="str">
-        <f aca="false">IF(D141="-", "-", IF(D141="", "", F141*VLOOKUP(D141, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D141="-", "-", IF(D141="", "", INT(F141*VLOOKUP(D141, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F141" s="20"/>
@@ -7701,7 +7339,7 @@
         <v/>
       </c>
       <c r="E142" s="19" t="str">
-        <f aca="false">IF(D142="-", "-", IF(D142="", "", F142*VLOOKUP(D142, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D142="-", "-", IF(D142="", "", INT(F142*VLOOKUP(D142, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F142" s="20"/>
@@ -7737,7 +7375,7 @@
         <v/>
       </c>
       <c r="E143" s="19" t="str">
-        <f aca="false">IF(D143="-", "-", IF(D143="", "", F143*VLOOKUP(D143, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D143="-", "-", IF(D143="", "", INT(F143*VLOOKUP(D143, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F143" s="20"/>
@@ -7773,7 +7411,7 @@
         <v/>
       </c>
       <c r="E144" s="19" t="str">
-        <f aca="false">IF(D144="-", "-", IF(D144="", "", F144*VLOOKUP(D144, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D144="-", "-", IF(D144="", "", INT(F144*VLOOKUP(D144, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F144" s="20"/>
@@ -7809,7 +7447,7 @@
         <v/>
       </c>
       <c r="E145" s="19" t="str">
-        <f aca="false">IF(D145="-", "-", IF(D145="", "", F145*VLOOKUP(D145, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D145="-", "-", IF(D145="", "", INT(F145*VLOOKUP(D145, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F145" s="20"/>
@@ -7845,7 +7483,7 @@
         <v/>
       </c>
       <c r="E146" s="19" t="str">
-        <f aca="false">IF(D146="-", "-", IF(D146="", "", F146*VLOOKUP(D146, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D146="-", "-", IF(D146="", "", INT(F146*VLOOKUP(D146, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F146" s="20"/>
@@ -7881,7 +7519,7 @@
         <v/>
       </c>
       <c r="E147" s="19" t="str">
-        <f aca="false">IF(D147="-", "-", IF(D147="", "", F147*VLOOKUP(D147, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D147="-", "-", IF(D147="", "", INT(F147*VLOOKUP(D147, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F147" s="20"/>
@@ -7917,7 +7555,7 @@
         <v/>
       </c>
       <c r="E148" s="19" t="str">
-        <f aca="false">IF(D148="-", "-", IF(D148="", "", F148*VLOOKUP(D148, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D148="-", "-", IF(D148="", "", INT(F148*VLOOKUP(D148, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F148" s="20"/>
@@ -7953,7 +7591,7 @@
         <v/>
       </c>
       <c r="E149" s="19" t="str">
-        <f aca="false">IF(D149="-", "-", IF(D149="", "", F149*VLOOKUP(D149, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D149="-", "-", IF(D149="", "", INT(F149*VLOOKUP(D149, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F149" s="20"/>
@@ -7989,7 +7627,7 @@
         <v/>
       </c>
       <c r="E150" s="19" t="str">
-        <f aca="false">IF(D150="-", "-", IF(D150="", "", F150*VLOOKUP(D150, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D150="-", "-", IF(D150="", "", INT(F150*VLOOKUP(D150, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F150" s="20"/>
@@ -8025,7 +7663,7 @@
         <v/>
       </c>
       <c r="E151" s="19" t="str">
-        <f aca="false">IF(D151="-", "-", IF(D151="", "", F151*VLOOKUP(D151, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D151="-", "-", IF(D151="", "", INT(F151*VLOOKUP(D151, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F151" s="20"/>
@@ -8061,7 +7699,7 @@
         <v/>
       </c>
       <c r="E152" s="19" t="str">
-        <f aca="false">IF(D152="-", "-", IF(D152="", "", F152*VLOOKUP(D152, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D152="-", "-", IF(D152="", "", INT(F152*VLOOKUP(D152, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F152" s="20"/>
@@ -8097,7 +7735,7 @@
         <v/>
       </c>
       <c r="E153" s="19" t="str">
-        <f aca="false">IF(D153="-", "-", IF(D153="", "", F153*VLOOKUP(D153, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D153="-", "-", IF(D153="", "", INT(F153*VLOOKUP(D153, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F153" s="20"/>
@@ -8133,7 +7771,7 @@
         <v/>
       </c>
       <c r="E154" s="19" t="str">
-        <f aca="false">IF(D154="-", "-", IF(D154="", "", F154*VLOOKUP(D154, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D154="-", "-", IF(D154="", "", INT(F154*VLOOKUP(D154, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F154" s="20"/>
@@ -8169,7 +7807,7 @@
         <v/>
       </c>
       <c r="E155" s="19" t="str">
-        <f aca="false">IF(D155="-", "-", IF(D155="", "", F155*VLOOKUP(D155, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D155="-", "-", IF(D155="", "", INT(F155*VLOOKUP(D155, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F155" s="20"/>
@@ -8205,7 +7843,7 @@
         <v/>
       </c>
       <c r="E156" s="19" t="str">
-        <f aca="false">IF(D156="-", "-", IF(D156="", "", F156*VLOOKUP(D156, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D156="-", "-", IF(D156="", "", INT(F156*VLOOKUP(D156, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F156" s="24"/>
@@ -8240,7 +7878,7 @@
         <v/>
       </c>
       <c r="E157" s="19" t="str">
-        <f aca="false">IF(D157="-", "-", IF(D157="", "", F157*VLOOKUP(D157, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D157="-", "-", IF(D157="", "", INT(F157*VLOOKUP(D157, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F157" s="24"/>
@@ -8275,7 +7913,7 @@
         <v/>
       </c>
       <c r="E158" s="19" t="str">
-        <f aca="false">IF(D158="-", "-", IF(D158="", "", F158*VLOOKUP(D158, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D158="-", "-", IF(D158="", "", INT(F158*VLOOKUP(D158, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F158" s="24"/>
@@ -8310,7 +7948,7 @@
         <v/>
       </c>
       <c r="E159" s="19" t="str">
-        <f aca="false">IF(D159="-", "-", IF(D159="", "", F159*VLOOKUP(D159, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D159="-", "-", IF(D159="", "", INT(F159*VLOOKUP(D159, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F159" s="24"/>
@@ -8345,7 +7983,7 @@
         <v/>
       </c>
       <c r="E160" s="19" t="str">
-        <f aca="false">IF(D160="-", "-", IF(D160="", "", F160*VLOOKUP(D160, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D160="-", "-", IF(D160="", "", INT(F160*VLOOKUP(D160, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F160" s="24"/>
@@ -8380,7 +8018,7 @@
         <v/>
       </c>
       <c r="E161" s="19" t="str">
-        <f aca="false">IF(D161="-", "-", IF(D161="", "", F161*VLOOKUP(D161, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D161="-", "-", IF(D161="", "", INT(F161*VLOOKUP(D161, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F161" s="24"/>
@@ -8415,7 +8053,7 @@
         <v/>
       </c>
       <c r="E162" s="19" t="str">
-        <f aca="false">IF(D162="-", "-", IF(D162="", "", F162*VLOOKUP(D162, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D162="-", "-", IF(D162="", "", INT(F162*VLOOKUP(D162, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F162" s="24"/>
@@ -8450,7 +8088,7 @@
         <v/>
       </c>
       <c r="E163" s="19" t="str">
-        <f aca="false">IF(D163="-", "-", IF(D163="", "", F163*VLOOKUP(D163, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D163="-", "-", IF(D163="", "", INT(F163*VLOOKUP(D163, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F163" s="24"/>
@@ -8485,7 +8123,7 @@
         <v/>
       </c>
       <c r="E164" s="19" t="str">
-        <f aca="false">IF(D164="-", "-", IF(D164="", "", F164*VLOOKUP(D164, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D164="-", "-", IF(D164="", "", INT(F164*VLOOKUP(D164, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F164" s="24"/>
@@ -8520,7 +8158,7 @@
         <v/>
       </c>
       <c r="E165" s="19" t="str">
-        <f aca="false">IF(D165="-", "-", IF(D165="", "", F165*VLOOKUP(D165, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D165="-", "-", IF(D165="", "", INT(F165*VLOOKUP(D165, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F165" s="24"/>
@@ -8555,7 +8193,7 @@
         <v/>
       </c>
       <c r="E166" s="19" t="str">
-        <f aca="false">IF(D166="-", "-", IF(D166="", "", F166*VLOOKUP(D166, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D166="-", "-", IF(D166="", "", INT(F166*VLOOKUP(D166, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F166" s="24"/>
@@ -8586,7 +8224,7 @@
         <v/>
       </c>
       <c r="E167" s="19" t="str">
-        <f aca="false">IF(D167="-", "-", IF(D167="", "", F167*VLOOKUP(D167, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D167="-", "-", IF(D167="", "", INT(F167*VLOOKUP(D167, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F167" s="24"/>
@@ -8617,7 +8255,7 @@
         <v/>
       </c>
       <c r="E168" s="19" t="str">
-        <f aca="false">IF(D168="-", "-", IF(D168="", "", F168*VLOOKUP(D168, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D168="-", "-", IF(D168="", "", INT(F168*VLOOKUP(D168, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F168" s="24"/>
@@ -8648,7 +8286,7 @@
         <v/>
       </c>
       <c r="E169" s="19" t="str">
-        <f aca="false">IF(D169="-", "-", IF(D169="", "", F169*VLOOKUP(D169, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D169="-", "-", IF(D169="", "", INT(F169*VLOOKUP(D169, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F169" s="24"/>
@@ -8679,7 +8317,7 @@
         <v/>
       </c>
       <c r="E170" s="19" t="str">
-        <f aca="false">IF(D170="-", "-", IF(D170="", "", F170*VLOOKUP(D170, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D170="-", "-", IF(D170="", "", INT(F170*VLOOKUP(D170, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F170" s="24"/>
@@ -8710,7 +8348,7 @@
         <v/>
       </c>
       <c r="E171" s="19" t="str">
-        <f aca="false">IF(D171="-", "-", IF(D171="", "", F171*VLOOKUP(D171, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D171="-", "-", IF(D171="", "", INT(F171*VLOOKUP(D171, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F171" s="24"/>
@@ -8741,7 +8379,7 @@
         <v/>
       </c>
       <c r="E172" s="19" t="str">
-        <f aca="false">IF(D172="-", "-", IF(D172="", "", F172*VLOOKUP(D172, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D172="-", "-", IF(D172="", "", INT(F172*VLOOKUP(D172, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F172" s="24"/>
@@ -8772,7 +8410,7 @@
         <v/>
       </c>
       <c r="E173" s="19" t="str">
-        <f aca="false">IF(D173="-", "-", IF(D173="", "", F173*VLOOKUP(D173, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D173="-", "-", IF(D173="", "", INT(F173*VLOOKUP(D173, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F173" s="24"/>
@@ -8803,7 +8441,7 @@
         <v/>
       </c>
       <c r="E174" s="19" t="str">
-        <f aca="false">IF(D174="-", "-", IF(D174="", "", F174*VLOOKUP(D174, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D174="-", "-", IF(D174="", "", INT(F174*VLOOKUP(D174, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F174" s="24"/>
@@ -8834,7 +8472,7 @@
         <v/>
       </c>
       <c r="E175" s="19" t="str">
-        <f aca="false">IF(D175="-", "-", IF(D175="", "", F175*VLOOKUP(D175, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D175="-", "-", IF(D175="", "", INT(F175*VLOOKUP(D175, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F175" s="24"/>
@@ -8865,7 +8503,7 @@
         <v/>
       </c>
       <c r="E176" s="19" t="str">
-        <f aca="false">IF(D176="-", "-", IF(D176="", "", F176*VLOOKUP(D176, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D176="-", "-", IF(D176="", "", INT(F176*VLOOKUP(D176, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F176" s="24"/>
@@ -8896,7 +8534,7 @@
         <v/>
       </c>
       <c r="E177" s="19" t="str">
-        <f aca="false">IF(D177="-", "-", IF(D177="", "", F177*VLOOKUP(D177, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D177="-", "-", IF(D177="", "", INT(F177*VLOOKUP(D177, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F177" s="24"/>
@@ -8927,7 +8565,7 @@
         <v/>
       </c>
       <c r="E178" s="19" t="str">
-        <f aca="false">IF(D178="-", "-", IF(D178="", "", F178*VLOOKUP(D178, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D178="-", "-", IF(D178="", "", INT(F178*VLOOKUP(D178, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F178" s="24"/>
@@ -8958,7 +8596,7 @@
         <v/>
       </c>
       <c r="E179" s="19" t="str">
-        <f aca="false">IF(D179="-", "-", IF(D179="", "", F179*VLOOKUP(D179, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0)))</f>
+        <f aca="false">IF(D179="-", "-", IF(D179="", "", INT(F179*VLOOKUP(D179, 'SKU Маскарпоне'!$A$1:$C$150, 3, 0))))</f>
         <v/>
       </c>
       <c r="F179" s="24"/>
@@ -12805,13 +12443,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -12906,34 +12544,34 @@
     <row r="1" s="29" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="28"/>
       <c r="B1" s="28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: dropdown list + schedule plan
</commit_message>
<xml_diff>
--- a/app/data/static/templates/constructor_mascarpone.xlsx
+++ b/app/data/static/templates/constructor_mascarpone.xlsx
@@ -148,12 +148,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0"/>
-    <numFmt numFmtId="168" formatCode="@"/>
+    <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="169" formatCode="@"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -280,7 +281,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -365,10 +366,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,19 +374,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -660,7 +657,7 @@
   <dimension ref="A1:AMJ335"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5597,7 +5594,7 @@
         <f aca="false">IF(D102="","",VLOOKUP(D102, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C102" s="21" t="str">
+      <c r="C102" s="17" t="str">
         <f aca="false">IF(D102="","",VLOOKUP(D102, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -5646,7 +5643,7 @@
         <f aca="false">IF(D103="","",VLOOKUP(D103, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C103" s="21" t="str">
+      <c r="C103" s="17" t="str">
         <f aca="false">IF(D103="","",VLOOKUP(D103, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -5695,7 +5692,7 @@
         <f aca="false">IF(D104="","",VLOOKUP(D104, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C104" s="21" t="str">
+      <c r="C104" s="17" t="str">
         <f aca="false">IF(D104="","",VLOOKUP(D104, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -5744,7 +5741,7 @@
         <f aca="false">IF(D105="","",VLOOKUP(D105, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C105" s="21" t="str">
+      <c r="C105" s="17" t="str">
         <f aca="false">IF(D105="","",VLOOKUP(D105, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -5793,7 +5790,7 @@
         <f aca="false">IF(D106="","",VLOOKUP(D106, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C106" s="21" t="str">
+      <c r="C106" s="17" t="str">
         <f aca="false">IF(D106="","",VLOOKUP(D106, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -5842,7 +5839,7 @@
         <f aca="false">IF(D107="","",VLOOKUP(D107, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C107" s="21" t="str">
+      <c r="C107" s="17" t="str">
         <f aca="false">IF(D107="","",VLOOKUP(D107, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -5891,7 +5888,7 @@
         <f aca="false">IF(D108="","",VLOOKUP(D108, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C108" s="21" t="str">
+      <c r="C108" s="17" t="str">
         <f aca="false">IF(D108="","",VLOOKUP(D108, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -5940,7 +5937,7 @@
         <f aca="false">IF(D109="","",VLOOKUP(D109, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C109" s="21" t="str">
+      <c r="C109" s="17" t="str">
         <f aca="false">IF(D109="","",VLOOKUP(D109, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -5989,7 +5986,7 @@
         <f aca="false">IF(D110="","",VLOOKUP(D110, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C110" s="21" t="str">
+      <c r="C110" s="17" t="str">
         <f aca="false">IF(D110="","",VLOOKUP(D110, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6038,7 +6035,7 @@
         <f aca="false">IF(D111="","",VLOOKUP(D111, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C111" s="21" t="str">
+      <c r="C111" s="17" t="str">
         <f aca="false">IF(D111="","",VLOOKUP(D111, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6087,7 +6084,7 @@
         <f aca="false">IF(D112="","",VLOOKUP(D112, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C112" s="21" t="str">
+      <c r="C112" s="17" t="str">
         <f aca="false">IF(D112="","",VLOOKUP(D112, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6136,7 +6133,7 @@
         <f aca="false">IF(D113="","",VLOOKUP(D113, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C113" s="21" t="str">
+      <c r="C113" s="17" t="str">
         <f aca="false">IF(D113="","",VLOOKUP(D113, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6185,7 +6182,7 @@
         <f aca="false">IF(D114="","",VLOOKUP(D114, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C114" s="21" t="str">
+      <c r="C114" s="17" t="str">
         <f aca="false">IF(D114="","",VLOOKUP(D114, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6234,7 +6231,7 @@
         <f aca="false">IF(D115="","",VLOOKUP(D115, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C115" s="21" t="str">
+      <c r="C115" s="17" t="str">
         <f aca="false">IF(D115="","",VLOOKUP(D115, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6283,7 +6280,7 @@
         <f aca="false">IF(D116="","",VLOOKUP(D116, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C116" s="21" t="str">
+      <c r="C116" s="17" t="str">
         <f aca="false">IF(D116="","",VLOOKUP(D116, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6332,7 +6329,7 @@
         <f aca="false">IF(D117="","",VLOOKUP(D117, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C117" s="21" t="str">
+      <c r="C117" s="17" t="str">
         <f aca="false">IF(D117="","",VLOOKUP(D117, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6377,11 +6374,11 @@
       <c r="AMJ117" s="0"/>
     </row>
     <row r="118" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="21" t="str">
+      <c r="B118" s="17" t="str">
         <f aca="false">IF(D118="","",VLOOKUP(D118, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C118" s="21" t="str">
+      <c r="C118" s="17" t="str">
         <f aca="false">IF(D118="","",VLOOKUP(D118, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6426,11 +6423,11 @@
       <c r="AMJ118" s="0"/>
     </row>
     <row r="119" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="21" t="str">
+      <c r="B119" s="17" t="str">
         <f aca="false">IF(D119="","",VLOOKUP(D119, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C119" s="21" t="str">
+      <c r="C119" s="17" t="str">
         <f aca="false">IF(D119="","",VLOOKUP(D119, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6475,11 +6472,11 @@
       <c r="AMJ119" s="0"/>
     </row>
     <row r="120" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="21" t="str">
+      <c r="B120" s="17" t="str">
         <f aca="false">IF(D120="","",VLOOKUP(D120, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C120" s="21" t="str">
+      <c r="C120" s="17" t="str">
         <f aca="false">IF(D120="","",VLOOKUP(D120, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6524,11 +6521,11 @@
       <c r="AMJ120" s="0"/>
     </row>
     <row r="121" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="21" t="str">
+      <c r="B121" s="17" t="str">
         <f aca="false">IF(D121="","",VLOOKUP(D121, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C121" s="21" t="str">
+      <c r="C121" s="17" t="str">
         <f aca="false">IF(D121="","",VLOOKUP(D121, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6573,11 +6570,11 @@
       <c r="AMJ121" s="0"/>
     </row>
     <row r="122" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="21" t="str">
+      <c r="B122" s="17" t="str">
         <f aca="false">IF(D122="","",VLOOKUP(D122, 'SKU Маскарпоне'!$A$1:$F$150, 6, 0))</f>
         <v/>
       </c>
-      <c r="C122" s="21" t="str">
+      <c r="C122" s="17" t="str">
         <f aca="false">IF(D122="","",VLOOKUP(D122, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6622,11 +6619,11 @@
       <c r="AMJ122" s="0"/>
     </row>
     <row r="123" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="21" t="str">
+      <c r="B123" s="17" t="str">
         <f aca="false">IF(D123="","",VLOOKUP(D123, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
-      <c r="C123" s="21" t="str">
+      <c r="C123" s="17" t="str">
         <f aca="false">IF(D123="","",VLOOKUP(D123, 'SKU Маскарпоне'!$A$1:$B$150, 2, 0))</f>
         <v/>
       </c>
@@ -6671,8 +6668,8 @@
       <c r="AMJ123" s="0"/>
     </row>
     <row r="124" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B124" s="21"/>
-      <c r="C124" s="21"/>
+      <c r="B124" s="17"/>
+      <c r="C124" s="17"/>
       <c r="E124" s="18"/>
       <c r="F124" s="19" t="str">
         <f aca="true">IF(I124="","",(INDIRECT("N" &amp; ROW() - 1) - M124))</f>
@@ -6698,8 +6695,8 @@
       <c r="AMJ124" s="0"/>
     </row>
     <row r="125" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="21"/>
-      <c r="C125" s="21"/>
+      <c r="B125" s="17"/>
+      <c r="C125" s="17"/>
       <c r="E125" s="18"/>
       <c r="F125" s="19" t="str">
         <f aca="true">IF(I125="","",(INDIRECT("N" &amp; ROW() - 1) - M125))</f>
@@ -6725,8 +6722,8 @@
       <c r="AMJ125" s="0"/>
     </row>
     <row r="126" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="21"/>
-      <c r="C126" s="21"/>
+      <c r="B126" s="17"/>
+      <c r="C126" s="17"/>
       <c r="E126" s="18"/>
       <c r="F126" s="19" t="str">
         <f aca="true">IF(I126="","",(INDIRECT("N" &amp; ROW() - 1) - M126))</f>
@@ -6752,8 +6749,8 @@
       <c r="AMJ126" s="0"/>
     </row>
     <row r="127" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="21"/>
-      <c r="C127" s="21"/>
+      <c r="B127" s="17"/>
+      <c r="C127" s="17"/>
       <c r="E127" s="18"/>
       <c r="F127" s="19" t="str">
         <f aca="true">IF(I127="","",(INDIRECT("N" &amp; ROW() - 1) - M127))</f>
@@ -6779,8 +6776,8 @@
       <c r="AMJ127" s="0"/>
     </row>
     <row r="128" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="21"/>
-      <c r="C128" s="21"/>
+      <c r="B128" s="17"/>
+      <c r="C128" s="17"/>
       <c r="E128" s="18"/>
       <c r="F128" s="19" t="str">
         <f aca="true">IF(I128="","",(INDIRECT("N" &amp; ROW() - 1) - M128))</f>
@@ -6806,8 +6803,8 @@
       <c r="AMJ128" s="0"/>
     </row>
     <row r="129" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B129" s="21"/>
-      <c r="C129" s="21"/>
+      <c r="B129" s="17"/>
+      <c r="C129" s="17"/>
       <c r="E129" s="18"/>
       <c r="F129" s="19" t="str">
         <f aca="true">IF(I129="","",(INDIRECT("N" &amp; ROW() - 1) - M129))</f>
@@ -6833,8 +6830,8 @@
       <c r="AMJ129" s="0"/>
     </row>
     <row r="130" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="21"/>
-      <c r="C130" s="21"/>
+      <c r="B130" s="17"/>
+      <c r="C130" s="17"/>
       <c r="E130" s="18"/>
       <c r="F130" s="19" t="str">
         <f aca="true">IF(I130="","",(INDIRECT("N" &amp; ROW() - 1) - M130))</f>
@@ -6860,8 +6857,8 @@
       <c r="AMJ130" s="0"/>
     </row>
     <row r="131" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="21"/>
-      <c r="C131" s="21"/>
+      <c r="B131" s="17"/>
+      <c r="C131" s="17"/>
       <c r="E131" s="18"/>
       <c r="F131" s="19" t="str">
         <f aca="true">IF(I131="","",(INDIRECT("N" &amp; ROW() - 1) - M131))</f>
@@ -6887,8 +6884,8 @@
       <c r="AMJ131" s="0"/>
     </row>
     <row r="132" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B132" s="21"/>
-      <c r="C132" s="21"/>
+      <c r="B132" s="17"/>
+      <c r="C132" s="17"/>
       <c r="E132" s="18"/>
       <c r="F132" s="19" t="str">
         <f aca="true">IF(I132="","",(INDIRECT("N" &amp; ROW() - 1) - M132))</f>
@@ -6914,8 +6911,8 @@
       <c r="AMJ132" s="0"/>
     </row>
     <row r="133" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B133" s="21"/>
-      <c r="C133" s="21"/>
+      <c r="B133" s="17"/>
+      <c r="C133" s="17"/>
       <c r="E133" s="18"/>
       <c r="F133" s="19" t="str">
         <f aca="true">IF(I133="","",(INDIRECT("N" &amp; ROW() - 1) - M133))</f>
@@ -6941,8 +6938,8 @@
       <c r="AMJ133" s="0"/>
     </row>
     <row r="134" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B134" s="21"/>
-      <c r="C134" s="21"/>
+      <c r="B134" s="17"/>
+      <c r="C134" s="17"/>
       <c r="E134" s="18"/>
       <c r="F134" s="19" t="str">
         <f aca="true">IF(I134="","",(INDIRECT("N" &amp; ROW() - 1) - M134))</f>
@@ -6968,8 +6965,8 @@
       <c r="AMJ134" s="0"/>
     </row>
     <row r="135" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="21"/>
-      <c r="C135" s="21"/>
+      <c r="B135" s="17"/>
+      <c r="C135" s="17"/>
       <c r="E135" s="18"/>
       <c r="F135" s="19" t="str">
         <f aca="true">IF(I135="","",(INDIRECT("N" &amp; ROW() - 1) - M135))</f>
@@ -6995,8 +6992,8 @@
       <c r="AMJ135" s="0"/>
     </row>
     <row r="136" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B136" s="21"/>
-      <c r="C136" s="21"/>
+      <c r="B136" s="17"/>
+      <c r="C136" s="17"/>
       <c r="E136" s="18"/>
       <c r="F136" s="19" t="str">
         <f aca="true">IF(I136="","",(INDIRECT("N" &amp; ROW() - 1) - M136))</f>
@@ -7022,8 +7019,8 @@
       <c r="AMJ136" s="0"/>
     </row>
     <row r="137" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B137" s="21"/>
-      <c r="C137" s="21"/>
+      <c r="B137" s="17"/>
+      <c r="C137" s="17"/>
       <c r="E137" s="18"/>
       <c r="F137" s="19" t="str">
         <f aca="true">IF(I137="","",(INDIRECT("N" &amp; ROW() - 1) - M137))</f>
@@ -7049,8 +7046,8 @@
       <c r="AMJ137" s="0"/>
     </row>
     <row r="138" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="21"/>
-      <c r="C138" s="21"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
       <c r="E138" s="18"/>
       <c r="F138" s="19" t="str">
         <f aca="true">IF(I138="","",(INDIRECT("N" &amp; ROW() - 1) - M138))</f>
@@ -7076,8 +7073,8 @@
       <c r="AMJ138" s="0"/>
     </row>
     <row r="139" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="21"/>
-      <c r="C139" s="21"/>
+      <c r="B139" s="17"/>
+      <c r="C139" s="17"/>
       <c r="E139" s="18"/>
       <c r="F139" s="19" t="str">
         <f aca="true">IF(I139="","",(INDIRECT("N" &amp; ROW() - 1) - M139))</f>
@@ -7103,8 +7100,8 @@
       <c r="AMJ139" s="0"/>
     </row>
     <row r="140" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="21"/>
-      <c r="C140" s="21"/>
+      <c r="B140" s="17"/>
+      <c r="C140" s="17"/>
       <c r="E140" s="18"/>
       <c r="F140" s="19" t="str">
         <f aca="true">IF(I140="","",(INDIRECT("N" &amp; ROW() - 1) - M140))</f>
@@ -7130,8 +7127,8 @@
       <c r="AMJ140" s="0"/>
     </row>
     <row r="141" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="21"/>
-      <c r="C141" s="21"/>
+      <c r="B141" s="17"/>
+      <c r="C141" s="17"/>
       <c r="E141" s="18"/>
       <c r="F141" s="19" t="str">
         <f aca="true">IF(I141="","",(INDIRECT("N" &amp; ROW() - 1) - M141))</f>
@@ -7157,8 +7154,8 @@
       <c r="AMJ141" s="0"/>
     </row>
     <row r="142" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="21"/>
-      <c r="C142" s="21"/>
+      <c r="B142" s="17"/>
+      <c r="C142" s="17"/>
       <c r="E142" s="18"/>
       <c r="F142" s="19" t="str">
         <f aca="true">IF(I142="","",(INDIRECT("N" &amp; ROW() - 1) - M142))</f>
@@ -7184,8 +7181,8 @@
       <c r="AMJ142" s="0"/>
     </row>
     <row r="143" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="21"/>
-      <c r="C143" s="21"/>
+      <c r="B143" s="17"/>
+      <c r="C143" s="17"/>
       <c r="E143" s="18"/>
       <c r="F143" s="19" t="str">
         <f aca="true">IF(I143="","",(INDIRECT("N" &amp; ROW() - 1) - M143))</f>
@@ -7211,8 +7208,8 @@
       <c r="AMJ143" s="0"/>
     </row>
     <row r="144" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B144" s="21"/>
-      <c r="C144" s="21"/>
+      <c r="B144" s="17"/>
+      <c r="C144" s="17"/>
       <c r="E144" s="18"/>
       <c r="F144" s="19" t="str">
         <f aca="true">IF(I144="","",(INDIRECT("N" &amp; ROW() - 1) - M144))</f>
@@ -7238,8 +7235,8 @@
       <c r="AMJ144" s="0"/>
     </row>
     <row r="145" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="21"/>
-      <c r="C145" s="21"/>
+      <c r="B145" s="17"/>
+      <c r="C145" s="17"/>
       <c r="E145" s="18"/>
       <c r="F145" s="19" t="str">
         <f aca="true">IF(I145="","",(INDIRECT("N" &amp; ROW() - 1) - M145))</f>
@@ -7265,8 +7262,8 @@
       <c r="AMJ145" s="0"/>
     </row>
     <row r="146" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="21"/>
-      <c r="C146" s="21"/>
+      <c r="B146" s="17"/>
+      <c r="C146" s="17"/>
       <c r="E146" s="18"/>
       <c r="F146" s="19" t="str">
         <f aca="true">IF(I146="","",(INDIRECT("N" &amp; ROW() - 1) - M146))</f>
@@ -7292,8 +7289,8 @@
       <c r="AMJ146" s="0"/>
     </row>
     <row r="147" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="21"/>
-      <c r="C147" s="21"/>
+      <c r="B147" s="17"/>
+      <c r="C147" s="17"/>
       <c r="E147" s="18"/>
       <c r="F147" s="19" t="str">
         <f aca="true">IF(I147="","",(INDIRECT("N" &amp; ROW() - 1) - M147))</f>
@@ -7319,8 +7316,8 @@
       <c r="AMJ147" s="0"/>
     </row>
     <row r="148" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="21"/>
-      <c r="C148" s="21"/>
+      <c r="B148" s="17"/>
+      <c r="C148" s="17"/>
       <c r="E148" s="18"/>
       <c r="F148" s="19" t="str">
         <f aca="true">IF(I148="","",(INDIRECT("N" &amp; ROW() - 1) - M148))</f>
@@ -7346,8 +7343,8 @@
       <c r="AMJ148" s="0"/>
     </row>
     <row r="149" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="21"/>
-      <c r="C149" s="21"/>
+      <c r="B149" s="17"/>
+      <c r="C149" s="17"/>
       <c r="E149" s="18"/>
       <c r="F149" s="19" t="str">
         <f aca="true">IF(I149="","",(INDIRECT("N" &amp; ROW() - 1) - M149))</f>
@@ -7373,8 +7370,8 @@
       <c r="AMJ149" s="0"/>
     </row>
     <row r="150" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="21"/>
-      <c r="C150" s="21"/>
+      <c r="B150" s="17"/>
+      <c r="C150" s="17"/>
       <c r="E150" s="18"/>
       <c r="F150" s="19" t="str">
         <f aca="true">IF(I150="","",(INDIRECT("N" &amp; ROW() - 1) - M150))</f>
@@ -7400,8 +7397,8 @@
       <c r="AMJ150" s="0"/>
     </row>
     <row r="151" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="21"/>
-      <c r="C151" s="21"/>
+      <c r="B151" s="17"/>
+      <c r="C151" s="17"/>
       <c r="E151" s="18"/>
       <c r="F151" s="19" t="str">
         <f aca="true">IF(I151="","",(INDIRECT("N" &amp; ROW() - 1) - M151))</f>
@@ -7427,8 +7424,8 @@
       <c r="AMJ151" s="0"/>
     </row>
     <row r="152" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="21"/>
-      <c r="C152" s="21"/>
+      <c r="B152" s="17"/>
+      <c r="C152" s="17"/>
       <c r="E152" s="18"/>
       <c r="F152" s="19" t="str">
         <f aca="true">IF(I152="","",(INDIRECT("N" &amp; ROW() - 1) - M152))</f>
@@ -7454,8 +7451,8 @@
       <c r="AMJ152" s="0"/>
     </row>
     <row r="153" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="21"/>
-      <c r="C153" s="21"/>
+      <c r="B153" s="17"/>
+      <c r="C153" s="17"/>
       <c r="E153" s="18"/>
       <c r="F153" s="19" t="str">
         <f aca="true">IF(I153="","",(INDIRECT("N" &amp; ROW() - 1) - M153))</f>
@@ -7481,8 +7478,8 @@
       <c r="AMJ153" s="0"/>
     </row>
     <row r="154" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B154" s="21"/>
-      <c r="C154" s="21"/>
+      <c r="B154" s="17"/>
+      <c r="C154" s="17"/>
       <c r="E154" s="18"/>
       <c r="F154" s="19" t="str">
         <f aca="true">IF(I154="","",(INDIRECT("N" &amp; ROW() - 1) - M154))</f>
@@ -7508,8 +7505,8 @@
       <c r="AMJ154" s="0"/>
     </row>
     <row r="155" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B155" s="21"/>
-      <c r="C155" s="21"/>
+      <c r="B155" s="17"/>
+      <c r="C155" s="17"/>
       <c r="E155" s="18"/>
       <c r="F155" s="19" t="str">
         <f aca="true">IF(I155="","",(INDIRECT("N" &amp; ROW() - 1) - M155))</f>
@@ -7535,2327 +7532,2327 @@
       <c r="AMJ155" s="0"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B156" s="21"/>
-      <c r="C156" s="21"/>
-      <c r="E156" s="22"/>
-      <c r="F156" s="23" t="str">
+      <c r="B156" s="17"/>
+      <c r="C156" s="17"/>
+      <c r="E156" s="21"/>
+      <c r="F156" s="22" t="str">
         <f aca="true">IF(I156="","",(INDIRECT("N" &amp; ROW() - 1) - M156))</f>
         <v/>
       </c>
-      <c r="G156" s="24" t="str">
+      <c r="G156" s="23" t="str">
         <f aca="true">IF(I156 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H156" s="24" t="str">
+      <c r="H156" s="23" t="str">
         <f aca="true">IF(I156 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q156" s="25" t="str">
+      <c r="Q156" s="24" t="str">
         <f aca="true">IF(P156 = "", "", P156 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R156" s="25" t="str">
+      <c r="R156" s="24" t="str">
         <f aca="true">IF(I156="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B157" s="21"/>
-      <c r="C157" s="21"/>
-      <c r="E157" s="22"/>
-      <c r="F157" s="23" t="str">
+      <c r="B157" s="17"/>
+      <c r="C157" s="17"/>
+      <c r="E157" s="21"/>
+      <c r="F157" s="22" t="str">
         <f aca="true">IF(I157="","",(INDIRECT("N" &amp; ROW() - 1) - M157))</f>
         <v/>
       </c>
-      <c r="G157" s="24" t="str">
+      <c r="G157" s="23" t="str">
         <f aca="true">IF(I157 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H157" s="24" t="str">
+      <c r="H157" s="23" t="str">
         <f aca="true">IF(I157 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q157" s="25" t="str">
+      <c r="Q157" s="24" t="str">
         <f aca="true">IF(P157 = "", "", P157 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R157" s="25" t="str">
+      <c r="R157" s="24" t="str">
         <f aca="true">IF(I157="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B158" s="21"/>
-      <c r="C158" s="21"/>
-      <c r="E158" s="22"/>
-      <c r="F158" s="23" t="str">
+      <c r="B158" s="17"/>
+      <c r="C158" s="17"/>
+      <c r="E158" s="21"/>
+      <c r="F158" s="22" t="str">
         <f aca="true">IF(I158="","",(INDIRECT("N" &amp; ROW() - 1) - M158))</f>
         <v/>
       </c>
-      <c r="G158" s="24" t="str">
+      <c r="G158" s="23" t="str">
         <f aca="true">IF(I158 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H158" s="24" t="str">
+      <c r="H158" s="23" t="str">
         <f aca="true">IF(I158 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q158" s="25" t="str">
+      <c r="Q158" s="24" t="str">
         <f aca="true">IF(P158 = "", "", P158 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R158" s="25" t="str">
+      <c r="R158" s="24" t="str">
         <f aca="true">IF(I158="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B159" s="21"/>
-      <c r="C159" s="21"/>
-      <c r="E159" s="22"/>
-      <c r="F159" s="23" t="str">
+      <c r="B159" s="17"/>
+      <c r="C159" s="17"/>
+      <c r="E159" s="21"/>
+      <c r="F159" s="22" t="str">
         <f aca="true">IF(I159="","",(INDIRECT("N" &amp; ROW() - 1) - M159))</f>
         <v/>
       </c>
-      <c r="G159" s="24" t="str">
+      <c r="G159" s="23" t="str">
         <f aca="true">IF(I159 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H159" s="24" t="str">
+      <c r="H159" s="23" t="str">
         <f aca="true">IF(I159 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q159" s="25" t="str">
+      <c r="Q159" s="24" t="str">
         <f aca="true">IF(P159 = "", "", P159 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R159" s="25" t="str">
+      <c r="R159" s="24" t="str">
         <f aca="true">IF(I159="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B160" s="21"/>
-      <c r="C160" s="21"/>
-      <c r="E160" s="22"/>
-      <c r="F160" s="23" t="str">
+      <c r="B160" s="17"/>
+      <c r="C160" s="17"/>
+      <c r="E160" s="21"/>
+      <c r="F160" s="22" t="str">
         <f aca="true">IF(I160="","",(INDIRECT("N" &amp; ROW() - 1) - M160))</f>
         <v/>
       </c>
-      <c r="G160" s="24" t="str">
+      <c r="G160" s="23" t="str">
         <f aca="true">IF(I160 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H160" s="24" t="str">
+      <c r="H160" s="23" t="str">
         <f aca="true">IF(I160 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q160" s="25" t="str">
+      <c r="Q160" s="24" t="str">
         <f aca="true">IF(P160 = "", "", P160 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R160" s="25" t="str">
+      <c r="R160" s="24" t="str">
         <f aca="true">IF(I160="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B161" s="21"/>
-      <c r="C161" s="21"/>
-      <c r="E161" s="22"/>
-      <c r="F161" s="23" t="str">
+      <c r="B161" s="17"/>
+      <c r="C161" s="17"/>
+      <c r="E161" s="21"/>
+      <c r="F161" s="22" t="str">
         <f aca="true">IF(I161="","",(INDIRECT("N" &amp; ROW() - 1) - M161))</f>
         <v/>
       </c>
-      <c r="G161" s="24" t="str">
+      <c r="G161" s="23" t="str">
         <f aca="true">IF(I161 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H161" s="24" t="str">
+      <c r="H161" s="23" t="str">
         <f aca="true">IF(I161 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q161" s="25" t="str">
+      <c r="Q161" s="24" t="str">
         <f aca="true">IF(P161 = "", "", P161 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R161" s="25" t="str">
+      <c r="R161" s="24" t="str">
         <f aca="true">IF(I161="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B162" s="21"/>
-      <c r="C162" s="21"/>
-      <c r="E162" s="22"/>
-      <c r="F162" s="23" t="str">
+      <c r="B162" s="17"/>
+      <c r="C162" s="17"/>
+      <c r="E162" s="21"/>
+      <c r="F162" s="22" t="str">
         <f aca="true">IF(I162="","",(INDIRECT("N" &amp; ROW() - 1) - M162))</f>
         <v/>
       </c>
-      <c r="G162" s="24" t="str">
+      <c r="G162" s="23" t="str">
         <f aca="true">IF(I162 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H162" s="24" t="str">
+      <c r="H162" s="23" t="str">
         <f aca="true">IF(I162 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q162" s="25" t="str">
+      <c r="Q162" s="24" t="str">
         <f aca="true">IF(P162 = "", "", P162 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R162" s="25" t="str">
+      <c r="R162" s="24" t="str">
         <f aca="true">IF(I162="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B163" s="21"/>
-      <c r="C163" s="21"/>
-      <c r="E163" s="22"/>
-      <c r="F163" s="23" t="str">
+      <c r="B163" s="17"/>
+      <c r="C163" s="17"/>
+      <c r="E163" s="21"/>
+      <c r="F163" s="22" t="str">
         <f aca="true">IF(I163="","",(INDIRECT("N" &amp; ROW() - 1) - M163))</f>
         <v/>
       </c>
-      <c r="G163" s="24" t="str">
+      <c r="G163" s="23" t="str">
         <f aca="true">IF(I163 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H163" s="24" t="str">
+      <c r="H163" s="23" t="str">
         <f aca="true">IF(I163 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q163" s="25" t="str">
+      <c r="Q163" s="24" t="str">
         <f aca="true">IF(P163 = "", "", P163 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R163" s="25" t="str">
+      <c r="R163" s="24" t="str">
         <f aca="true">IF(I163="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B164" s="21"/>
-      <c r="C164" s="21"/>
-      <c r="E164" s="22"/>
-      <c r="F164" s="23" t="str">
+      <c r="B164" s="17"/>
+      <c r="C164" s="17"/>
+      <c r="E164" s="21"/>
+      <c r="F164" s="22" t="str">
         <f aca="true">IF(I164="","",(INDIRECT("N" &amp; ROW() - 1) - M164))</f>
         <v/>
       </c>
-      <c r="G164" s="24" t="str">
+      <c r="G164" s="23" t="str">
         <f aca="true">IF(I164 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H164" s="24" t="str">
+      <c r="H164" s="23" t="str">
         <f aca="true">IF(I164 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q164" s="25" t="str">
+      <c r="Q164" s="24" t="str">
         <f aca="true">IF(P164 = "", "", P164 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R164" s="25" t="str">
+      <c r="R164" s="24" t="str">
         <f aca="true">IF(I164="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B165" s="21"/>
-      <c r="C165" s="21"/>
-      <c r="E165" s="22"/>
-      <c r="F165" s="23" t="str">
+      <c r="B165" s="17"/>
+      <c r="C165" s="17"/>
+      <c r="E165" s="21"/>
+      <c r="F165" s="22" t="str">
         <f aca="true">IF(I165="","",(INDIRECT("N" &amp; ROW() - 1) - M165))</f>
         <v/>
       </c>
-      <c r="G165" s="24" t="str">
+      <c r="G165" s="23" t="str">
         <f aca="true">IF(I165 = "-", INDIRECT("D" &amp; ROW() - 1) * 1890,"")</f>
         <v/>
       </c>
-      <c r="H165" s="24" t="str">
+      <c r="H165" s="23" t="str">
         <f aca="true">IF(I165 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q165" s="25" t="str">
+      <c r="Q165" s="24" t="str">
         <f aca="true">IF(P165 = "", "", P165 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R165" s="25" t="str">
+      <c r="R165" s="24" t="str">
         <f aca="true">IF(I165="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B166" s="21"/>
-      <c r="C166" s="21"/>
-      <c r="E166" s="22"/>
-      <c r="F166" s="23" t="str">
+      <c r="B166" s="17"/>
+      <c r="C166" s="17"/>
+      <c r="E166" s="21"/>
+      <c r="F166" s="22" t="str">
         <f aca="true">IF(I166="","",(INDIRECT("N" &amp; ROW() - 1) - M166))</f>
         <v/>
       </c>
-      <c r="H166" s="24" t="str">
+      <c r="H166" s="23" t="str">
         <f aca="true">IF(I166 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q166" s="25" t="str">
+      <c r="Q166" s="24" t="str">
         <f aca="true">IF(P166 = "", "", P166 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R166" s="25" t="str">
+      <c r="R166" s="24" t="str">
         <f aca="true">IF(I166="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B167" s="21"/>
-      <c r="C167" s="21"/>
-      <c r="E167" s="22"/>
-      <c r="F167" s="23" t="str">
+      <c r="B167" s="17"/>
+      <c r="C167" s="17"/>
+      <c r="E167" s="21"/>
+      <c r="F167" s="22" t="str">
         <f aca="true">IF(I167="","",(INDIRECT("N" &amp; ROW() - 1) - M167))</f>
         <v/>
       </c>
-      <c r="H167" s="24" t="str">
+      <c r="H167" s="23" t="str">
         <f aca="true">IF(I167 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q167" s="25" t="str">
+      <c r="Q167" s="24" t="str">
         <f aca="true">IF(P167 = "", "", P167 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R167" s="25" t="str">
+      <c r="R167" s="24" t="str">
         <f aca="true">IF(I167="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B168" s="21"/>
-      <c r="C168" s="21"/>
-      <c r="E168" s="22"/>
-      <c r="F168" s="23" t="str">
+      <c r="B168" s="17"/>
+      <c r="C168" s="17"/>
+      <c r="E168" s="21"/>
+      <c r="F168" s="22" t="str">
         <f aca="true">IF(I168="","",(INDIRECT("N" &amp; ROW() - 1) - M168))</f>
         <v/>
       </c>
-      <c r="H168" s="24" t="str">
+      <c r="H168" s="23" t="str">
         <f aca="true">IF(I168 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q168" s="25" t="str">
+      <c r="Q168" s="24" t="str">
         <f aca="true">IF(P168 = "", "", P168 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R168" s="25" t="str">
+      <c r="R168" s="24" t="str">
         <f aca="true">IF(I168="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B169" s="21"/>
-      <c r="C169" s="21"/>
-      <c r="E169" s="22"/>
-      <c r="F169" s="23" t="str">
+      <c r="B169" s="17"/>
+      <c r="C169" s="17"/>
+      <c r="E169" s="21"/>
+      <c r="F169" s="22" t="str">
         <f aca="true">IF(I169="","",(INDIRECT("N" &amp; ROW() - 1) - M169))</f>
         <v/>
       </c>
-      <c r="H169" s="24" t="str">
+      <c r="H169" s="23" t="str">
         <f aca="true">IF(I169 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q169" s="25" t="str">
+      <c r="Q169" s="24" t="str">
         <f aca="true">IF(P169 = "", "", P169 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R169" s="25" t="str">
+      <c r="R169" s="24" t="str">
         <f aca="true">IF(I169="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B170" s="21"/>
-      <c r="C170" s="21"/>
-      <c r="E170" s="22"/>
-      <c r="F170" s="23" t="str">
+      <c r="B170" s="17"/>
+      <c r="C170" s="17"/>
+      <c r="E170" s="21"/>
+      <c r="F170" s="22" t="str">
         <f aca="true">IF(I170="","",(INDIRECT("N" &amp; ROW() - 1) - M170))</f>
         <v/>
       </c>
-      <c r="H170" s="24" t="str">
+      <c r="H170" s="23" t="str">
         <f aca="true">IF(I170 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q170" s="25" t="str">
+      <c r="Q170" s="24" t="str">
         <f aca="true">IF(P170 = "", "", P170 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R170" s="25" t="str">
+      <c r="R170" s="24" t="str">
         <f aca="true">IF(I170="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B171" s="21"/>
-      <c r="C171" s="21"/>
-      <c r="E171" s="22"/>
-      <c r="F171" s="23" t="str">
+      <c r="B171" s="17"/>
+      <c r="C171" s="17"/>
+      <c r="E171" s="21"/>
+      <c r="F171" s="22" t="str">
         <f aca="true">IF(I171="","",(INDIRECT("N" &amp; ROW() - 1) - M171))</f>
         <v/>
       </c>
-      <c r="H171" s="24" t="str">
+      <c r="H171" s="23" t="str">
         <f aca="true">IF(I171 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q171" s="25" t="str">
+      <c r="Q171" s="24" t="str">
         <f aca="true">IF(P171 = "", "", P171 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R171" s="25" t="str">
+      <c r="R171" s="24" t="str">
         <f aca="true">IF(I171="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B172" s="21"/>
-      <c r="C172" s="21"/>
-      <c r="E172" s="22"/>
-      <c r="F172" s="23" t="str">
+      <c r="B172" s="17"/>
+      <c r="C172" s="17"/>
+      <c r="E172" s="21"/>
+      <c r="F172" s="22" t="str">
         <f aca="true">IF(I172="","",(INDIRECT("N" &amp; ROW() - 1) - M172))</f>
         <v/>
       </c>
-      <c r="H172" s="24" t="str">
+      <c r="H172" s="23" t="str">
         <f aca="true">IF(I172 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q172" s="25" t="str">
+      <c r="Q172" s="24" t="str">
         <f aca="true">IF(P172 = "", "", P172 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R172" s="25" t="str">
+      <c r="R172" s="24" t="str">
         <f aca="true">IF(I172="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B173" s="21"/>
-      <c r="C173" s="21"/>
-      <c r="E173" s="22"/>
-      <c r="F173" s="23" t="str">
+      <c r="B173" s="17"/>
+      <c r="C173" s="17"/>
+      <c r="E173" s="21"/>
+      <c r="F173" s="22" t="str">
         <f aca="true">IF(I173="","",(INDIRECT("N" &amp; ROW() - 1) - M173))</f>
         <v/>
       </c>
-      <c r="H173" s="24" t="str">
+      <c r="H173" s="23" t="str">
         <f aca="true">IF(I173 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q173" s="25" t="str">
+      <c r="Q173" s="24" t="str">
         <f aca="true">IF(P173 = "", "", P173 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R173" s="25" t="str">
+      <c r="R173" s="24" t="str">
         <f aca="true">IF(I173="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="21"/>
-      <c r="C174" s="21"/>
-      <c r="E174" s="22"/>
-      <c r="F174" s="23" t="str">
+      <c r="B174" s="17"/>
+      <c r="C174" s="17"/>
+      <c r="E174" s="21"/>
+      <c r="F174" s="22" t="str">
         <f aca="true">IF(I174="","",(INDIRECT("N" &amp; ROW() - 1) - M174))</f>
         <v/>
       </c>
-      <c r="H174" s="24" t="str">
+      <c r="H174" s="23" t="str">
         <f aca="true">IF(I174 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q174" s="25" t="str">
+      <c r="Q174" s="24" t="str">
         <f aca="true">IF(P174 = "", "", P174 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R174" s="25" t="str">
+      <c r="R174" s="24" t="str">
         <f aca="true">IF(I174="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="21"/>
-      <c r="C175" s="21"/>
-      <c r="E175" s="22"/>
-      <c r="F175" s="23" t="str">
+      <c r="B175" s="17"/>
+      <c r="C175" s="17"/>
+      <c r="E175" s="21"/>
+      <c r="F175" s="22" t="str">
         <f aca="true">IF(I175="","",(INDIRECT("N" &amp; ROW() - 1) - M175))</f>
         <v/>
       </c>
-      <c r="H175" s="24" t="str">
+      <c r="H175" s="23" t="str">
         <f aca="true">IF(I175 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q175" s="25" t="str">
+      <c r="Q175" s="24" t="str">
         <f aca="true">IF(P175 = "", "", P175 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R175" s="25" t="str">
+      <c r="R175" s="24" t="str">
         <f aca="true">IF(I175="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B176" s="21"/>
-      <c r="C176" s="21"/>
-      <c r="E176" s="22"/>
-      <c r="F176" s="23" t="str">
+      <c r="B176" s="17"/>
+      <c r="C176" s="17"/>
+      <c r="E176" s="21"/>
+      <c r="F176" s="22" t="str">
         <f aca="true">IF(I176="","",(INDIRECT("N" &amp; ROW() - 1) - M176))</f>
         <v/>
       </c>
-      <c r="H176" s="24" t="str">
+      <c r="H176" s="23" t="str">
         <f aca="true">IF(I176 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q176" s="25" t="str">
+      <c r="Q176" s="24" t="str">
         <f aca="true">IF(P176 = "", "", P176 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R176" s="25" t="str">
+      <c r="R176" s="24" t="str">
         <f aca="true">IF(I176="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B177" s="21"/>
-      <c r="C177" s="21"/>
-      <c r="E177" s="22"/>
-      <c r="F177" s="23" t="str">
+      <c r="B177" s="17"/>
+      <c r="C177" s="17"/>
+      <c r="E177" s="21"/>
+      <c r="F177" s="22" t="str">
         <f aca="true">IF(I177="","",(INDIRECT("N" &amp; ROW() - 1) - M177))</f>
         <v/>
       </c>
-      <c r="H177" s="24" t="str">
+      <c r="H177" s="23" t="str">
         <f aca="true">IF(I177 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q177" s="25" t="str">
+      <c r="Q177" s="24" t="str">
         <f aca="true">IF(P177 = "", "", P177 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R177" s="25" t="str">
+      <c r="R177" s="24" t="str">
         <f aca="true">IF(I177="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B178" s="21"/>
-      <c r="C178" s="21"/>
-      <c r="E178" s="22"/>
-      <c r="F178" s="23" t="str">
+      <c r="B178" s="17"/>
+      <c r="C178" s="17"/>
+      <c r="E178" s="21"/>
+      <c r="F178" s="22" t="str">
         <f aca="true">IF(I178="","",(INDIRECT("N" &amp; ROW() - 1) - M178))</f>
         <v/>
       </c>
-      <c r="H178" s="24" t="str">
+      <c r="H178" s="23" t="str">
         <f aca="true">IF(I178 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q178" s="25" t="str">
+      <c r="Q178" s="24" t="str">
         <f aca="true">IF(P178 = "", "", P178 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R178" s="25" t="str">
+      <c r="R178" s="24" t="str">
         <f aca="true">IF(I178="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B179" s="21"/>
-      <c r="C179" s="21"/>
-      <c r="E179" s="22"/>
-      <c r="F179" s="23" t="str">
+      <c r="B179" s="17"/>
+      <c r="C179" s="17"/>
+      <c r="E179" s="21"/>
+      <c r="F179" s="22" t="str">
         <f aca="true">IF(I179="","",(INDIRECT("N" &amp; ROW() - 1) - M179))</f>
         <v/>
       </c>
-      <c r="H179" s="24" t="str">
+      <c r="H179" s="23" t="str">
         <f aca="true">IF(I179 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q179" s="25" t="str">
+      <c r="Q179" s="24" t="str">
         <f aca="true">IF(P179 = "", "", P179 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R179" s="25" t="str">
+      <c r="R179" s="24" t="str">
         <f aca="true">IF(I179="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B180" s="21"/>
-      <c r="C180" s="21"/>
-      <c r="E180" s="22"/>
-      <c r="F180" s="23" t="str">
+      <c r="B180" s="17"/>
+      <c r="C180" s="17"/>
+      <c r="E180" s="21"/>
+      <c r="F180" s="22" t="str">
         <f aca="true">IF(I180="","",(INDIRECT("N" &amp; ROW() - 1) - M180))</f>
         <v/>
       </c>
-      <c r="H180" s="24" t="str">
+      <c r="H180" s="23" t="str">
         <f aca="true">IF(I180 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q180" s="25" t="str">
+      <c r="Q180" s="24" t="str">
         <f aca="true">IF(P180 = "", "", P180 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R180" s="25" t="str">
+      <c r="R180" s="24" t="str">
         <f aca="true">IF(I180="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B181" s="21"/>
-      <c r="C181" s="21"/>
-      <c r="E181" s="22"/>
-      <c r="F181" s="23" t="str">
+      <c r="B181" s="17"/>
+      <c r="C181" s="17"/>
+      <c r="E181" s="21"/>
+      <c r="F181" s="22" t="str">
         <f aca="true">IF(I181="","",(INDIRECT("N" &amp; ROW() - 1) - M181))</f>
         <v/>
       </c>
-      <c r="H181" s="24" t="str">
+      <c r="H181" s="23" t="str">
         <f aca="true">IF(I181 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q181" s="25" t="str">
+      <c r="Q181" s="24" t="str">
         <f aca="true">IF(P181 = "", "", P181 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R181" s="25" t="str">
+      <c r="R181" s="24" t="str">
         <f aca="true">IF(I181="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B182" s="21"/>
-      <c r="C182" s="21"/>
-      <c r="E182" s="22"/>
-      <c r="F182" s="23" t="str">
+      <c r="B182" s="17"/>
+      <c r="C182" s="17"/>
+      <c r="E182" s="21"/>
+      <c r="F182" s="22" t="str">
         <f aca="true">IF(I182="","",(INDIRECT("N" &amp; ROW() - 1) - M182))</f>
         <v/>
       </c>
-      <c r="H182" s="24" t="str">
+      <c r="H182" s="23" t="str">
         <f aca="true">IF(I182 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q182" s="25" t="str">
+      <c r="Q182" s="24" t="str">
         <f aca="true">IF(P182 = "", "", P182 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R182" s="25" t="str">
+      <c r="R182" s="24" t="str">
         <f aca="true">IF(I182="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B183" s="21"/>
-      <c r="C183" s="21"/>
-      <c r="E183" s="22"/>
-      <c r="F183" s="23" t="str">
+      <c r="B183" s="17"/>
+      <c r="C183" s="17"/>
+      <c r="E183" s="21"/>
+      <c r="F183" s="22" t="str">
         <f aca="true">IF(I183="","",(INDIRECT("N" &amp; ROW() - 1) - M183))</f>
         <v/>
       </c>
-      <c r="H183" s="24" t="str">
+      <c r="H183" s="23" t="str">
         <f aca="true">IF(I183 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q183" s="25" t="str">
+      <c r="Q183" s="24" t="str">
         <f aca="true">IF(P183 = "", "", P183 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R183" s="25" t="str">
+      <c r="R183" s="24" t="str">
         <f aca="true">IF(I183="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B184" s="21"/>
-      <c r="C184" s="21"/>
-      <c r="E184" s="22"/>
-      <c r="F184" s="23" t="str">
+      <c r="B184" s="17"/>
+      <c r="C184" s="17"/>
+      <c r="E184" s="21"/>
+      <c r="F184" s="22" t="str">
         <f aca="true">IF(I184="","",(INDIRECT("N" &amp; ROW() - 1) - M184))</f>
         <v/>
       </c>
-      <c r="H184" s="24" t="str">
+      <c r="H184" s="23" t="str">
         <f aca="true">IF(I184 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q184" s="25" t="str">
+      <c r="Q184" s="24" t="str">
         <f aca="true">IF(P184 = "", "", P184 / INDIRECT("D" &amp; ROW() - 1) )</f>
         <v/>
       </c>
-      <c r="R184" s="25" t="str">
+      <c r="R184" s="24" t="str">
         <f aca="true">IF(I184="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B185" s="21"/>
-      <c r="C185" s="21"/>
-      <c r="E185" s="22"/>
-      <c r="F185" s="23" t="str">
+      <c r="B185" s="17"/>
+      <c r="C185" s="17"/>
+      <c r="E185" s="21"/>
+      <c r="F185" s="22" t="str">
         <f aca="true">IF(I185="","",(INDIRECT("N" &amp; ROW() - 1) - M185))</f>
         <v/>
       </c>
-      <c r="H185" s="24" t="str">
+      <c r="H185" s="23" t="str">
         <f aca="true">IF(I185 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q185" s="25"/>
-      <c r="R185" s="25" t="str">
+      <c r="Q185" s="24"/>
+      <c r="R185" s="24" t="str">
         <f aca="true">IF(I185="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B186" s="21"/>
-      <c r="C186" s="21"/>
-      <c r="E186" s="22"/>
-      <c r="F186" s="23" t="str">
+      <c r="B186" s="17"/>
+      <c r="C186" s="17"/>
+      <c r="E186" s="21"/>
+      <c r="F186" s="22" t="str">
         <f aca="true">IF(I186="","",(INDIRECT("N" &amp; ROW() - 1) - M186))</f>
         <v/>
       </c>
-      <c r="H186" s="24" t="str">
+      <c r="H186" s="23" t="str">
         <f aca="true">IF(I186 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q186" s="25"/>
-      <c r="R186" s="25" t="str">
+      <c r="Q186" s="24"/>
+      <c r="R186" s="24" t="str">
         <f aca="true">IF(I186="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B187" s="21"/>
-      <c r="C187" s="21"/>
-      <c r="E187" s="22"/>
-      <c r="F187" s="23" t="str">
+      <c r="B187" s="17"/>
+      <c r="C187" s="17"/>
+      <c r="E187" s="21"/>
+      <c r="F187" s="22" t="str">
         <f aca="true">IF(I187="","",(INDIRECT("N" &amp; ROW() - 1) - M187))</f>
         <v/>
       </c>
-      <c r="H187" s="24" t="str">
+      <c r="H187" s="23" t="str">
         <f aca="true">IF(I187 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q187" s="25"/>
-      <c r="R187" s="25" t="str">
+      <c r="Q187" s="24"/>
+      <c r="R187" s="24" t="str">
         <f aca="true">IF(I187="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B188" s="21"/>
-      <c r="C188" s="21"/>
-      <c r="E188" s="22"/>
-      <c r="F188" s="23" t="str">
+      <c r="B188" s="17"/>
+      <c r="C188" s="17"/>
+      <c r="E188" s="21"/>
+      <c r="F188" s="22" t="str">
         <f aca="true">IF(I188="","",(INDIRECT("N" &amp; ROW() - 1) - M188))</f>
         <v/>
       </c>
-      <c r="H188" s="24" t="str">
+      <c r="H188" s="23" t="str">
         <f aca="true">IF(I188 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q188" s="25"/>
-      <c r="R188" s="25" t="str">
+      <c r="Q188" s="24"/>
+      <c r="R188" s="24" t="str">
         <f aca="true">IF(I188="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B189" s="21"/>
-      <c r="C189" s="21"/>
-      <c r="E189" s="22"/>
-      <c r="F189" s="23" t="str">
+      <c r="B189" s="17"/>
+      <c r="C189" s="17"/>
+      <c r="E189" s="21"/>
+      <c r="F189" s="22" t="str">
         <f aca="true">IF(I189="","",(INDIRECT("N" &amp; ROW() - 1) - M189))</f>
         <v/>
       </c>
-      <c r="H189" s="24" t="str">
+      <c r="H189" s="23" t="str">
         <f aca="true">IF(I189 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q189" s="25"/>
-      <c r="R189" s="25" t="str">
+      <c r="Q189" s="24"/>
+      <c r="R189" s="24" t="str">
         <f aca="true">IF(I189="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B190" s="21"/>
-      <c r="C190" s="21"/>
-      <c r="E190" s="22"/>
-      <c r="F190" s="23" t="str">
+      <c r="B190" s="17"/>
+      <c r="C190" s="17"/>
+      <c r="E190" s="21"/>
+      <c r="F190" s="22" t="str">
         <f aca="true">IF(I190="","",(INDIRECT("N" &amp; ROW() - 1) - M190))</f>
         <v/>
       </c>
-      <c r="H190" s="24" t="str">
+      <c r="H190" s="23" t="str">
         <f aca="true">IF(I190 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q190" s="25"/>
-      <c r="R190" s="25" t="str">
+      <c r="Q190" s="24"/>
+      <c r="R190" s="24" t="str">
         <f aca="true">IF(I190="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B191" s="21"/>
-      <c r="C191" s="21"/>
-      <c r="E191" s="22"/>
-      <c r="F191" s="23" t="str">
+      <c r="B191" s="17"/>
+      <c r="C191" s="17"/>
+      <c r="E191" s="21"/>
+      <c r="F191" s="22" t="str">
         <f aca="true">IF(I191="","",(INDIRECT("N" &amp; ROW() - 1) - M191))</f>
         <v/>
       </c>
-      <c r="H191" s="24" t="str">
+      <c r="H191" s="23" t="str">
         <f aca="true">IF(I191 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q191" s="25"/>
-      <c r="R191" s="25" t="str">
+      <c r="Q191" s="24"/>
+      <c r="R191" s="24" t="str">
         <f aca="true">IF(I191="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B192" s="21"/>
-      <c r="C192" s="21"/>
-      <c r="E192" s="22"/>
-      <c r="F192" s="23" t="str">
+      <c r="B192" s="17"/>
+      <c r="C192" s="17"/>
+      <c r="E192" s="21"/>
+      <c r="F192" s="22" t="str">
         <f aca="true">IF(I192="","",(INDIRECT("N" &amp; ROW() - 1) - M192))</f>
         <v/>
       </c>
-      <c r="H192" s="24" t="str">
+      <c r="H192" s="23" t="str">
         <f aca="true">IF(I192 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q192" s="25"/>
-      <c r="R192" s="25" t="str">
+      <c r="Q192" s="24"/>
+      <c r="R192" s="24" t="str">
         <f aca="true">IF(I192="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B193" s="21"/>
-      <c r="C193" s="21"/>
-      <c r="E193" s="22"/>
-      <c r="F193" s="23" t="str">
+      <c r="B193" s="17"/>
+      <c r="C193" s="17"/>
+      <c r="E193" s="21"/>
+      <c r="F193" s="22" t="str">
         <f aca="true">IF(I193="","",(INDIRECT("N" &amp; ROW() - 1) - M193))</f>
         <v/>
       </c>
-      <c r="H193" s="24" t="str">
+      <c r="H193" s="23" t="str">
         <f aca="true">IF(I193 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q193" s="25"/>
-      <c r="R193" s="25" t="str">
+      <c r="Q193" s="24"/>
+      <c r="R193" s="24" t="str">
         <f aca="true">IF(I193="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B194" s="21"/>
-      <c r="C194" s="21"/>
-      <c r="E194" s="22"/>
-      <c r="F194" s="23" t="str">
+      <c r="B194" s="17"/>
+      <c r="C194" s="17"/>
+      <c r="E194" s="21"/>
+      <c r="F194" s="22" t="str">
         <f aca="true">IF(I194="","",(INDIRECT("N" &amp; ROW() - 1) - M194))</f>
         <v/>
       </c>
-      <c r="H194" s="24" t="str">
+      <c r="H194" s="23" t="str">
         <f aca="true">IF(I194 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q194" s="25"/>
-      <c r="R194" s="25" t="str">
+      <c r="Q194" s="24"/>
+      <c r="R194" s="24" t="str">
         <f aca="true">IF(I194="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B195" s="21"/>
-      <c r="C195" s="21"/>
-      <c r="E195" s="22"/>
-      <c r="F195" s="23" t="str">
+      <c r="B195" s="17"/>
+      <c r="C195" s="17"/>
+      <c r="E195" s="21"/>
+      <c r="F195" s="22" t="str">
         <f aca="true">IF(I195="","",(INDIRECT("N" &amp; ROW() - 1) - M195))</f>
         <v/>
       </c>
-      <c r="H195" s="24" t="str">
+      <c r="H195" s="23" t="str">
         <f aca="true">IF(I195 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q195" s="25"/>
-      <c r="R195" s="25" t="str">
+      <c r="Q195" s="24"/>
+      <c r="R195" s="24" t="str">
         <f aca="true">IF(I195="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B196" s="21"/>
-      <c r="C196" s="21"/>
-      <c r="E196" s="22"/>
-      <c r="F196" s="23" t="str">
+      <c r="B196" s="17"/>
+      <c r="C196" s="17"/>
+      <c r="E196" s="21"/>
+      <c r="F196" s="22" t="str">
         <f aca="true">IF(I196="","",(INDIRECT("N" &amp; ROW() - 1) - M196))</f>
         <v/>
       </c>
-      <c r="H196" s="24" t="str">
+      <c r="H196" s="23" t="str">
         <f aca="true">IF(I196 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q196" s="25"/>
-      <c r="R196" s="25" t="str">
+      <c r="Q196" s="24"/>
+      <c r="R196" s="24" t="str">
         <f aca="true">IF(I196="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B197" s="21"/>
-      <c r="C197" s="21"/>
-      <c r="E197" s="22"/>
-      <c r="F197" s="23" t="str">
+      <c r="B197" s="17"/>
+      <c r="C197" s="17"/>
+      <c r="E197" s="21"/>
+      <c r="F197" s="22" t="str">
         <f aca="true">IF(I197="","",(INDIRECT("N" &amp; ROW() - 1) - M197))</f>
         <v/>
       </c>
-      <c r="H197" s="24" t="str">
+      <c r="H197" s="23" t="str">
         <f aca="true">IF(I197 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q197" s="25"/>
-      <c r="R197" s="25" t="str">
+      <c r="Q197" s="24"/>
+      <c r="R197" s="24" t="str">
         <f aca="true">IF(I197="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B198" s="21"/>
-      <c r="C198" s="21"/>
-      <c r="E198" s="22"/>
-      <c r="F198" s="22"/>
-      <c r="H198" s="24" t="str">
+      <c r="B198" s="17"/>
+      <c r="C198" s="17"/>
+      <c r="E198" s="21"/>
+      <c r="F198" s="21"/>
+      <c r="H198" s="23" t="str">
         <f aca="true">IF(I198 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q198" s="25"/>
-      <c r="R198" s="25" t="str">
+      <c r="Q198" s="24"/>
+      <c r="R198" s="24" t="str">
         <f aca="true">IF(I198="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B199" s="21"/>
-      <c r="C199" s="21"/>
-      <c r="E199" s="22"/>
-      <c r="F199" s="22"/>
-      <c r="H199" s="24" t="str">
+      <c r="B199" s="17"/>
+      <c r="C199" s="17"/>
+      <c r="E199" s="21"/>
+      <c r="F199" s="21"/>
+      <c r="H199" s="23" t="str">
         <f aca="true">IF(I199 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q199" s="25"/>
-      <c r="R199" s="25" t="str">
+      <c r="Q199" s="24"/>
+      <c r="R199" s="24" t="str">
         <f aca="true">IF(I199="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B200" s="21"/>
-      <c r="C200" s="21"/>
-      <c r="E200" s="22"/>
-      <c r="F200" s="22"/>
-      <c r="H200" s="24" t="str">
+      <c r="B200" s="17"/>
+      <c r="C200" s="17"/>
+      <c r="E200" s="21"/>
+      <c r="F200" s="21"/>
+      <c r="H200" s="23" t="str">
         <f aca="true">IF(I200 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q200" s="25"/>
-      <c r="R200" s="25" t="str">
+      <c r="Q200" s="24"/>
+      <c r="R200" s="24" t="str">
         <f aca="true">IF(I200="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B201" s="21"/>
-      <c r="C201" s="21"/>
-      <c r="E201" s="22"/>
-      <c r="F201" s="22"/>
-      <c r="H201" s="24" t="str">
+      <c r="B201" s="17"/>
+      <c r="C201" s="17"/>
+      <c r="E201" s="21"/>
+      <c r="F201" s="21"/>
+      <c r="H201" s="23" t="str">
         <f aca="true">IF(I201 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q201" s="25"/>
-      <c r="R201" s="25" t="str">
+      <c r="Q201" s="24"/>
+      <c r="R201" s="24" t="str">
         <f aca="true">IF(I201="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B202" s="21"/>
-      <c r="C202" s="21"/>
-      <c r="E202" s="22"/>
-      <c r="F202" s="22"/>
-      <c r="H202" s="24" t="str">
+      <c r="B202" s="17"/>
+      <c r="C202" s="17"/>
+      <c r="E202" s="21"/>
+      <c r="F202" s="21"/>
+      <c r="H202" s="23" t="str">
         <f aca="true">IF(I202 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q202" s="25"/>
-      <c r="R202" s="25" t="str">
+      <c r="Q202" s="24"/>
+      <c r="R202" s="24" t="str">
         <f aca="true">IF(I202="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B203" s="21"/>
-      <c r="C203" s="21"/>
-      <c r="E203" s="22"/>
-      <c r="F203" s="22"/>
-      <c r="H203" s="24" t="str">
+      <c r="B203" s="17"/>
+      <c r="C203" s="17"/>
+      <c r="E203" s="21"/>
+      <c r="F203" s="21"/>
+      <c r="H203" s="23" t="str">
         <f aca="true">IF(I203 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q203" s="25"/>
-      <c r="R203" s="25" t="str">
+      <c r="Q203" s="24"/>
+      <c r="R203" s="24" t="str">
         <f aca="true">IF(I203="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B204" s="21"/>
-      <c r="C204" s="21"/>
-      <c r="E204" s="22"/>
-      <c r="F204" s="22"/>
-      <c r="H204" s="24" t="str">
+      <c r="B204" s="17"/>
+      <c r="C204" s="17"/>
+      <c r="E204" s="21"/>
+      <c r="F204" s="21"/>
+      <c r="H204" s="23" t="str">
         <f aca="true">IF(I204 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q204" s="25"/>
-      <c r="R204" s="25" t="str">
+      <c r="Q204" s="24"/>
+      <c r="R204" s="24" t="str">
         <f aca="true">IF(I204="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B205" s="21"/>
-      <c r="C205" s="21"/>
-      <c r="E205" s="22"/>
-      <c r="F205" s="22"/>
-      <c r="H205" s="24" t="str">
+      <c r="B205" s="17"/>
+      <c r="C205" s="17"/>
+      <c r="E205" s="21"/>
+      <c r="F205" s="21"/>
+      <c r="H205" s="23" t="str">
         <f aca="true">IF(I205 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q205" s="25"/>
-      <c r="R205" s="25" t="str">
+      <c r="Q205" s="24"/>
+      <c r="R205" s="24" t="str">
         <f aca="true">IF(I205="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B206" s="21"/>
-      <c r="C206" s="21"/>
-      <c r="E206" s="22"/>
-      <c r="F206" s="22"/>
-      <c r="H206" s="24" t="str">
+      <c r="B206" s="17"/>
+      <c r="C206" s="17"/>
+      <c r="E206" s="21"/>
+      <c r="F206" s="21"/>
+      <c r="H206" s="23" t="str">
         <f aca="true">IF(I206 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q206" s="25"/>
-      <c r="R206" s="25" t="str">
+      <c r="Q206" s="24"/>
+      <c r="R206" s="24" t="str">
         <f aca="true">IF(I206="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B207" s="21"/>
-      <c r="C207" s="21"/>
-      <c r="E207" s="22"/>
-      <c r="F207" s="22"/>
-      <c r="H207" s="24" t="str">
+      <c r="B207" s="17"/>
+      <c r="C207" s="17"/>
+      <c r="E207" s="21"/>
+      <c r="F207" s="21"/>
+      <c r="H207" s="23" t="str">
         <f aca="true">IF(I207 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q207" s="25"/>
-      <c r="R207" s="25" t="str">
+      <c r="Q207" s="24"/>
+      <c r="R207" s="24" t="str">
         <f aca="true">IF(I207="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B208" s="21"/>
-      <c r="C208" s="21"/>
-      <c r="E208" s="22"/>
-      <c r="F208" s="22"/>
-      <c r="H208" s="24" t="str">
+      <c r="B208" s="17"/>
+      <c r="C208" s="17"/>
+      <c r="E208" s="21"/>
+      <c r="F208" s="21"/>
+      <c r="H208" s="23" t="str">
         <f aca="true">IF(I208 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q208" s="25"/>
-      <c r="R208" s="25" t="str">
+      <c r="Q208" s="24"/>
+      <c r="R208" s="24" t="str">
         <f aca="true">IF(I208="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B209" s="21"/>
-      <c r="C209" s="21"/>
-      <c r="E209" s="22"/>
-      <c r="F209" s="22"/>
-      <c r="H209" s="24" t="str">
+      <c r="B209" s="17"/>
+      <c r="C209" s="17"/>
+      <c r="E209" s="21"/>
+      <c r="F209" s="21"/>
+      <c r="H209" s="23" t="str">
         <f aca="true">IF(I209 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q209" s="25"/>
-      <c r="R209" s="25" t="str">
+      <c r="Q209" s="24"/>
+      <c r="R209" s="24" t="str">
         <f aca="true">IF(I209="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B210" s="21"/>
-      <c r="C210" s="21"/>
-      <c r="E210" s="22"/>
-      <c r="H210" s="24" t="str">
+      <c r="B210" s="17"/>
+      <c r="C210" s="17"/>
+      <c r="E210" s="21"/>
+      <c r="H210" s="23" t="str">
         <f aca="true">IF(I210 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q210" s="25"/>
-      <c r="R210" s="25" t="str">
+      <c r="Q210" s="24"/>
+      <c r="R210" s="24" t="str">
         <f aca="true">IF(I210="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B211" s="21"/>
-      <c r="C211" s="21"/>
-      <c r="E211" s="22"/>
-      <c r="H211" s="24" t="str">
+      <c r="B211" s="17"/>
+      <c r="C211" s="17"/>
+      <c r="E211" s="21"/>
+      <c r="H211" s="23" t="str">
         <f aca="true">IF(I211 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q211" s="25"/>
-      <c r="R211" s="25" t="str">
+      <c r="Q211" s="24"/>
+      <c r="R211" s="24" t="str">
         <f aca="true">IF(I211="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B212" s="21"/>
-      <c r="C212" s="21"/>
-      <c r="E212" s="22"/>
-      <c r="H212" s="24" t="str">
+      <c r="B212" s="17"/>
+      <c r="C212" s="17"/>
+      <c r="E212" s="21"/>
+      <c r="H212" s="23" t="str">
         <f aca="true">IF(I212 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q212" s="25"/>
-      <c r="R212" s="25" t="str">
+      <c r="Q212" s="24"/>
+      <c r="R212" s="24" t="str">
         <f aca="true">IF(I212="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B213" s="21"/>
-      <c r="C213" s="21"/>
-      <c r="E213" s="22"/>
-      <c r="H213" s="24" t="str">
+      <c r="B213" s="17"/>
+      <c r="C213" s="17"/>
+      <c r="E213" s="21"/>
+      <c r="H213" s="23" t="str">
         <f aca="true">IF(I213 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q213" s="25"/>
-      <c r="R213" s="25" t="str">
+      <c r="Q213" s="24"/>
+      <c r="R213" s="24" t="str">
         <f aca="true">IF(I213="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
-      <c r="E214" s="22"/>
-      <c r="H214" s="24" t="str">
+      <c r="B214" s="17"/>
+      <c r="C214" s="17"/>
+      <c r="E214" s="21"/>
+      <c r="H214" s="23" t="str">
         <f aca="true">IF(I214 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q214" s="25"/>
-      <c r="R214" s="25" t="str">
+      <c r="Q214" s="24"/>
+      <c r="R214" s="24" t="str">
         <f aca="true">IF(I214="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B215" s="21"/>
-      <c r="C215" s="21"/>
-      <c r="E215" s="22"/>
-      <c r="H215" s="24" t="str">
+      <c r="B215" s="17"/>
+      <c r="C215" s="17"/>
+      <c r="E215" s="21"/>
+      <c r="H215" s="23" t="str">
         <f aca="true">IF(I215 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q215" s="25"/>
-      <c r="R215" s="25" t="str">
+      <c r="Q215" s="24"/>
+      <c r="R215" s="24" t="str">
         <f aca="true">IF(I215="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B216" s="21"/>
-      <c r="C216" s="21"/>
-      <c r="E216" s="22"/>
-      <c r="H216" s="24" t="str">
+      <c r="B216" s="17"/>
+      <c r="C216" s="17"/>
+      <c r="E216" s="21"/>
+      <c r="H216" s="23" t="str">
         <f aca="true">IF(I216 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q216" s="25"/>
-      <c r="R216" s="25" t="str">
+      <c r="Q216" s="24"/>
+      <c r="R216" s="24" t="str">
         <f aca="true">IF(I216="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B217" s="21"/>
-      <c r="C217" s="21"/>
-      <c r="E217" s="22"/>
-      <c r="H217" s="24" t="str">
+      <c r="B217" s="17"/>
+      <c r="C217" s="17"/>
+      <c r="E217" s="21"/>
+      <c r="H217" s="23" t="str">
         <f aca="true">IF(I217 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q217" s="25"/>
-      <c r="R217" s="25" t="str">
+      <c r="Q217" s="24"/>
+      <c r="R217" s="24" t="str">
         <f aca="true">IF(I217="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B218" s="21"/>
-      <c r="C218" s="21"/>
-      <c r="E218" s="22"/>
-      <c r="H218" s="24" t="str">
+      <c r="B218" s="17"/>
+      <c r="C218" s="17"/>
+      <c r="E218" s="21"/>
+      <c r="H218" s="23" t="str">
         <f aca="true">IF(I218 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q218" s="25"/>
-      <c r="R218" s="25" t="str">
+      <c r="Q218" s="24"/>
+      <c r="R218" s="24" t="str">
         <f aca="true">IF(I218="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B219" s="21"/>
-      <c r="C219" s="21"/>
-      <c r="E219" s="22"/>
-      <c r="H219" s="24" t="str">
+      <c r="B219" s="17"/>
+      <c r="C219" s="17"/>
+      <c r="E219" s="21"/>
+      <c r="H219" s="23" t="str">
         <f aca="true">IF(I219 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q219" s="25"/>
-      <c r="R219" s="25" t="str">
+      <c r="Q219" s="24"/>
+      <c r="R219" s="24" t="str">
         <f aca="true">IF(I219="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B220" s="21"/>
-      <c r="C220" s="21"/>
-      <c r="E220" s="22"/>
-      <c r="H220" s="24" t="str">
+      <c r="B220" s="17"/>
+      <c r="C220" s="17"/>
+      <c r="E220" s="21"/>
+      <c r="H220" s="23" t="str">
         <f aca="true">IF(I220 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q220" s="25"/>
-      <c r="R220" s="25" t="str">
+      <c r="Q220" s="24"/>
+      <c r="R220" s="24" t="str">
         <f aca="true">IF(I220="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B221" s="21"/>
-      <c r="C221" s="21"/>
-      <c r="E221" s="22"/>
-      <c r="H221" s="24" t="str">
+      <c r="B221" s="17"/>
+      <c r="C221" s="17"/>
+      <c r="E221" s="21"/>
+      <c r="H221" s="23" t="str">
         <f aca="true">IF(I221 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q221" s="25"/>
-      <c r="R221" s="25" t="str">
+      <c r="Q221" s="24"/>
+      <c r="R221" s="24" t="str">
         <f aca="true">IF(I221="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B222" s="21"/>
-      <c r="C222" s="21"/>
-      <c r="E222" s="22"/>
-      <c r="H222" s="24" t="str">
+      <c r="B222" s="17"/>
+      <c r="C222" s="17"/>
+      <c r="E222" s="21"/>
+      <c r="H222" s="23" t="str">
         <f aca="true">IF(I222 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q222" s="25"/>
-      <c r="R222" s="25" t="str">
+      <c r="Q222" s="24"/>
+      <c r="R222" s="24" t="str">
         <f aca="true">IF(I222="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B223" s="21"/>
-      <c r="C223" s="21"/>
-      <c r="E223" s="22"/>
-      <c r="H223" s="24" t="str">
+      <c r="B223" s="17"/>
+      <c r="C223" s="17"/>
+      <c r="E223" s="21"/>
+      <c r="H223" s="23" t="str">
         <f aca="true">IF(I223 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q223" s="25"/>
-      <c r="R223" s="25" t="str">
+      <c r="Q223" s="24"/>
+      <c r="R223" s="24" t="str">
         <f aca="true">IF(I223="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B224" s="21"/>
-      <c r="C224" s="21"/>
-      <c r="E224" s="22"/>
-      <c r="H224" s="24" t="str">
+      <c r="B224" s="17"/>
+      <c r="C224" s="17"/>
+      <c r="E224" s="21"/>
+      <c r="H224" s="23" t="str">
         <f aca="true">IF(I224 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q224" s="25"/>
-      <c r="R224" s="25" t="str">
+      <c r="Q224" s="24"/>
+      <c r="R224" s="24" t="str">
         <f aca="true">IF(I224="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B225" s="21"/>
-      <c r="C225" s="21"/>
-      <c r="E225" s="22"/>
-      <c r="H225" s="24" t="str">
+      <c r="B225" s="17"/>
+      <c r="C225" s="17"/>
+      <c r="E225" s="21"/>
+      <c r="H225" s="23" t="str">
         <f aca="true">IF(I225 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q225" s="25"/>
-      <c r="R225" s="25" t="str">
+      <c r="Q225" s="24"/>
+      <c r="R225" s="24" t="str">
         <f aca="true">IF(I225="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B226" s="21"/>
-      <c r="C226" s="21"/>
-      <c r="E226" s="22"/>
-      <c r="H226" s="24" t="str">
+      <c r="B226" s="17"/>
+      <c r="C226" s="17"/>
+      <c r="E226" s="21"/>
+      <c r="H226" s="23" t="str">
         <f aca="true">IF(I226 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q226" s="25"/>
-      <c r="R226" s="25" t="str">
+      <c r="Q226" s="24"/>
+      <c r="R226" s="24" t="str">
         <f aca="true">IF(I226="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B227" s="21"/>
-      <c r="C227" s="21"/>
-      <c r="E227" s="22"/>
-      <c r="H227" s="24" t="str">
+      <c r="B227" s="17"/>
+      <c r="C227" s="17"/>
+      <c r="E227" s="21"/>
+      <c r="H227" s="23" t="str">
         <f aca="true">IF(I227 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q227" s="25"/>
-      <c r="R227" s="25" t="str">
+      <c r="Q227" s="24"/>
+      <c r="R227" s="24" t="str">
         <f aca="true">IF(I227="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B228" s="21"/>
-      <c r="C228" s="21"/>
-      <c r="E228" s="22"/>
-      <c r="H228" s="24" t="str">
+      <c r="B228" s="17"/>
+      <c r="C228" s="17"/>
+      <c r="E228" s="21"/>
+      <c r="H228" s="23" t="str">
         <f aca="true">IF(I228 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q228" s="25"/>
-      <c r="R228" s="25" t="str">
+      <c r="Q228" s="24"/>
+      <c r="R228" s="24" t="str">
         <f aca="true">IF(I228="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B229" s="21"/>
-      <c r="C229" s="21"/>
-      <c r="E229" s="22"/>
-      <c r="H229" s="24" t="str">
+      <c r="B229" s="17"/>
+      <c r="C229" s="17"/>
+      <c r="E229" s="21"/>
+      <c r="H229" s="23" t="str">
         <f aca="true">IF(I229 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q229" s="25"/>
-      <c r="R229" s="25" t="str">
+      <c r="Q229" s="24"/>
+      <c r="R229" s="24" t="str">
         <f aca="true">IF(I229="-",IF(ISNUMBER(SEARCH(",", INDIRECT("B" &amp; ROW() - 1) )),1,""), "")</f>
         <v/>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B230" s="21"/>
-      <c r="C230" s="21"/>
-      <c r="E230" s="22"/>
-      <c r="H230" s="24" t="str">
+      <c r="B230" s="17"/>
+      <c r="C230" s="17"/>
+      <c r="E230" s="21"/>
+      <c r="H230" s="23" t="str">
         <f aca="true">IF(I230 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q230" s="25"/>
-      <c r="R230" s="25"/>
+      <c r="Q230" s="24"/>
+      <c r="R230" s="24"/>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B231" s="21"/>
-      <c r="C231" s="21"/>
-      <c r="E231" s="22"/>
-      <c r="H231" s="24" t="str">
+      <c r="B231" s="17"/>
+      <c r="C231" s="17"/>
+      <c r="E231" s="21"/>
+      <c r="H231" s="23" t="str">
         <f aca="true">IF(I231 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q231" s="25"/>
-      <c r="R231" s="25"/>
+      <c r="Q231" s="24"/>
+      <c r="R231" s="24"/>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B232" s="21"/>
-      <c r="C232" s="21"/>
-      <c r="E232" s="22"/>
-      <c r="H232" s="24" t="str">
+      <c r="B232" s="17"/>
+      <c r="C232" s="17"/>
+      <c r="E232" s="21"/>
+      <c r="H232" s="23" t="str">
         <f aca="true">IF(I232 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q232" s="25"/>
-      <c r="R232" s="25"/>
+      <c r="Q232" s="24"/>
+      <c r="R232" s="24"/>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B233" s="21"/>
-      <c r="C233" s="21"/>
-      <c r="E233" s="22"/>
-      <c r="H233" s="24" t="str">
+      <c r="B233" s="17"/>
+      <c r="C233" s="17"/>
+      <c r="E233" s="21"/>
+      <c r="H233" s="23" t="str">
         <f aca="true">IF(I233 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q233" s="25"/>
-      <c r="R233" s="25"/>
+      <c r="Q233" s="24"/>
+      <c r="R233" s="24"/>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B234" s="21"/>
-      <c r="C234" s="21"/>
-      <c r="E234" s="22"/>
-      <c r="H234" s="24" t="str">
+      <c r="B234" s="17"/>
+      <c r="C234" s="17"/>
+      <c r="E234" s="21"/>
+      <c r="H234" s="23" t="str">
         <f aca="true">IF(I234 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q234" s="25"/>
-      <c r="R234" s="25"/>
+      <c r="Q234" s="24"/>
+      <c r="R234" s="24"/>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B235" s="21"/>
-      <c r="C235" s="21"/>
-      <c r="E235" s="22"/>
-      <c r="H235" s="24" t="str">
+      <c r="B235" s="17"/>
+      <c r="C235" s="17"/>
+      <c r="E235" s="21"/>
+      <c r="H235" s="23" t="str">
         <f aca="true">IF(I235 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q235" s="25"/>
-      <c r="R235" s="25"/>
+      <c r="Q235" s="24"/>
+      <c r="R235" s="24"/>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B236" s="21"/>
-      <c r="C236" s="21"/>
-      <c r="E236" s="22"/>
-      <c r="H236" s="24" t="str">
+      <c r="B236" s="17"/>
+      <c r="C236" s="17"/>
+      <c r="E236" s="21"/>
+      <c r="H236" s="23" t="str">
         <f aca="true">IF(I236 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q236" s="25"/>
-      <c r="R236" s="25"/>
+      <c r="Q236" s="24"/>
+      <c r="R236" s="24"/>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B237" s="21"/>
-      <c r="C237" s="21"/>
-      <c r="E237" s="22"/>
-      <c r="H237" s="24" t="str">
+      <c r="B237" s="17"/>
+      <c r="C237" s="17"/>
+      <c r="E237" s="21"/>
+      <c r="H237" s="23" t="str">
         <f aca="true">IF(I237 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q237" s="25"/>
-      <c r="R237" s="25"/>
+      <c r="Q237" s="24"/>
+      <c r="R237" s="24"/>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B238" s="21"/>
-      <c r="C238" s="21"/>
-      <c r="E238" s="22"/>
-      <c r="H238" s="24" t="str">
+      <c r="B238" s="17"/>
+      <c r="C238" s="17"/>
+      <c r="E238" s="21"/>
+      <c r="H238" s="23" t="str">
         <f aca="true">IF(I238 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q238" s="25"/>
-      <c r="R238" s="25"/>
+      <c r="Q238" s="24"/>
+      <c r="R238" s="24"/>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B239" s="21"/>
-      <c r="C239" s="21"/>
-      <c r="E239" s="22"/>
-      <c r="H239" s="24" t="str">
+      <c r="B239" s="17"/>
+      <c r="C239" s="17"/>
+      <c r="E239" s="21"/>
+      <c r="H239" s="23" t="str">
         <f aca="true">IF(I239 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q239" s="25"/>
-      <c r="R239" s="25"/>
+      <c r="Q239" s="24"/>
+      <c r="R239" s="24"/>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B240" s="21"/>
-      <c r="C240" s="21"/>
-      <c r="E240" s="22"/>
-      <c r="H240" s="24" t="str">
+      <c r="B240" s="17"/>
+      <c r="C240" s="17"/>
+      <c r="E240" s="21"/>
+      <c r="H240" s="23" t="str">
         <f aca="true">IF(I240 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q240" s="25"/>
-      <c r="R240" s="25"/>
+      <c r="Q240" s="24"/>
+      <c r="R240" s="24"/>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B241" s="21"/>
-      <c r="C241" s="21"/>
-      <c r="E241" s="22"/>
-      <c r="H241" s="24" t="str">
+      <c r="B241" s="17"/>
+      <c r="C241" s="17"/>
+      <c r="E241" s="21"/>
+      <c r="H241" s="23" t="str">
         <f aca="true">IF(I241 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q241" s="25"/>
-      <c r="R241" s="25"/>
+      <c r="Q241" s="24"/>
+      <c r="R241" s="24"/>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B242" s="21"/>
-      <c r="C242" s="21"/>
-      <c r="E242" s="22"/>
-      <c r="H242" s="24" t="str">
+      <c r="B242" s="17"/>
+      <c r="C242" s="17"/>
+      <c r="E242" s="21"/>
+      <c r="H242" s="23" t="str">
         <f aca="true">IF(I242 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q242" s="25"/>
-      <c r="R242" s="25"/>
+      <c r="Q242" s="24"/>
+      <c r="R242" s="24"/>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B243" s="21"/>
-      <c r="C243" s="21"/>
-      <c r="E243" s="22"/>
-      <c r="H243" s="24" t="str">
+      <c r="B243" s="17"/>
+      <c r="C243" s="17"/>
+      <c r="E243" s="21"/>
+      <c r="H243" s="23" t="str">
         <f aca="true">IF(I243 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q243" s="25"/>
-      <c r="R243" s="25"/>
+      <c r="Q243" s="24"/>
+      <c r="R243" s="24"/>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B244" s="21"/>
-      <c r="C244" s="21"/>
-      <c r="E244" s="22"/>
-      <c r="H244" s="24" t="str">
+      <c r="B244" s="17"/>
+      <c r="C244" s="17"/>
+      <c r="E244" s="21"/>
+      <c r="H244" s="23" t="str">
         <f aca="true">IF(I244 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q244" s="25"/>
-      <c r="R244" s="25"/>
+      <c r="Q244" s="24"/>
+      <c r="R244" s="24"/>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B245" s="21"/>
-      <c r="C245" s="21"/>
-      <c r="E245" s="22"/>
-      <c r="H245" s="24" t="str">
+      <c r="B245" s="17"/>
+      <c r="C245" s="17"/>
+      <c r="E245" s="21"/>
+      <c r="H245" s="23" t="str">
         <f aca="true">IF(I245 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q245" s="25"/>
-      <c r="R245" s="25"/>
+      <c r="Q245" s="24"/>
+      <c r="R245" s="24"/>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B246" s="21"/>
-      <c r="C246" s="21"/>
-      <c r="E246" s="22"/>
-      <c r="H246" s="24" t="str">
+      <c r="B246" s="17"/>
+      <c r="C246" s="17"/>
+      <c r="E246" s="21"/>
+      <c r="H246" s="23" t="str">
         <f aca="true">IF(I246 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q246" s="25"/>
-      <c r="R246" s="25"/>
+      <c r="Q246" s="24"/>
+      <c r="R246" s="24"/>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B247" s="21"/>
-      <c r="C247" s="21"/>
-      <c r="E247" s="22"/>
-      <c r="H247" s="24" t="str">
+      <c r="B247" s="17"/>
+      <c r="C247" s="17"/>
+      <c r="E247" s="21"/>
+      <c r="H247" s="23" t="str">
         <f aca="true">IF(I247 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q247" s="25"/>
-      <c r="R247" s="25"/>
+      <c r="Q247" s="24"/>
+      <c r="R247" s="24"/>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B248" s="21"/>
-      <c r="C248" s="21"/>
-      <c r="E248" s="22"/>
-      <c r="H248" s="24" t="str">
+      <c r="B248" s="17"/>
+      <c r="C248" s="17"/>
+      <c r="E248" s="21"/>
+      <c r="H248" s="23" t="str">
         <f aca="true">IF(I248 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q248" s="25"/>
-      <c r="R248" s="25"/>
+      <c r="Q248" s="24"/>
+      <c r="R248" s="24"/>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B249" s="21"/>
-      <c r="C249" s="21"/>
-      <c r="E249" s="22"/>
-      <c r="H249" s="24" t="str">
+      <c r="B249" s="17"/>
+      <c r="C249" s="17"/>
+      <c r="E249" s="21"/>
+      <c r="H249" s="23" t="str">
         <f aca="true">IF(I249 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q249" s="25"/>
-      <c r="R249" s="25"/>
+      <c r="Q249" s="24"/>
+      <c r="R249" s="24"/>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B250" s="21"/>
-      <c r="C250" s="21"/>
-      <c r="E250" s="22"/>
-      <c r="H250" s="24" t="str">
+      <c r="B250" s="17"/>
+      <c r="C250" s="17"/>
+      <c r="E250" s="21"/>
+      <c r="H250" s="23" t="str">
         <f aca="true">IF(I250 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q250" s="25"/>
-      <c r="R250" s="25"/>
+      <c r="Q250" s="24"/>
+      <c r="R250" s="24"/>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B251" s="21"/>
-      <c r="C251" s="21"/>
-      <c r="E251" s="22"/>
-      <c r="H251" s="24" t="str">
+      <c r="B251" s="17"/>
+      <c r="C251" s="17"/>
+      <c r="E251" s="21"/>
+      <c r="H251" s="23" t="str">
         <f aca="true">IF(I251 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q251" s="25"/>
-      <c r="R251" s="25"/>
+      <c r="Q251" s="24"/>
+      <c r="R251" s="24"/>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B252" s="21"/>
-      <c r="C252" s="21"/>
-      <c r="E252" s="22"/>
-      <c r="H252" s="24" t="str">
+      <c r="B252" s="17"/>
+      <c r="C252" s="17"/>
+      <c r="E252" s="21"/>
+      <c r="H252" s="23" t="str">
         <f aca="true">IF(I252 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q252" s="25"/>
-      <c r="R252" s="25"/>
+      <c r="Q252" s="24"/>
+      <c r="R252" s="24"/>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B253" s="21"/>
-      <c r="C253" s="21"/>
-      <c r="E253" s="22"/>
-      <c r="H253" s="24" t="str">
+      <c r="B253" s="17"/>
+      <c r="C253" s="17"/>
+      <c r="E253" s="21"/>
+      <c r="H253" s="23" t="str">
         <f aca="true">IF(I253 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q253" s="25"/>
-      <c r="R253" s="25"/>
+      <c r="Q253" s="24"/>
+      <c r="R253" s="24"/>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B254" s="21"/>
-      <c r="C254" s="21"/>
-      <c r="E254" s="22"/>
-      <c r="H254" s="24" t="str">
+      <c r="B254" s="17"/>
+      <c r="C254" s="17"/>
+      <c r="E254" s="21"/>
+      <c r="H254" s="23" t="str">
         <f aca="true">IF(I254 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q254" s="25"/>
-      <c r="R254" s="25"/>
+      <c r="Q254" s="24"/>
+      <c r="R254" s="24"/>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B255" s="21"/>
-      <c r="C255" s="21"/>
-      <c r="E255" s="22"/>
-      <c r="H255" s="24" t="str">
+      <c r="B255" s="17"/>
+      <c r="C255" s="17"/>
+      <c r="E255" s="21"/>
+      <c r="H255" s="23" t="str">
         <f aca="true">IF(I255 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q255" s="25"/>
-      <c r="R255" s="25"/>
+      <c r="Q255" s="24"/>
+      <c r="R255" s="24"/>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B256" s="21"/>
-      <c r="C256" s="21"/>
-      <c r="E256" s="22"/>
-      <c r="H256" s="24" t="str">
+      <c r="B256" s="17"/>
+      <c r="C256" s="17"/>
+      <c r="E256" s="21"/>
+      <c r="H256" s="23" t="str">
         <f aca="true">IF(I256 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q256" s="25"/>
-      <c r="R256" s="25"/>
+      <c r="Q256" s="24"/>
+      <c r="R256" s="24"/>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B257" s="21"/>
-      <c r="C257" s="21"/>
-      <c r="E257" s="22"/>
-      <c r="H257" s="24" t="str">
+      <c r="B257" s="17"/>
+      <c r="C257" s="17"/>
+      <c r="E257" s="21"/>
+      <c r="H257" s="23" t="str">
         <f aca="true">IF(I257 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q257" s="25"/>
-      <c r="R257" s="25"/>
+      <c r="Q257" s="24"/>
+      <c r="R257" s="24"/>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B258" s="21"/>
-      <c r="C258" s="21"/>
-      <c r="E258" s="22"/>
-      <c r="H258" s="24" t="str">
+      <c r="B258" s="17"/>
+      <c r="C258" s="17"/>
+      <c r="E258" s="21"/>
+      <c r="H258" s="23" t="str">
         <f aca="true">IF(I258 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q258" s="25"/>
-      <c r="R258" s="25"/>
+      <c r="Q258" s="24"/>
+      <c r="R258" s="24"/>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B259" s="21"/>
-      <c r="C259" s="21"/>
-      <c r="E259" s="22"/>
-      <c r="H259" s="24" t="str">
+      <c r="B259" s="17"/>
+      <c r="C259" s="17"/>
+      <c r="E259" s="21"/>
+      <c r="H259" s="23" t="str">
         <f aca="true">IF(I259 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q259" s="25"/>
-      <c r="R259" s="25"/>
+      <c r="Q259" s="24"/>
+      <c r="R259" s="24"/>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B260" s="21"/>
-      <c r="C260" s="21"/>
-      <c r="E260" s="22"/>
-      <c r="H260" s="24" t="str">
+      <c r="B260" s="17"/>
+      <c r="C260" s="17"/>
+      <c r="E260" s="21"/>
+      <c r="H260" s="23" t="str">
         <f aca="true">IF(I260 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q260" s="25"/>
-      <c r="R260" s="25"/>
+      <c r="Q260" s="24"/>
+      <c r="R260" s="24"/>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B261" s="21"/>
-      <c r="C261" s="21"/>
-      <c r="E261" s="22"/>
-      <c r="H261" s="24" t="str">
+      <c r="B261" s="17"/>
+      <c r="C261" s="17"/>
+      <c r="E261" s="21"/>
+      <c r="H261" s="23" t="str">
         <f aca="true">IF(I261 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q261" s="25"/>
-      <c r="R261" s="25"/>
+      <c r="Q261" s="24"/>
+      <c r="R261" s="24"/>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B262" s="21"/>
-      <c r="C262" s="21"/>
-      <c r="E262" s="22"/>
-      <c r="H262" s="24" t="str">
+      <c r="B262" s="17"/>
+      <c r="C262" s="17"/>
+      <c r="E262" s="21"/>
+      <c r="H262" s="23" t="str">
         <f aca="true">IF(I262 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q262" s="25"/>
-      <c r="R262" s="25"/>
+      <c r="Q262" s="24"/>
+      <c r="R262" s="24"/>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B263" s="21"/>
-      <c r="C263" s="21"/>
-      <c r="E263" s="22"/>
-      <c r="H263" s="24" t="str">
+      <c r="B263" s="17"/>
+      <c r="C263" s="17"/>
+      <c r="E263" s="21"/>
+      <c r="H263" s="23" t="str">
         <f aca="true">IF(I263 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q263" s="25"/>
-      <c r="R263" s="25"/>
+      <c r="Q263" s="24"/>
+      <c r="R263" s="24"/>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B264" s="21"/>
-      <c r="C264" s="21"/>
-      <c r="E264" s="22"/>
-      <c r="H264" s="24" t="str">
+      <c r="B264" s="17"/>
+      <c r="C264" s="17"/>
+      <c r="E264" s="21"/>
+      <c r="H264" s="23" t="str">
         <f aca="true">IF(I264 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q264" s="25"/>
-      <c r="R264" s="25"/>
+      <c r="Q264" s="24"/>
+      <c r="R264" s="24"/>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B265" s="21"/>
-      <c r="C265" s="21"/>
-      <c r="E265" s="22"/>
-      <c r="H265" s="24" t="str">
+      <c r="B265" s="17"/>
+      <c r="C265" s="17"/>
+      <c r="E265" s="21"/>
+      <c r="H265" s="23" t="str">
         <f aca="true">IF(I265 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q265" s="25"/>
-      <c r="R265" s="25"/>
+      <c r="Q265" s="24"/>
+      <c r="R265" s="24"/>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B266" s="21"/>
-      <c r="C266" s="21"/>
-      <c r="E266" s="22"/>
-      <c r="H266" s="24" t="str">
+      <c r="B266" s="17"/>
+      <c r="C266" s="17"/>
+      <c r="E266" s="21"/>
+      <c r="H266" s="23" t="str">
         <f aca="true">IF(I266 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q266" s="25"/>
-      <c r="R266" s="25"/>
+      <c r="Q266" s="24"/>
+      <c r="R266" s="24"/>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B267" s="21"/>
-      <c r="C267" s="21"/>
-      <c r="E267" s="22"/>
-      <c r="H267" s="24" t="str">
+      <c r="B267" s="17"/>
+      <c r="C267" s="17"/>
+      <c r="E267" s="21"/>
+      <c r="H267" s="23" t="str">
         <f aca="true">IF(I267 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
-      <c r="Q267" s="25"/>
-      <c r="R267" s="25"/>
+      <c r="Q267" s="24"/>
+      <c r="R267" s="24"/>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B268" s="21"/>
-      <c r="C268" s="21"/>
-      <c r="E268" s="22"/>
-      <c r="H268" s="24" t="str">
+      <c r="B268" s="17"/>
+      <c r="C268" s="17"/>
+      <c r="E268" s="21"/>
+      <c r="H268" s="23" t="str">
         <f aca="true">IF(I268 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B269" s="21"/>
-      <c r="C269" s="21"/>
-      <c r="E269" s="22"/>
-      <c r="H269" s="24" t="str">
+      <c r="B269" s="17"/>
+      <c r="C269" s="17"/>
+      <c r="E269" s="21"/>
+      <c r="H269" s="23" t="str">
         <f aca="true">IF(I269 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B270" s="21"/>
-      <c r="C270" s="21"/>
-      <c r="E270" s="22"/>
-      <c r="H270" s="24" t="str">
+      <c r="B270" s="17"/>
+      <c r="C270" s="17"/>
+      <c r="E270" s="21"/>
+      <c r="H270" s="23" t="str">
         <f aca="true">IF(I270 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B271" s="21"/>
-      <c r="C271" s="21"/>
-      <c r="E271" s="22"/>
-      <c r="H271" s="24" t="str">
+      <c r="B271" s="17"/>
+      <c r="C271" s="17"/>
+      <c r="E271" s="21"/>
+      <c r="H271" s="23" t="str">
         <f aca="true">IF(I271 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B272" s="21"/>
-      <c r="C272" s="21"/>
-      <c r="E272" s="22"/>
-      <c r="H272" s="24" t="str">
+      <c r="B272" s="17"/>
+      <c r="C272" s="17"/>
+      <c r="E272" s="21"/>
+      <c r="H272" s="23" t="str">
         <f aca="true">IF(I272 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B273" s="21"/>
-      <c r="C273" s="21"/>
-      <c r="E273" s="22"/>
-      <c r="H273" s="24" t="str">
+      <c r="B273" s="17"/>
+      <c r="C273" s="17"/>
+      <c r="E273" s="21"/>
+      <c r="H273" s="23" t="str">
         <f aca="true">IF(I273 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B274" s="21"/>
-      <c r="C274" s="21"/>
-      <c r="E274" s="22"/>
-      <c r="H274" s="24" t="str">
+      <c r="B274" s="17"/>
+      <c r="C274" s="17"/>
+      <c r="E274" s="21"/>
+      <c r="H274" s="23" t="str">
         <f aca="true">IF(I274 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
-      <c r="E275" s="22"/>
-      <c r="H275" s="24" t="str">
+      <c r="B275" s="17"/>
+      <c r="C275" s="17"/>
+      <c r="E275" s="21"/>
+      <c r="H275" s="23" t="str">
         <f aca="true">IF(I275 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B276" s="21"/>
-      <c r="C276" s="21"/>
-      <c r="E276" s="22"/>
-      <c r="H276" s="24" t="str">
+      <c r="B276" s="17"/>
+      <c r="C276" s="17"/>
+      <c r="E276" s="21"/>
+      <c r="H276" s="23" t="str">
         <f aca="true">IF(I276 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B277" s="21"/>
-      <c r="C277" s="21"/>
-      <c r="E277" s="22"/>
-      <c r="H277" s="24" t="str">
+      <c r="B277" s="17"/>
+      <c r="C277" s="17"/>
+      <c r="E277" s="21"/>
+      <c r="H277" s="23" t="str">
         <f aca="true">IF(I277 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B278" s="21"/>
-      <c r="C278" s="21"/>
-      <c r="E278" s="22"/>
-      <c r="H278" s="24" t="str">
+      <c r="B278" s="17"/>
+      <c r="C278" s="17"/>
+      <c r="E278" s="21"/>
+      <c r="H278" s="23" t="str">
         <f aca="true">IF(I278 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B279" s="21"/>
-      <c r="C279" s="21"/>
-      <c r="E279" s="22"/>
-      <c r="H279" s="24" t="str">
+      <c r="B279" s="17"/>
+      <c r="C279" s="17"/>
+      <c r="E279" s="21"/>
+      <c r="H279" s="23" t="str">
         <f aca="true">IF(I279 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B280" s="21"/>
-      <c r="C280" s="21"/>
-      <c r="E280" s="22"/>
-      <c r="H280" s="24" t="str">
+      <c r="B280" s="17"/>
+      <c r="C280" s="17"/>
+      <c r="E280" s="21"/>
+      <c r="H280" s="23" t="str">
         <f aca="true">IF(I280 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B281" s="21"/>
-      <c r="C281" s="21"/>
-      <c r="E281" s="22"/>
-      <c r="H281" s="24" t="str">
+      <c r="B281" s="17"/>
+      <c r="C281" s="17"/>
+      <c r="E281" s="21"/>
+      <c r="H281" s="23" t="str">
         <f aca="true">IF(I281 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B282" s="21"/>
-      <c r="C282" s="21"/>
-      <c r="E282" s="22"/>
-      <c r="H282" s="24" t="str">
+      <c r="B282" s="17"/>
+      <c r="C282" s="17"/>
+      <c r="E282" s="21"/>
+      <c r="H282" s="23" t="str">
         <f aca="true">IF(I282 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B283" s="21"/>
-      <c r="C283" s="21"/>
-      <c r="E283" s="22"/>
-      <c r="H283" s="24" t="str">
+      <c r="B283" s="17"/>
+      <c r="C283" s="17"/>
+      <c r="E283" s="21"/>
+      <c r="H283" s="23" t="str">
         <f aca="true">IF(I283 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B284" s="21"/>
-      <c r="C284" s="21"/>
-      <c r="E284" s="22"/>
-      <c r="H284" s="24" t="str">
+      <c r="B284" s="17"/>
+      <c r="C284" s="17"/>
+      <c r="E284" s="21"/>
+      <c r="H284" s="23" t="str">
         <f aca="true">IF(I284 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B285" s="21"/>
-      <c r="C285" s="21"/>
-      <c r="E285" s="22"/>
-      <c r="H285" s="24" t="str">
+      <c r="B285" s="17"/>
+      <c r="C285" s="17"/>
+      <c r="E285" s="21"/>
+      <c r="H285" s="23" t="str">
         <f aca="true">IF(I285 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B286" s="21"/>
-      <c r="C286" s="21"/>
-      <c r="E286" s="22"/>
-      <c r="H286" s="24" t="str">
+      <c r="B286" s="17"/>
+      <c r="C286" s="17"/>
+      <c r="E286" s="21"/>
+      <c r="H286" s="23" t="str">
         <f aca="true">IF(I286 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B287" s="21"/>
-      <c r="C287" s="21"/>
-      <c r="E287" s="22"/>
-      <c r="H287" s="24" t="str">
+      <c r="B287" s="17"/>
+      <c r="C287" s="17"/>
+      <c r="E287" s="21"/>
+      <c r="H287" s="23" t="str">
         <f aca="true">IF(I287 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B288" s="21"/>
-      <c r="C288" s="21"/>
-      <c r="E288" s="22"/>
-      <c r="H288" s="24" t="str">
+      <c r="B288" s="17"/>
+      <c r="C288" s="17"/>
+      <c r="E288" s="21"/>
+      <c r="H288" s="23" t="str">
         <f aca="true">IF(I288 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B289" s="21"/>
-      <c r="C289" s="21"/>
-      <c r="E289" s="22"/>
-      <c r="H289" s="24" t="str">
+      <c r="B289" s="17"/>
+      <c r="C289" s="17"/>
+      <c r="E289" s="21"/>
+      <c r="H289" s="23" t="str">
         <f aca="true">IF(I289 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B290" s="21"/>
-      <c r="C290" s="21"/>
-      <c r="E290" s="22"/>
-      <c r="H290" s="24" t="str">
+      <c r="B290" s="17"/>
+      <c r="C290" s="17"/>
+      <c r="E290" s="21"/>
+      <c r="H290" s="23" t="str">
         <f aca="true">IF(I290 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B291" s="21"/>
-      <c r="C291" s="21"/>
-      <c r="E291" s="22"/>
-      <c r="H291" s="24" t="str">
+      <c r="B291" s="17"/>
+      <c r="C291" s="17"/>
+      <c r="E291" s="21"/>
+      <c r="H291" s="23" t="str">
         <f aca="true">IF(I291 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B292" s="21"/>
-      <c r="C292" s="21"/>
-      <c r="E292" s="22"/>
-      <c r="H292" s="24" t="str">
+      <c r="B292" s="17"/>
+      <c r="C292" s="17"/>
+      <c r="E292" s="21"/>
+      <c r="H292" s="23" t="str">
         <f aca="true">IF(I292 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B293" s="21"/>
-      <c r="C293" s="21"/>
-      <c r="E293" s="22"/>
-      <c r="H293" s="24" t="str">
+      <c r="B293" s="17"/>
+      <c r="C293" s="17"/>
+      <c r="E293" s="21"/>
+      <c r="H293" s="23" t="str">
         <f aca="true">IF(I293 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B294" s="21"/>
-      <c r="C294" s="21"/>
-      <c r="E294" s="22"/>
-      <c r="H294" s="24" t="str">
+      <c r="B294" s="17"/>
+      <c r="C294" s="17"/>
+      <c r="E294" s="21"/>
+      <c r="H294" s="23" t="str">
         <f aca="true">IF(I294 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B295" s="21"/>
-      <c r="C295" s="21"/>
-      <c r="E295" s="22"/>
-      <c r="H295" s="24" t="str">
+      <c r="B295" s="17"/>
+      <c r="C295" s="17"/>
+      <c r="E295" s="21"/>
+      <c r="H295" s="23" t="str">
         <f aca="true">IF(I295 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B296" s="21"/>
-      <c r="C296" s="21"/>
-      <c r="E296" s="22"/>
-      <c r="H296" s="24" t="str">
+      <c r="B296" s="17"/>
+      <c r="C296" s="17"/>
+      <c r="E296" s="21"/>
+      <c r="H296" s="23" t="str">
         <f aca="true">IF(I296 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B297" s="21"/>
-      <c r="C297" s="21"/>
-      <c r="E297" s="22"/>
-      <c r="H297" s="24" t="str">
+      <c r="B297" s="17"/>
+      <c r="C297" s="17"/>
+      <c r="E297" s="21"/>
+      <c r="H297" s="23" t="str">
         <f aca="true">IF(I297 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B298" s="21"/>
-      <c r="C298" s="21"/>
-      <c r="E298" s="22"/>
-      <c r="H298" s="24" t="str">
+      <c r="B298" s="17"/>
+      <c r="C298" s="17"/>
+      <c r="E298" s="21"/>
+      <c r="H298" s="23" t="str">
         <f aca="true">IF(I298 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B299" s="21"/>
-      <c r="C299" s="21"/>
-      <c r="E299" s="22"/>
-      <c r="H299" s="24" t="str">
+      <c r="B299" s="17"/>
+      <c r="C299" s="17"/>
+      <c r="E299" s="21"/>
+      <c r="H299" s="23" t="str">
         <f aca="true">IF(I299 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B300" s="21"/>
-      <c r="C300" s="21"/>
-      <c r="E300" s="22"/>
-      <c r="H300" s="24" t="str">
+      <c r="B300" s="17"/>
+      <c r="C300" s="17"/>
+      <c r="E300" s="21"/>
+      <c r="H300" s="23" t="str">
         <f aca="true">IF(I300 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B301" s="21"/>
-      <c r="C301" s="21"/>
-      <c r="E301" s="22"/>
-      <c r="H301" s="24" t="str">
+      <c r="B301" s="17"/>
+      <c r="C301" s="17"/>
+      <c r="E301" s="21"/>
+      <c r="H301" s="23" t="str">
         <f aca="true">IF(I301 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B302" s="21"/>
-      <c r="C302" s="21"/>
-      <c r="E302" s="22"/>
-      <c r="H302" s="24" t="str">
+      <c r="B302" s="17"/>
+      <c r="C302" s="17"/>
+      <c r="E302" s="21"/>
+      <c r="H302" s="23" t="str">
         <f aca="true">IF(I302 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B303" s="21"/>
-      <c r="C303" s="21"/>
-      <c r="E303" s="22"/>
-      <c r="H303" s="24" t="str">
+      <c r="B303" s="17"/>
+      <c r="C303" s="17"/>
+      <c r="E303" s="21"/>
+      <c r="H303" s="23" t="str">
         <f aca="true">IF(I303 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B304" s="21"/>
-      <c r="C304" s="21"/>
-      <c r="E304" s="22"/>
-      <c r="H304" s="24" t="str">
+      <c r="B304" s="17"/>
+      <c r="C304" s="17"/>
+      <c r="E304" s="21"/>
+      <c r="H304" s="23" t="str">
         <f aca="true">IF(I304 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B305" s="21"/>
-      <c r="C305" s="21"/>
-      <c r="E305" s="22"/>
-      <c r="H305" s="24" t="str">
+      <c r="B305" s="17"/>
+      <c r="C305" s="17"/>
+      <c r="E305" s="21"/>
+      <c r="H305" s="23" t="str">
         <f aca="true">IF(I305 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B306" s="21"/>
-      <c r="C306" s="21"/>
-      <c r="E306" s="22"/>
-      <c r="H306" s="24" t="str">
+      <c r="B306" s="17"/>
+      <c r="C306" s="17"/>
+      <c r="E306" s="21"/>
+      <c r="H306" s="23" t="str">
         <f aca="true">IF(I306 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B307" s="21"/>
-      <c r="C307" s="21"/>
-      <c r="E307" s="22"/>
-      <c r="H307" s="24" t="str">
+      <c r="B307" s="17"/>
+      <c r="C307" s="17"/>
+      <c r="E307" s="21"/>
+      <c r="H307" s="23" t="str">
         <f aca="true">IF(I307 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B308" s="21"/>
-      <c r="C308" s="21"/>
-      <c r="E308" s="22"/>
-      <c r="H308" s="24" t="str">
+      <c r="B308" s="17"/>
+      <c r="C308" s="17"/>
+      <c r="E308" s="21"/>
+      <c r="H308" s="23" t="str">
         <f aca="true">IF(I308 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B309" s="21"/>
-      <c r="C309" s="21"/>
-      <c r="E309" s="22"/>
-      <c r="H309" s="24" t="str">
+      <c r="B309" s="17"/>
+      <c r="C309" s="17"/>
+      <c r="E309" s="21"/>
+      <c r="H309" s="23" t="str">
         <f aca="true">IF(I309 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B310" s="21"/>
-      <c r="C310" s="21"/>
-      <c r="E310" s="22"/>
-      <c r="H310" s="24" t="str">
+      <c r="B310" s="17"/>
+      <c r="C310" s="17"/>
+      <c r="E310" s="21"/>
+      <c r="H310" s="23" t="str">
         <f aca="true">IF(I310 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B311" s="21"/>
-      <c r="C311" s="21"/>
-      <c r="E311" s="22"/>
-      <c r="H311" s="24" t="str">
+      <c r="B311" s="17"/>
+      <c r="C311" s="17"/>
+      <c r="E311" s="21"/>
+      <c r="H311" s="23" t="str">
         <f aca="true">IF(I311 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B312" s="21"/>
-      <c r="C312" s="21"/>
-      <c r="E312" s="22"/>
-      <c r="H312" s="24" t="str">
+      <c r="B312" s="17"/>
+      <c r="C312" s="17"/>
+      <c r="E312" s="21"/>
+      <c r="H312" s="23" t="str">
         <f aca="true">IF(I312 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B313" s="21"/>
-      <c r="C313" s="21"/>
-      <c r="E313" s="22"/>
-      <c r="H313" s="24" t="str">
+      <c r="B313" s="17"/>
+      <c r="C313" s="17"/>
+      <c r="E313" s="21"/>
+      <c r="H313" s="23" t="str">
         <f aca="true">IF(I313 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B314" s="21"/>
-      <c r="C314" s="21"/>
-      <c r="E314" s="22"/>
-      <c r="H314" s="24" t="str">
+      <c r="B314" s="17"/>
+      <c r="C314" s="17"/>
+      <c r="E314" s="21"/>
+      <c r="H314" s="23" t="str">
         <f aca="true">IF(I314 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B315" s="21"/>
-      <c r="C315" s="21"/>
-      <c r="E315" s="22"/>
-      <c r="H315" s="24" t="str">
+      <c r="B315" s="17"/>
+      <c r="C315" s="17"/>
+      <c r="E315" s="21"/>
+      <c r="H315" s="23" t="str">
         <f aca="true">IF(I315 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B316" s="21"/>
-      <c r="C316" s="21"/>
-      <c r="E316" s="22"/>
-      <c r="H316" s="24" t="str">
+      <c r="B316" s="17"/>
+      <c r="C316" s="17"/>
+      <c r="E316" s="21"/>
+      <c r="H316" s="23" t="str">
         <f aca="true">IF(I316 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B317" s="21"/>
-      <c r="C317" s="21"/>
-      <c r="E317" s="22"/>
-      <c r="H317" s="24" t="str">
+      <c r="B317" s="17"/>
+      <c r="C317" s="17"/>
+      <c r="E317" s="21"/>
+      <c r="H317" s="23" t="str">
         <f aca="true">IF(I317 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B318" s="21"/>
-      <c r="C318" s="21"/>
-      <c r="E318" s="22"/>
-      <c r="H318" s="24" t="str">
+      <c r="B318" s="17"/>
+      <c r="C318" s="17"/>
+      <c r="E318" s="21"/>
+      <c r="H318" s="23" t="str">
         <f aca="true">IF(I318 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B319" s="21"/>
-      <c r="C319" s="21"/>
-      <c r="E319" s="22"/>
-      <c r="H319" s="24" t="str">
+      <c r="B319" s="17"/>
+      <c r="C319" s="17"/>
+      <c r="E319" s="21"/>
+      <c r="H319" s="23" t="str">
         <f aca="true">IF(I319 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B320" s="21"/>
-      <c r="C320" s="21"/>
-      <c r="E320" s="22"/>
-      <c r="H320" s="24" t="str">
+      <c r="B320" s="17"/>
+      <c r="C320" s="17"/>
+      <c r="E320" s="21"/>
+      <c r="H320" s="23" t="str">
         <f aca="true">IF(I320 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B321" s="21"/>
-      <c r="C321" s="21"/>
-      <c r="E321" s="22"/>
-      <c r="H321" s="24" t="str">
+      <c r="B321" s="17"/>
+      <c r="C321" s="17"/>
+      <c r="E321" s="21"/>
+      <c r="H321" s="23" t="str">
         <f aca="true">IF(I321 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B322" s="21"/>
-      <c r="C322" s="21"/>
-      <c r="H322" s="24" t="str">
+      <c r="B322" s="17"/>
+      <c r="C322" s="17"/>
+      <c r="H322" s="23" t="str">
         <f aca="true">IF(I322 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B323" s="21"/>
-      <c r="C323" s="21"/>
-      <c r="H323" s="24" t="str">
+      <c r="B323" s="17"/>
+      <c r="C323" s="17"/>
+      <c r="H323" s="23" t="str">
         <f aca="true">IF(I323 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B324" s="21"/>
-      <c r="C324" s="21"/>
-      <c r="H324" s="24" t="str">
+      <c r="B324" s="17"/>
+      <c r="C324" s="17"/>
+      <c r="H324" s="23" t="str">
         <f aca="true">IF(I324 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B325" s="21"/>
-      <c r="C325" s="21"/>
-      <c r="H325" s="24" t="str">
+      <c r="B325" s="17"/>
+      <c r="C325" s="17"/>
+      <c r="H325" s="23" t="str">
         <f aca="true">IF(I325 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B326" s="21"/>
-      <c r="C326" s="21"/>
-      <c r="H326" s="24" t="str">
+      <c r="B326" s="17"/>
+      <c r="C326" s="17"/>
+      <c r="H326" s="23" t="str">
         <f aca="true">IF(I326 = "-", INDIRECT("C" &amp; ROW() - 1) ,"")</f>
         <v/>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B327" s="21"/>
-      <c r="C327" s="21"/>
+      <c r="B327" s="17"/>
+      <c r="C327" s="17"/>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B328" s="21"/>
-      <c r="C328" s="21"/>
+      <c r="B328" s="17"/>
+      <c r="C328" s="17"/>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B329" s="21"/>
-      <c r="C329" s="21"/>
+      <c r="B329" s="17"/>
+      <c r="C329" s="17"/>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B330" s="21"/>
-      <c r="C330" s="21"/>
+      <c r="B330" s="17"/>
+      <c r="C330" s="17"/>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B331" s="21"/>
-      <c r="C331" s="21"/>
+      <c r="B331" s="17"/>
+      <c r="C331" s="17"/>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B332" s="21"/>
-      <c r="C332" s="21"/>
+      <c r="B332" s="17"/>
+      <c r="C332" s="17"/>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B333" s="21"/>
-      <c r="C333" s="21"/>
+      <c r="B333" s="17"/>
+      <c r="C333" s="17"/>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B334" s="21"/>
-      <c r="C334" s="21"/>
+      <c r="B334" s="17"/>
+      <c r="C334" s="17"/>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B335" s="21"/>
-      <c r="C335" s="21"/>
+      <c r="B335" s="17"/>
+      <c r="C335" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -10019,10 +10016,6 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D100" type="list">
-      <formula1>'SKU Маскарпоне'!$A$1:$A$50</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="C102:C123 B118:B123 B124:C335" type="list">
       <formula1>'SKU Маскарпоне'!$B$1:$B$50</formula1>
       <formula2>0</formula2>
@@ -10033,6 +10026,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="C3:C101" type="list">
       <formula1>'SKU Маскарпоне'!$B$1:$B$150</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D136" type="list">
+      <formula1>'SKU Маскарпоне'!$A$1:$A$150</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -10187,36 +10184,36 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26" t="s">
+    <row r="1" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="25" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>